<commit_message>
Repaired stock screening and dividend ploting. Updated Stocks class with multiple checks for data retrieved from the database
</commit_message>
<xml_diff>
--- a/outData/FilledPriceDaily.xlsx
+++ b/outData/FilledPriceDaily.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="700">
   <si>
     <t>GPC</t>
   </si>
@@ -403,6 +403,9 @@
     <t>WLY</t>
   </si>
   <si>
+    <t>WLYB</t>
+  </si>
+  <si>
     <t>ALRS</t>
   </si>
   <si>
@@ -1372,6 +1375,9 @@
     <t>PEBK</t>
   </si>
   <si>
+    <t>HFBL</t>
+  </si>
+  <si>
     <t>OTTR</t>
   </si>
   <si>
@@ -2107,7 +2113,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-17</t>
+    <t>2025-03-21</t>
   </si>
 </sst>
 </file>
@@ -2465,15 +2471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ZU2"/>
+  <dimension ref="A1:ZW2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:697">
+    <row r="1" spans="1:699">
       <c r="A1" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4563,2098 +4569,2110 @@
       <c r="ZU1" s="1" t="s">
         <v>695</v>
       </c>
+      <c r="ZV1" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="ZW1" s="1" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="2" spans="1:697">
+    <row r="2" spans="1:699">
       <c r="A2" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B2">
-        <v>123.48</v>
+        <v>118.78</v>
       </c>
       <c r="C2">
-        <v>94.31</v>
+        <v>92.83</v>
       </c>
       <c r="D2">
-        <v>467.61</v>
+        <v>439.7</v>
       </c>
       <c r="E2">
-        <v>78</v>
+        <v>75.44</v>
       </c>
       <c r="F2">
-        <v>182.96</v>
+        <v>179.64</v>
       </c>
       <c r="G2">
-        <v>41.91</v>
+        <v>41.27</v>
       </c>
       <c r="H2">
-        <v>169.76</v>
+        <v>166.69</v>
       </c>
       <c r="I2">
-        <v>621.58</v>
+        <v>622.1</v>
       </c>
       <c r="J2">
-        <v>113.59</v>
+        <v>113.11</v>
       </c>
       <c r="K2">
-        <v>147.22</v>
+        <v>145.62</v>
       </c>
       <c r="L2">
-        <v>225.85</v>
+        <v>227.07</v>
       </c>
       <c r="M2">
-        <v>162.84</v>
+        <v>163.63</v>
       </c>
       <c r="N2">
-        <v>70.12</v>
+        <v>68.67</v>
       </c>
       <c r="O2">
-        <v>183.21</v>
+        <v>175.33</v>
       </c>
       <c r="P2">
-        <v>210.68</v>
+        <v>203.86</v>
       </c>
       <c r="Q2">
-        <v>256.13</v>
+        <v>251.34</v>
       </c>
       <c r="R2">
-        <v>90.70999999999999</v>
+        <v>90.3</v>
       </c>
       <c r="S2">
-        <v>31.63</v>
+        <v>31.28</v>
       </c>
       <c r="T2">
-        <v>29.96</v>
+        <v>29.98</v>
       </c>
       <c r="U2">
-        <v>47.69</v>
+        <v>46.94</v>
       </c>
       <c r="V2">
-        <v>105.67</v>
+        <v>104.06</v>
       </c>
       <c r="W2">
-        <v>81.55</v>
+        <v>79.56</v>
       </c>
       <c r="X2">
-        <v>47.45</v>
+        <v>46.07</v>
       </c>
       <c r="Y2">
-        <v>97.91</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="Z2">
-        <v>53.9</v>
+        <v>51.41</v>
       </c>
       <c r="AA2">
-        <v>58.48</v>
+        <v>57.91</v>
       </c>
       <c r="AB2">
-        <v>61.83</v>
+        <v>61.24</v>
       </c>
       <c r="AC2">
-        <v>53.95</v>
+        <v>53.57</v>
       </c>
       <c r="AD2">
-        <v>58.9</v>
+        <v>57.6</v>
       </c>
       <c r="AE2">
-        <v>77.03</v>
+        <v>78.17</v>
       </c>
       <c r="AF2">
-        <v>61.35</v>
+        <v>59.23</v>
       </c>
       <c r="AG2">
+        <v>71.11</v>
+      </c>
+      <c r="AH2">
+        <v>54.11</v>
+      </c>
+      <c r="AI2">
+        <v>973.09</v>
+      </c>
+      <c r="AJ2">
+        <v>149.85</v>
+      </c>
+      <c r="AK2">
+        <v>110.73</v>
+      </c>
+      <c r="AL2">
+        <v>81.95999999999999</v>
+      </c>
+      <c r="AM2">
+        <v>145.45</v>
+      </c>
+      <c r="AN2">
+        <v>230.23</v>
+      </c>
+      <c r="AO2">
+        <v>138.67</v>
+      </c>
+      <c r="AP2">
+        <v>497.88</v>
+      </c>
+      <c r="AQ2">
+        <v>122.01</v>
+      </c>
+      <c r="AR2">
+        <v>85.98</v>
+      </c>
+      <c r="AS2">
+        <v>114.27</v>
+      </c>
+      <c r="AT2">
+        <v>107.8</v>
+      </c>
+      <c r="AU2">
+        <v>34.38</v>
+      </c>
+      <c r="AV2">
+        <v>295.32</v>
+      </c>
+      <c r="AW2">
+        <v>91.31</v>
+      </c>
+      <c r="AX2">
+        <v>305.44</v>
+      </c>
+      <c r="AY2">
+        <v>76.18000000000001</v>
+      </c>
+      <c r="AZ2">
+        <v>46.1</v>
+      </c>
+      <c r="BA2">
+        <v>336.29</v>
+      </c>
+      <c r="BB2">
+        <v>90.33</v>
+      </c>
+      <c r="BC2">
+        <v>144.84</v>
+      </c>
+      <c r="BD2">
+        <v>334.41</v>
+      </c>
+      <c r="BE2">
+        <v>19.87</v>
+      </c>
+      <c r="BF2">
+        <v>51.26</v>
+      </c>
+      <c r="BG2">
+        <v>37.64</v>
+      </c>
+      <c r="BH2">
+        <v>46.68</v>
+      </c>
+      <c r="BI2">
+        <v>115.5</v>
+      </c>
+      <c r="BJ2">
+        <v>108.24</v>
+      </c>
+      <c r="BK2">
+        <v>291.65</v>
+      </c>
+      <c r="BL2">
+        <v>191.17</v>
+      </c>
+      <c r="BM2">
+        <v>148.63</v>
+      </c>
+      <c r="BN2">
+        <v>70.54000000000001</v>
+      </c>
+      <c r="BO2">
+        <v>40.77</v>
+      </c>
+      <c r="BP2">
+        <v>63.92</v>
+      </c>
+      <c r="BQ2">
+        <v>67.20999999999999</v>
+      </c>
+      <c r="BR2">
+        <v>164.75</v>
+      </c>
+      <c r="BS2">
+        <v>33.2</v>
+      </c>
+      <c r="BT2">
+        <v>61.5</v>
+      </c>
+      <c r="BU2">
+        <v>49.35</v>
+      </c>
+      <c r="BV2">
+        <v>41.42</v>
+      </c>
+      <c r="BW2">
+        <v>173.05</v>
+      </c>
+      <c r="BX2">
+        <v>409.94</v>
+      </c>
+      <c r="BY2">
+        <v>263.41</v>
+      </c>
+      <c r="BZ2">
+        <v>16.77</v>
+      </c>
+      <c r="CA2">
+        <v>38.51</v>
+      </c>
+      <c r="CB2">
+        <v>75.84</v>
+      </c>
+      <c r="CC2">
+        <v>113.41</v>
+      </c>
+      <c r="CD2">
+        <v>51.09</v>
+      </c>
+      <c r="CE2">
+        <v>189.49</v>
+      </c>
+      <c r="CF2">
+        <v>251</v>
+      </c>
+      <c r="CG2">
+        <v>57.59</v>
+      </c>
+      <c r="CH2">
+        <v>102.35</v>
+      </c>
+      <c r="CI2">
+        <v>95.56</v>
+      </c>
+      <c r="CJ2">
+        <v>144.82</v>
+      </c>
+      <c r="CK2">
+        <v>572.1799999999999</v>
+      </c>
+      <c r="CL2">
+        <v>55.8</v>
+      </c>
+      <c r="CM2">
+        <v>25.69</v>
+      </c>
+      <c r="CN2">
+        <v>335.78</v>
+      </c>
+      <c r="CO2">
+        <v>122.6</v>
+      </c>
+      <c r="CP2">
+        <v>66.5</v>
+      </c>
+      <c r="CQ2">
+        <v>291.43</v>
+      </c>
+      <c r="CR2">
+        <v>228.68</v>
+      </c>
+      <c r="CS2">
+        <v>458.33</v>
+      </c>
+      <c r="CT2">
+        <v>371.11</v>
+      </c>
+      <c r="CU2">
+        <v>109.61</v>
+      </c>
+      <c r="CV2">
+        <v>132.37</v>
+      </c>
+      <c r="CW2">
+        <v>77.56</v>
+      </c>
+      <c r="CX2">
+        <v>300.06</v>
+      </c>
+      <c r="CY2">
+        <v>116.3</v>
+      </c>
+      <c r="CZ2">
+        <v>38.88</v>
+      </c>
+      <c r="DA2">
+        <v>70.88</v>
+      </c>
+      <c r="DB2">
+        <v>118.52</v>
+      </c>
+      <c r="DC2">
+        <v>29.28</v>
+      </c>
+      <c r="DD2">
+        <v>236.34</v>
+      </c>
+      <c r="DE2">
+        <v>41.99</v>
+      </c>
+      <c r="DF2">
+        <v>96.81</v>
+      </c>
+      <c r="DG2">
+        <v>243.87</v>
+      </c>
+      <c r="DH2">
+        <v>192.02</v>
+      </c>
+      <c r="DI2">
+        <v>23.15</v>
+      </c>
+      <c r="DJ2">
+        <v>48.48</v>
+      </c>
+      <c r="DK2">
+        <v>131.89</v>
+      </c>
+      <c r="DL2">
+        <v>107.15</v>
+      </c>
+      <c r="DM2">
+        <v>42.32</v>
+      </c>
+      <c r="DN2">
+        <v>43.87</v>
+      </c>
+      <c r="DO2">
+        <v>44.31</v>
+      </c>
+      <c r="DP2">
+        <v>33.46</v>
+      </c>
+      <c r="DQ2">
+        <v>109.7</v>
+      </c>
+      <c r="DR2">
+        <v>12.07</v>
+      </c>
+      <c r="DS2">
+        <v>33.85</v>
+      </c>
+      <c r="DT2">
+        <v>82.17</v>
+      </c>
+      <c r="DU2">
+        <v>70.54000000000001</v>
+      </c>
+      <c r="DV2">
+        <v>61.49</v>
+      </c>
+      <c r="DW2">
+        <v>99.95</v>
+      </c>
+      <c r="DX2">
+        <v>432.86</v>
+      </c>
+      <c r="DY2">
+        <v>60.93</v>
+      </c>
+      <c r="DZ2">
+        <v>44.44</v>
+      </c>
+      <c r="EA2">
+        <v>44.65</v>
+      </c>
+      <c r="EB2">
+        <v>18.6</v>
+      </c>
+      <c r="EC2">
+        <v>404</v>
+      </c>
+      <c r="ED2">
+        <v>80.17</v>
+      </c>
+      <c r="EE2">
         <v>74.73</v>
       </c>
-      <c r="AH2">
-        <v>55.73</v>
-      </c>
-      <c r="AI2">
-        <v>977.41</v>
-      </c>
-      <c r="AJ2">
-        <v>152.03</v>
-      </c>
-      <c r="AK2">
-        <v>113.84</v>
-      </c>
-      <c r="AL2">
+      <c r="EF2">
+        <v>25</v>
+      </c>
+      <c r="EG2">
+        <v>21.45</v>
+      </c>
+      <c r="EH2">
+        <v>157.01</v>
+      </c>
+      <c r="EI2">
+        <v>42.86</v>
+      </c>
+      <c r="EJ2">
+        <v>27.3</v>
+      </c>
+      <c r="EK2">
+        <v>89.36</v>
+      </c>
+      <c r="EL2">
+        <v>207.98</v>
+      </c>
+      <c r="EM2">
+        <v>67.94</v>
+      </c>
+      <c r="EN2">
+        <v>63.24</v>
+      </c>
+      <c r="EO2">
+        <v>126.92</v>
+      </c>
+      <c r="EP2">
+        <v>21.75</v>
+      </c>
+      <c r="EQ2">
+        <v>27.94</v>
+      </c>
+      <c r="ER2">
+        <v>204.4</v>
+      </c>
+      <c r="ES2">
+        <v>391.26</v>
+      </c>
+      <c r="ET2">
+        <v>39.7</v>
+      </c>
+      <c r="EU2">
+        <v>18.16</v>
+      </c>
+      <c r="EV2">
+        <v>156.82</v>
+      </c>
+      <c r="EW2">
+        <v>256.7</v>
+      </c>
+      <c r="EX2">
+        <v>51.63</v>
+      </c>
+      <c r="EY2">
+        <v>90.72</v>
+      </c>
+      <c r="EZ2">
+        <v>59.97</v>
+      </c>
+      <c r="FA2">
+        <v>46.03</v>
+      </c>
+      <c r="FB2">
+        <v>490.72</v>
+      </c>
+      <c r="FC2">
+        <v>51.72</v>
+      </c>
+      <c r="FD2">
+        <v>179</v>
+      </c>
+      <c r="FE2">
+        <v>67.45</v>
+      </c>
+      <c r="FF2">
+        <v>58.17</v>
+      </c>
+      <c r="FG2">
+        <v>98.95999999999999</v>
+      </c>
+      <c r="FH2">
+        <v>73.56</v>
+      </c>
+      <c r="FI2">
+        <v>124.07</v>
+      </c>
+      <c r="FJ2">
+        <v>76.41</v>
+      </c>
+      <c r="FK2">
+        <v>233.34</v>
+      </c>
+      <c r="FL2">
+        <v>148.55</v>
+      </c>
+      <c r="FM2">
+        <v>29.73</v>
+      </c>
+      <c r="FN2">
+        <v>224.91</v>
+      </c>
+      <c r="FO2">
+        <v>73</v>
+      </c>
+      <c r="FP2">
+        <v>69.11</v>
+      </c>
+      <c r="FQ2">
+        <v>63.05</v>
+      </c>
+      <c r="FR2">
+        <v>106.81</v>
+      </c>
+      <c r="FS2">
+        <v>170.05</v>
+      </c>
+      <c r="FT2">
+        <v>100.89</v>
+      </c>
+      <c r="FU2">
+        <v>206.84</v>
+      </c>
+      <c r="FV2">
+        <v>909.26</v>
+      </c>
+      <c r="FW2">
+        <v>43.99</v>
+      </c>
+      <c r="FX2">
+        <v>261.5</v>
+      </c>
+      <c r="FY2">
+        <v>82.51000000000001</v>
+      </c>
+      <c r="FZ2">
+        <v>105.77</v>
+      </c>
+      <c r="GA2">
+        <v>126.71</v>
+      </c>
+      <c r="GB2">
+        <v>141.64</v>
+      </c>
+      <c r="GC2">
+        <v>119.1</v>
+      </c>
+      <c r="GD2">
+        <v>68.47</v>
+      </c>
+      <c r="GE2">
+        <v>55.32</v>
+      </c>
+      <c r="GF2">
+        <v>53.14</v>
+      </c>
+      <c r="GG2">
+        <v>150.38</v>
+      </c>
+      <c r="GH2">
+        <v>267.43</v>
+      </c>
+      <c r="GI2">
+        <v>29.57</v>
+      </c>
+      <c r="GJ2">
+        <v>95</v>
+      </c>
+      <c r="GK2">
+        <v>69.54000000000001</v>
+      </c>
+      <c r="GL2">
+        <v>49.77</v>
+      </c>
+      <c r="GM2">
+        <v>322.1</v>
+      </c>
+      <c r="GN2">
+        <v>492.64</v>
+      </c>
+      <c r="GO2">
+        <v>220.42</v>
+      </c>
+      <c r="GP2">
+        <v>126.83</v>
+      </c>
+      <c r="GQ2">
+        <v>120.74</v>
+      </c>
+      <c r="GR2">
+        <v>102.02</v>
+      </c>
+      <c r="GS2">
+        <v>44.96</v>
+      </c>
+      <c r="GT2">
+        <v>124.73</v>
+      </c>
+      <c r="GU2">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="GV2">
+        <v>35.19</v>
+      </c>
+      <c r="GW2">
+        <v>22.09</v>
+      </c>
+      <c r="GX2">
+        <v>73.5</v>
+      </c>
+      <c r="GY2">
+        <v>61.07</v>
+      </c>
+      <c r="GZ2">
+        <v>163.65</v>
+      </c>
+      <c r="HA2">
+        <v>43.74</v>
+      </c>
+      <c r="HB2">
+        <v>206.84</v>
+      </c>
+      <c r="HC2">
+        <v>233.88</v>
+      </c>
+      <c r="HD2">
+        <v>232.9</v>
+      </c>
+      <c r="HE2">
+        <v>129.28</v>
+      </c>
+      <c r="HF2">
+        <v>661.17</v>
+      </c>
+      <c r="HG2">
+        <v>128.24</v>
+      </c>
+      <c r="HH2">
+        <v>338.36</v>
+      </c>
+      <c r="HI2">
+        <v>75.13</v>
+      </c>
+      <c r="HJ2">
+        <v>335.66</v>
+      </c>
+      <c r="HK2">
+        <v>83.26000000000001</v>
+      </c>
+      <c r="HL2">
+        <v>25.77</v>
+      </c>
+      <c r="HM2">
+        <v>151.48</v>
+      </c>
+      <c r="HN2">
+        <v>110.27</v>
+      </c>
+      <c r="HO2">
+        <v>81.34</v>
+      </c>
+      <c r="HP2">
+        <v>234.75</v>
+      </c>
+      <c r="HQ2">
+        <v>79.08</v>
+      </c>
+      <c r="HR2">
+        <v>141.13</v>
+      </c>
+      <c r="HS2">
+        <v>594.11</v>
+      </c>
+      <c r="HT2">
+        <v>36.75</v>
+      </c>
+      <c r="HU2">
+        <v>69.06999999999999</v>
+      </c>
+      <c r="HV2">
+        <v>230.67</v>
+      </c>
+      <c r="HW2">
+        <v>569.55</v>
+      </c>
+      <c r="HX2">
+        <v>224.54</v>
+      </c>
+      <c r="HY2">
+        <v>52.46</v>
+      </c>
+      <c r="HZ2">
+        <v>951.73</v>
+      </c>
+      <c r="IA2">
+        <v>41.61</v>
+      </c>
+      <c r="IB2">
+        <v>13.34</v>
+      </c>
+      <c r="IC2">
+        <v>327.97</v>
+      </c>
+      <c r="ID2">
+        <v>57.1</v>
+      </c>
+      <c r="IE2">
+        <v>78.92</v>
+      </c>
+      <c r="IF2">
+        <v>119.21</v>
+      </c>
+      <c r="IG2">
+        <v>73.52</v>
+      </c>
+      <c r="IH2">
+        <v>152.23</v>
+      </c>
+      <c r="II2">
+        <v>191.86</v>
+      </c>
+      <c r="IJ2">
+        <v>88.69</v>
+      </c>
+      <c r="IK2">
+        <v>295.44</v>
+      </c>
+      <c r="IL2">
+        <v>258.79</v>
+      </c>
+      <c r="IM2">
+        <v>24.25</v>
+      </c>
+      <c r="IN2">
+        <v>41.23</v>
+      </c>
+      <c r="IO2">
+        <v>115.1</v>
+      </c>
+      <c r="IP2">
+        <v>459.49</v>
+      </c>
+      <c r="IQ2">
+        <v>63.44</v>
+      </c>
+      <c r="IR2">
+        <v>181.91</v>
+      </c>
+      <c r="IS2">
+        <v>232.31</v>
+      </c>
+      <c r="IT2">
+        <v>216.87</v>
+      </c>
+      <c r="IU2">
+        <v>36.42</v>
+      </c>
+      <c r="IV2">
+        <v>28.68</v>
+      </c>
+      <c r="IW2">
+        <v>351.15</v>
+      </c>
+      <c r="IX2">
+        <v>167.18</v>
+      </c>
+      <c r="IY2">
+        <v>516.85</v>
+      </c>
+      <c r="IZ2">
+        <v>43.36</v>
+      </c>
+      <c r="JA2">
+        <v>191.66</v>
+      </c>
+      <c r="JB2">
+        <v>161.27</v>
+      </c>
+      <c r="JC2">
+        <v>706.49</v>
+      </c>
+      <c r="JD2">
+        <v>105.11</v>
+      </c>
+      <c r="JE2">
+        <v>31.55</v>
+      </c>
+      <c r="JF2">
+        <v>130.33</v>
+      </c>
+      <c r="JG2">
+        <v>306.21</v>
+      </c>
+      <c r="JH2">
+        <v>241.63</v>
+      </c>
+      <c r="JI2">
+        <v>83.48999999999999</v>
+      </c>
+      <c r="JJ2">
+        <v>209.79</v>
+      </c>
+      <c r="JK2">
+        <v>57.68</v>
+      </c>
+      <c r="JL2">
+        <v>57.54</v>
+      </c>
+      <c r="JM2">
+        <v>63.07</v>
+      </c>
+      <c r="JN2">
+        <v>43.36</v>
+      </c>
+      <c r="JO2">
+        <v>119.25</v>
+      </c>
+      <c r="JP2">
+        <v>210.12</v>
+      </c>
+      <c r="JQ2">
+        <v>28</v>
+      </c>
+      <c r="JR2">
+        <v>93.11</v>
+      </c>
+      <c r="JS2">
+        <v>86.59999999999999</v>
+      </c>
+      <c r="JT2">
+        <v>143.02</v>
+      </c>
+      <c r="JU2">
+        <v>97.11</v>
+      </c>
+      <c r="JV2">
+        <v>26.28</v>
+      </c>
+      <c r="JW2">
+        <v>154.91</v>
+      </c>
+      <c r="JX2">
+        <v>62.69</v>
+      </c>
+      <c r="JY2">
+        <v>29.38</v>
+      </c>
+      <c r="JZ2">
+        <v>214.77</v>
+      </c>
+      <c r="KA2">
+        <v>161.17</v>
+      </c>
+      <c r="KB2">
+        <v>83.55</v>
+      </c>
+      <c r="KC2">
+        <v>65.69</v>
+      </c>
+      <c r="KD2">
+        <v>331.79</v>
+      </c>
+      <c r="KE2">
+        <v>174.58</v>
+      </c>
+      <c r="KF2">
+        <v>38.39</v>
+      </c>
+      <c r="KG2">
+        <v>263.35</v>
+      </c>
+      <c r="KH2">
+        <v>60.3</v>
+      </c>
+      <c r="KI2">
+        <v>427.19</v>
+      </c>
+      <c r="KJ2">
+        <v>77.97</v>
+      </c>
+      <c r="KK2">
+        <v>97.06999999999999</v>
+      </c>
+      <c r="KL2">
+        <v>277.56</v>
+      </c>
+      <c r="KM2">
+        <v>167.11</v>
+      </c>
+      <c r="KN2">
+        <v>353.25</v>
+      </c>
+      <c r="KO2">
+        <v>164.83</v>
+      </c>
+      <c r="KP2">
+        <v>19.62</v>
+      </c>
+      <c r="KQ2">
+        <v>35.02</v>
+      </c>
+      <c r="KR2">
+        <v>64.8</v>
+      </c>
+      <c r="KS2">
+        <v>143.8</v>
+      </c>
+      <c r="KT2">
+        <v>39.48</v>
+      </c>
+      <c r="KU2">
+        <v>35.7</v>
+      </c>
+      <c r="KV2">
+        <v>284.52</v>
+      </c>
+      <c r="KW2">
+        <v>320.14</v>
+      </c>
+      <c r="KX2">
+        <v>173.61</v>
+      </c>
+      <c r="KY2">
+        <v>122.67</v>
+      </c>
+      <c r="KZ2">
+        <v>90.55</v>
+      </c>
+      <c r="LA2">
+        <v>164.72</v>
+      </c>
+      <c r="LB2">
+        <v>118.12</v>
+      </c>
+      <c r="LC2">
+        <v>112.1</v>
+      </c>
+      <c r="LD2">
+        <v>42.84</v>
+      </c>
+      <c r="LE2">
+        <v>32.01</v>
+      </c>
+      <c r="LF2">
+        <v>96.27</v>
+      </c>
+      <c r="LG2">
+        <v>206.47</v>
+      </c>
+      <c r="LH2">
+        <v>27.66</v>
+      </c>
+      <c r="LI2">
+        <v>189.32</v>
+      </c>
+      <c r="LJ2">
+        <v>20.39</v>
+      </c>
+      <c r="LK2">
+        <v>52.97</v>
+      </c>
+      <c r="LL2">
+        <v>93.76000000000001</v>
+      </c>
+      <c r="LM2">
+        <v>25.37</v>
+      </c>
+      <c r="LN2">
+        <v>38.22</v>
+      </c>
+      <c r="LO2">
+        <v>46.73</v>
+      </c>
+      <c r="LP2">
+        <v>104.14</v>
+      </c>
+      <c r="LQ2">
+        <v>66.59999999999999</v>
+      </c>
+      <c r="LR2">
+        <v>60.43</v>
+      </c>
+      <c r="LS2">
+        <v>118.47</v>
+      </c>
+      <c r="LT2">
+        <v>54</v>
+      </c>
+      <c r="LU2">
+        <v>85.38</v>
+      </c>
+      <c r="LV2">
+        <v>316.04</v>
+      </c>
+      <c r="LW2">
+        <v>34.47</v>
+      </c>
+      <c r="LX2">
+        <v>19.53</v>
+      </c>
+      <c r="LY2">
+        <v>173.11</v>
+      </c>
+      <c r="LZ2">
+        <v>92.45</v>
+      </c>
+      <c r="MA2">
+        <v>28.51</v>
+      </c>
+      <c r="MB2">
+        <v>16.9</v>
+      </c>
+      <c r="MC2">
+        <v>71.05</v>
+      </c>
+      <c r="MD2">
+        <v>82.20999999999999</v>
+      </c>
+      <c r="ME2">
+        <v>390.35</v>
+      </c>
+      <c r="MF2">
+        <v>120.75</v>
+      </c>
+      <c r="MG2">
+        <v>31.3</v>
+      </c>
+      <c r="MH2">
+        <v>63.53</v>
+      </c>
+      <c r="MI2">
+        <v>23.7</v>
+      </c>
+      <c r="MJ2">
+        <v>422.71</v>
+      </c>
+      <c r="MK2">
+        <v>48.53</v>
+      </c>
+      <c r="ML2">
+        <v>565.14</v>
+      </c>
+      <c r="MM2">
+        <v>15.56</v>
+      </c>
+      <c r="MN2">
+        <v>71.55</v>
+      </c>
+      <c r="MO2">
+        <v>604.04</v>
+      </c>
+      <c r="MP2">
+        <v>70.8</v>
+      </c>
+      <c r="MQ2">
+        <v>82.98</v>
+      </c>
+      <c r="MR2">
+        <v>40.24</v>
+      </c>
+      <c r="MS2">
+        <v>23.78</v>
+      </c>
+      <c r="MT2">
+        <v>15.28</v>
+      </c>
+      <c r="MU2">
+        <v>29.2</v>
+      </c>
+      <c r="MV2">
+        <v>266.17</v>
+      </c>
+      <c r="MW2">
+        <v>29.5</v>
+      </c>
+      <c r="MX2">
+        <v>305.32</v>
+      </c>
+      <c r="MY2">
+        <v>191.51</v>
+      </c>
+      <c r="MZ2">
+        <v>114.24</v>
+      </c>
+      <c r="NA2">
+        <v>535.6900000000001</v>
+      </c>
+      <c r="NB2">
+        <v>16.15</v>
+      </c>
+      <c r="NC2">
+        <v>194.41</v>
+      </c>
+      <c r="ND2">
+        <v>22.51</v>
+      </c>
+      <c r="NE2">
+        <v>218.27</v>
+      </c>
+      <c r="NF2">
+        <v>210.01</v>
+      </c>
+      <c r="NG2">
+        <v>82.36</v>
+      </c>
+      <c r="NH2">
+        <v>44.25</v>
+      </c>
+      <c r="NI2">
+        <v>13.05</v>
+      </c>
+      <c r="NJ2">
+        <v>12.27</v>
+      </c>
+      <c r="NK2">
+        <v>93.09</v>
+      </c>
+      <c r="NL2">
+        <v>125.49</v>
+      </c>
+      <c r="NM2">
+        <v>352.15</v>
+      </c>
+      <c r="NN2">
+        <v>54.88</v>
+      </c>
+      <c r="NO2">
+        <v>47.07</v>
+      </c>
+      <c r="NP2">
+        <v>107.5</v>
+      </c>
+      <c r="NQ2">
+        <v>51.72</v>
+      </c>
+      <c r="NR2">
+        <v>49.51</v>
+      </c>
+      <c r="NS2">
+        <v>56.63</v>
+      </c>
+      <c r="NT2">
+        <v>40.39</v>
+      </c>
+      <c r="NU2">
+        <v>68.31</v>
+      </c>
+      <c r="NV2">
+        <v>163.03</v>
+      </c>
+      <c r="NW2">
+        <v>30.09</v>
+      </c>
+      <c r="NX2">
+        <v>37.03</v>
+      </c>
+      <c r="NY2">
+        <v>34.02</v>
+      </c>
+      <c r="NZ2">
+        <v>461.4</v>
+      </c>
+      <c r="OA2">
+        <v>38.71</v>
+      </c>
+      <c r="OB2">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="OC2">
+        <v>219.7</v>
+      </c>
+      <c r="OD2">
+        <v>88.27</v>
+      </c>
+      <c r="OE2">
+        <v>141.06</v>
+      </c>
+      <c r="OF2">
+        <v>67</v>
+      </c>
+      <c r="OG2">
+        <v>71.5</v>
+      </c>
+      <c r="OH2">
+        <v>21.71</v>
+      </c>
+      <c r="OI2">
+        <v>40.99</v>
+      </c>
+      <c r="OJ2">
+        <v>47.49</v>
+      </c>
+      <c r="OK2">
+        <v>176.99</v>
+      </c>
+      <c r="OL2">
+        <v>38.2</v>
+      </c>
+      <c r="OM2">
+        <v>30.53</v>
+      </c>
+      <c r="ON2">
+        <v>26.03</v>
+      </c>
+      <c r="OO2">
+        <v>25.08</v>
+      </c>
+      <c r="OP2">
+        <v>26.51</v>
+      </c>
+      <c r="OQ2">
+        <v>53.7</v>
+      </c>
+      <c r="OR2">
+        <v>201.47</v>
+      </c>
+      <c r="OS2">
+        <v>135.05</v>
+      </c>
+      <c r="OT2">
+        <v>42.8</v>
+      </c>
+      <c r="OU2">
+        <v>44.56</v>
+      </c>
+      <c r="OV2">
+        <v>75.55</v>
+      </c>
+      <c r="OW2">
+        <v>85.63</v>
+      </c>
+      <c r="OX2">
+        <v>28.04</v>
+      </c>
+      <c r="OY2">
+        <v>53.51</v>
+      </c>
+      <c r="OZ2">
+        <v>335.28</v>
+      </c>
+      <c r="PA2">
+        <v>206.95</v>
+      </c>
+      <c r="PB2">
+        <v>126.34</v>
+      </c>
+      <c r="PC2">
+        <v>98.91</v>
+      </c>
+      <c r="PD2">
+        <v>149.08</v>
+      </c>
+      <c r="PE2">
+        <v>497</v>
+      </c>
+      <c r="PF2">
+        <v>64.51000000000001</v>
+      </c>
+      <c r="PG2">
+        <v>174.39</v>
+      </c>
+      <c r="PH2">
+        <v>69.59999999999999</v>
+      </c>
+      <c r="PI2">
+        <v>129.23</v>
+      </c>
+      <c r="PJ2">
+        <v>113.45</v>
+      </c>
+      <c r="PK2">
+        <v>60.19</v>
+      </c>
+      <c r="PL2">
+        <v>837.5700000000001</v>
+      </c>
+      <c r="PM2">
+        <v>24.79</v>
+      </c>
+      <c r="PN2">
+        <v>96.01000000000001</v>
+      </c>
+      <c r="PO2">
+        <v>10.45</v>
+      </c>
+      <c r="PP2">
+        <v>144.44</v>
+      </c>
+      <c r="PQ2">
+        <v>20.86</v>
+      </c>
+      <c r="PR2">
+        <v>298.12</v>
+      </c>
+      <c r="PS2">
+        <v>22.5</v>
+      </c>
+      <c r="PT2">
+        <v>18.02</v>
+      </c>
+      <c r="PU2">
+        <v>37.11</v>
+      </c>
+      <c r="PV2">
+        <v>234.08</v>
+      </c>
+      <c r="PW2">
+        <v>42.14</v>
+      </c>
+      <c r="PX2">
+        <v>46.99</v>
+      </c>
+      <c r="PY2">
+        <v>100.53</v>
+      </c>
+      <c r="PZ2">
+        <v>165.57</v>
+      </c>
+      <c r="QA2">
+        <v>41.04</v>
+      </c>
+      <c r="QB2">
+        <v>74.18000000000001</v>
+      </c>
+      <c r="QC2">
+        <v>13.1</v>
+      </c>
+      <c r="QD2">
+        <v>127.06</v>
+      </c>
+      <c r="QE2">
+        <v>155.45</v>
+      </c>
+      <c r="QF2">
+        <v>35.79</v>
+      </c>
+      <c r="QG2">
+        <v>20.99</v>
+      </c>
+      <c r="QH2">
+        <v>128.84</v>
+      </c>
+      <c r="QI2">
+        <v>42.47</v>
+      </c>
+      <c r="QJ2">
+        <v>21.52</v>
+      </c>
+      <c r="QK2">
+        <v>59.81</v>
+      </c>
+      <c r="QL2">
+        <v>27.42</v>
+      </c>
+      <c r="QM2">
+        <v>13.21</v>
+      </c>
+      <c r="QN2">
+        <v>80.87</v>
+      </c>
+      <c r="QO2">
+        <v>95.78</v>
+      </c>
+      <c r="QP2">
+        <v>24.14</v>
+      </c>
+      <c r="QQ2">
+        <v>16.03</v>
+      </c>
+      <c r="QR2">
+        <v>531.42</v>
+      </c>
+      <c r="QS2">
+        <v>120.14</v>
+      </c>
+      <c r="QT2">
+        <v>88.70999999999999</v>
+      </c>
+      <c r="QU2">
+        <v>39.04</v>
+      </c>
+      <c r="QV2">
+        <v>108.42</v>
+      </c>
+      <c r="QW2">
+        <v>108.22</v>
+      </c>
+      <c r="QX2">
+        <v>52.05</v>
+      </c>
+      <c r="QY2">
+        <v>39.78</v>
+      </c>
+      <c r="QZ2">
+        <v>75.84</v>
+      </c>
+      <c r="RA2">
+        <v>31.06</v>
+      </c>
+      <c r="RB2">
+        <v>22.27</v>
+      </c>
+      <c r="RC2">
+        <v>172.26</v>
+      </c>
+      <c r="RD2">
+        <v>44.41</v>
+      </c>
+      <c r="RE2">
+        <v>73.08</v>
+      </c>
+      <c r="RF2">
+        <v>92.25</v>
+      </c>
+      <c r="RG2">
+        <v>50.2</v>
+      </c>
+      <c r="RH2">
+        <v>56.53</v>
+      </c>
+      <c r="RI2">
+        <v>562.5599999999999</v>
+      </c>
+      <c r="RJ2">
+        <v>17.73</v>
+      </c>
+      <c r="RK2">
+        <v>17.2</v>
+      </c>
+      <c r="RL2">
+        <v>26.84</v>
+      </c>
+      <c r="RM2">
+        <v>111.72</v>
+      </c>
+      <c r="RN2">
+        <v>89.97</v>
+      </c>
+      <c r="RO2">
+        <v>834.59</v>
+      </c>
+      <c r="RP2">
+        <v>43.33</v>
+      </c>
+      <c r="RQ2">
+        <v>80.79000000000001</v>
+      </c>
+      <c r="RR2">
+        <v>195.45</v>
+      </c>
+      <c r="RS2">
+        <v>211.36</v>
+      </c>
+      <c r="RT2">
+        <v>47.44</v>
+      </c>
+      <c r="RU2">
+        <v>28.64</v>
+      </c>
+      <c r="RV2">
+        <v>55.03</v>
+      </c>
+      <c r="RW2">
+        <v>81.78</v>
+      </c>
+      <c r="RX2">
+        <v>83.88</v>
+      </c>
+      <c r="RY2">
+        <v>28.7</v>
+      </c>
+      <c r="RZ2">
+        <v>29.04</v>
+      </c>
+      <c r="SA2">
+        <v>106.39</v>
+      </c>
+      <c r="SB2">
+        <v>67.25</v>
+      </c>
+      <c r="SC2">
+        <v>27.98</v>
+      </c>
+      <c r="SD2">
+        <v>37.97</v>
+      </c>
+      <c r="SE2">
+        <v>183.56</v>
+      </c>
+      <c r="SF2">
+        <v>55.23</v>
+      </c>
+      <c r="SG2">
+        <v>155.83</v>
+      </c>
+      <c r="SH2">
+        <v>28.72</v>
+      </c>
+      <c r="SI2">
+        <v>216.23</v>
+      </c>
+      <c r="SJ2">
+        <v>43.67</v>
+      </c>
+      <c r="SK2">
+        <v>26.38</v>
+      </c>
+      <c r="SL2">
+        <v>30.44</v>
+      </c>
+      <c r="SM2">
+        <v>60.87</v>
+      </c>
+      <c r="SN2">
+        <v>25.23</v>
+      </c>
+      <c r="SO2">
+        <v>177.42</v>
+      </c>
+      <c r="SP2">
+        <v>28.11</v>
+      </c>
+      <c r="SQ2">
+        <v>22.7</v>
+      </c>
+      <c r="SR2">
+        <v>170.3</v>
+      </c>
+      <c r="SS2">
         <v>83.66</v>
       </c>
-      <c r="AM2">
-        <v>151.34</v>
-      </c>
-      <c r="AN2">
-        <v>227.83</v>
-      </c>
-      <c r="AO2">
-        <v>139.91</v>
-      </c>
-      <c r="AP2">
-        <v>494.27</v>
-      </c>
-      <c r="AQ2">
-        <v>129.5</v>
-      </c>
-      <c r="AR2">
-        <v>87.45999999999999</v>
-      </c>
-      <c r="AS2">
-        <v>116.13</v>
-      </c>
-      <c r="AT2">
-        <v>107.62</v>
-      </c>
-      <c r="AU2">
-        <v>34.86</v>
-      </c>
-      <c r="AV2">
-        <v>296.58</v>
-      </c>
-      <c r="AW2">
-        <v>93.04000000000001</v>
-      </c>
-      <c r="AX2">
-        <v>303.97</v>
-      </c>
-      <c r="AY2">
-        <v>76.62</v>
-      </c>
-      <c r="AZ2">
-        <v>47.99</v>
-      </c>
-      <c r="BA2">
-        <v>342.77</v>
-      </c>
-      <c r="BB2">
-        <v>93.34999999999999</v>
-      </c>
-      <c r="BC2">
-        <v>148.43</v>
-      </c>
-      <c r="BD2">
-        <v>342.25</v>
-      </c>
-      <c r="BE2">
-        <v>19.8</v>
-      </c>
-      <c r="BF2">
-        <v>51.54</v>
-      </c>
-      <c r="BG2">
-        <v>37.5</v>
-      </c>
-      <c r="BH2">
-        <v>47.17</v>
-      </c>
-      <c r="BI2">
-        <v>113.76</v>
-      </c>
-      <c r="BJ2">
-        <v>108.4</v>
-      </c>
-      <c r="BK2">
-        <v>295.62</v>
-      </c>
-      <c r="BL2">
-        <v>195.17</v>
-      </c>
-      <c r="BM2">
-        <v>151.48</v>
-      </c>
-      <c r="BN2">
-        <v>71.97</v>
-      </c>
-      <c r="BO2">
-        <v>41.77</v>
-      </c>
-      <c r="BP2">
-        <v>64.14</v>
-      </c>
-      <c r="BQ2">
-        <v>69.01000000000001</v>
-      </c>
-      <c r="BR2">
-        <v>158.72</v>
-      </c>
-      <c r="BS2">
-        <v>33.04</v>
-      </c>
-      <c r="BT2">
-        <v>62.78</v>
-      </c>
-      <c r="BU2">
-        <v>49.66</v>
-      </c>
-      <c r="BV2">
-        <v>42.37</v>
-      </c>
-      <c r="BW2">
-        <v>177.19</v>
-      </c>
-      <c r="BX2">
-        <v>425.25</v>
-      </c>
-      <c r="BY2">
-        <v>265.18</v>
-      </c>
-      <c r="BZ2">
-        <v>16.9</v>
-      </c>
-      <c r="CA2">
-        <v>39.85</v>
-      </c>
-      <c r="CB2">
-        <v>74.95999999999999</v>
-      </c>
-      <c r="CC2">
-        <v>114.49</v>
-      </c>
-      <c r="CD2">
-        <v>51.17</v>
-      </c>
-      <c r="CE2">
-        <v>199.74</v>
-      </c>
-      <c r="CF2">
-        <v>251.88</v>
-      </c>
-      <c r="CG2">
-        <v>57.12</v>
-      </c>
-      <c r="CH2">
-        <v>101.94</v>
-      </c>
-      <c r="CI2">
-        <v>100.28</v>
-      </c>
-      <c r="CJ2">
-        <v>147.84</v>
-      </c>
-      <c r="CK2">
-        <v>575.59</v>
-      </c>
-      <c r="CL2">
-        <v>56.98</v>
-      </c>
-      <c r="CM2">
-        <v>25.96</v>
-      </c>
-      <c r="CN2">
-        <v>342.64</v>
-      </c>
-      <c r="CO2">
-        <v>124.49</v>
-      </c>
-      <c r="CP2">
-        <v>67.48999999999999</v>
-      </c>
-      <c r="CQ2">
-        <v>297.4</v>
-      </c>
-      <c r="CR2">
-        <v>231.46</v>
-      </c>
-      <c r="CS2">
-        <v>460.31</v>
-      </c>
-      <c r="CT2">
-        <v>373.49</v>
-      </c>
-      <c r="CU2">
-        <v>111.13</v>
-      </c>
-      <c r="CV2">
-        <v>132.05</v>
-      </c>
-      <c r="CW2">
-        <v>79.34</v>
-      </c>
-      <c r="CX2">
-        <v>300.29</v>
-      </c>
-      <c r="CY2">
-        <v>116.9</v>
-      </c>
-      <c r="CZ2">
-        <v>39.84</v>
-      </c>
-      <c r="DA2">
-        <v>72.11</v>
-      </c>
-      <c r="DB2">
-        <v>120.08</v>
-      </c>
-      <c r="DC2">
-        <v>29.32</v>
-      </c>
-      <c r="DD2">
-        <v>245.29</v>
-      </c>
-      <c r="DE2">
-        <v>44.01</v>
-      </c>
-      <c r="DF2">
-        <v>98.2</v>
-      </c>
-      <c r="DG2">
-        <v>252.97</v>
-      </c>
-      <c r="DH2">
-        <v>190.98</v>
-      </c>
-      <c r="DI2">
-        <v>22.88</v>
-      </c>
-      <c r="DJ2">
-        <v>49.24</v>
-      </c>
-      <c r="DK2">
-        <v>130.03</v>
-      </c>
-      <c r="DL2">
-        <v>109.32</v>
-      </c>
-      <c r="DM2">
-        <v>43.64</v>
-      </c>
-      <c r="DN2">
-        <v>43.5</v>
-      </c>
-      <c r="DO2">
-        <v>44.26</v>
-      </c>
-      <c r="DP2">
-        <v>34.47</v>
-      </c>
-      <c r="DQ2">
-        <v>111.87</v>
-      </c>
-      <c r="DR2">
-        <v>12.1</v>
-      </c>
-      <c r="DS2">
-        <v>33.92</v>
-      </c>
-      <c r="DT2">
-        <v>84.37</v>
-      </c>
-      <c r="DU2">
-        <v>70.84</v>
-      </c>
-      <c r="DV2">
-        <v>62.61</v>
-      </c>
-      <c r="DW2">
-        <v>101</v>
-      </c>
-      <c r="DX2">
-        <v>439.65</v>
-      </c>
-      <c r="DY2">
-        <v>61.5</v>
-      </c>
-      <c r="DZ2">
-        <v>44.49</v>
-      </c>
-      <c r="EA2">
-        <v>18.42</v>
-      </c>
-      <c r="EB2">
-        <v>399.68</v>
-      </c>
-      <c r="EC2">
-        <v>81.86</v>
-      </c>
-      <c r="ED2">
-        <v>76.06999999999999</v>
-      </c>
-      <c r="EE2">
-        <v>25.07</v>
-      </c>
-      <c r="EF2">
-        <v>20.59</v>
-      </c>
-      <c r="EG2">
-        <v>155.09</v>
-      </c>
-      <c r="EH2">
-        <v>43.34</v>
-      </c>
-      <c r="EI2">
-        <v>24.97</v>
-      </c>
-      <c r="EJ2">
-        <v>90.54000000000001</v>
-      </c>
-      <c r="EK2">
-        <v>212.98</v>
-      </c>
-      <c r="EL2">
-        <v>73.7</v>
-      </c>
-      <c r="EM2">
-        <v>64.08</v>
-      </c>
-      <c r="EN2">
-        <v>129.93</v>
-      </c>
-      <c r="EO2">
-        <v>20.95</v>
-      </c>
-      <c r="EP2">
-        <v>28.27</v>
-      </c>
-      <c r="EQ2">
-        <v>211.68</v>
-      </c>
-      <c r="ER2">
-        <v>388.7</v>
-      </c>
-      <c r="ES2">
-        <v>39.99</v>
-      </c>
-      <c r="ET2">
-        <v>18.78</v>
-      </c>
-      <c r="EU2">
-        <v>157.95</v>
-      </c>
-      <c r="EV2">
-        <v>265.13</v>
-      </c>
-      <c r="EW2">
-        <v>51.8</v>
-      </c>
-      <c r="EX2">
-        <v>92.81999999999999</v>
-      </c>
-      <c r="EY2">
-        <v>60.9</v>
-      </c>
-      <c r="EZ2">
+      <c r="ST2">
+        <v>82.12</v>
+      </c>
+      <c r="SU2">
+        <v>11.61</v>
+      </c>
+      <c r="SV2">
+        <v>162.64</v>
+      </c>
+      <c r="SW2">
+        <v>71.20999999999999</v>
+      </c>
+      <c r="SX2">
+        <v>56.2</v>
+      </c>
+      <c r="SY2">
+        <v>52.49</v>
+      </c>
+      <c r="SZ2">
+        <v>18.21</v>
+      </c>
+      <c r="TA2">
+        <v>113.6</v>
+      </c>
+      <c r="TB2">
+        <v>477.03</v>
+      </c>
+      <c r="TC2">
+        <v>107.08</v>
+      </c>
+      <c r="TD2">
+        <v>88.16</v>
+      </c>
+      <c r="TE2">
+        <v>99.38</v>
+      </c>
+      <c r="TF2">
+        <v>96.7</v>
+      </c>
+      <c r="TG2">
+        <v>30.92</v>
+      </c>
+      <c r="TH2">
+        <v>38.85</v>
+      </c>
+      <c r="TI2">
+        <v>53.08</v>
+      </c>
+      <c r="TJ2">
+        <v>37.84</v>
+      </c>
+      <c r="TK2">
+        <v>38.15</v>
+      </c>
+      <c r="TL2">
+        <v>256.05</v>
+      </c>
+      <c r="TM2">
+        <v>22.3</v>
+      </c>
+      <c r="TN2">
+        <v>81.93000000000001</v>
+      </c>
+      <c r="TO2">
+        <v>29.73</v>
+      </c>
+      <c r="TP2">
+        <v>30.5</v>
+      </c>
+      <c r="TQ2">
+        <v>30.33</v>
+      </c>
+      <c r="TR2">
+        <v>470.04</v>
+      </c>
+      <c r="TS2">
+        <v>16.29</v>
+      </c>
+      <c r="TT2">
+        <v>61.89</v>
+      </c>
+      <c r="TU2">
+        <v>175.92</v>
+      </c>
+      <c r="TV2">
+        <v>45</v>
+      </c>
+      <c r="TW2">
+        <v>70.45999999999999</v>
+      </c>
+      <c r="TX2">
+        <v>28.72</v>
+      </c>
+      <c r="TY2">
+        <v>148.5</v>
+      </c>
+      <c r="TZ2">
+        <v>101.92</v>
+      </c>
+      <c r="UA2">
         <v>48.74</v>
       </c>
-      <c r="FA2">
-        <v>490.5</v>
-      </c>
-      <c r="FB2">
-        <v>55.26</v>
-      </c>
-      <c r="FC2">
-        <v>179.99</v>
-      </c>
-      <c r="FD2">
-        <v>67.64</v>
-      </c>
-      <c r="FE2">
-        <v>58.96</v>
-      </c>
-      <c r="FF2">
-        <v>97.98</v>
-      </c>
-      <c r="FG2">
-        <v>73.77</v>
-      </c>
-      <c r="FH2">
-        <v>127.69</v>
-      </c>
-      <c r="FI2">
-        <v>76.27</v>
-      </c>
-      <c r="FJ2">
-        <v>235.76</v>
-      </c>
-      <c r="FK2">
-        <v>149.46</v>
-      </c>
-      <c r="FL2">
-        <v>30.57</v>
-      </c>
-      <c r="FM2">
-        <v>228.19</v>
-      </c>
-      <c r="FN2">
-        <v>73.22</v>
-      </c>
-      <c r="FO2">
-        <v>69.95999999999999</v>
-      </c>
-      <c r="FP2">
-        <v>63.53</v>
-      </c>
-      <c r="FQ2">
-        <v>107.12</v>
-      </c>
-      <c r="FR2">
-        <v>170.84</v>
-      </c>
-      <c r="FS2">
-        <v>107.69</v>
-      </c>
-      <c r="FT2">
-        <v>214.69</v>
-      </c>
-      <c r="FU2">
-        <v>916.61</v>
-      </c>
-      <c r="FV2">
-        <v>43.65</v>
-      </c>
-      <c r="FW2">
-        <v>260.25</v>
-      </c>
-      <c r="FX2">
-        <v>82.38</v>
-      </c>
-      <c r="FY2">
-        <v>106.79</v>
-      </c>
-      <c r="FZ2">
-        <v>133.48</v>
-      </c>
-      <c r="GA2">
-        <v>142.05</v>
-      </c>
-      <c r="GB2">
-        <v>120.81</v>
-      </c>
-      <c r="GC2">
-        <v>68.27</v>
-      </c>
-      <c r="GD2">
-        <v>56.29</v>
-      </c>
-      <c r="GE2">
-        <v>53.51</v>
-      </c>
-      <c r="GF2">
-        <v>151.85</v>
-      </c>
-      <c r="GG2">
-        <v>260.96</v>
-      </c>
-      <c r="GH2">
-        <v>30.33</v>
-      </c>
-      <c r="GI2">
-        <v>95.59</v>
-      </c>
-      <c r="GJ2">
-        <v>71.06</v>
-      </c>
-      <c r="GK2">
-        <v>49.83</v>
-      </c>
-      <c r="GL2">
-        <v>326.15</v>
-      </c>
-      <c r="GM2">
-        <v>492.71</v>
-      </c>
-      <c r="GN2">
-        <v>227.81</v>
-      </c>
-      <c r="GO2">
-        <v>127.62</v>
-      </c>
-      <c r="GP2">
-        <v>118.41</v>
-      </c>
-      <c r="GQ2">
-        <v>103.05</v>
-      </c>
-      <c r="GR2">
-        <v>44.86</v>
-      </c>
-      <c r="GS2">
-        <v>126.52</v>
-      </c>
-      <c r="GT2">
-        <v>66.39</v>
-      </c>
-      <c r="GU2">
-        <v>37.65</v>
-      </c>
-      <c r="GV2">
-        <v>22.35</v>
-      </c>
-      <c r="GW2">
-        <v>73.26000000000001</v>
-      </c>
-      <c r="GX2">
-        <v>59.99</v>
-      </c>
-      <c r="GY2">
-        <v>175</v>
-      </c>
-      <c r="GZ2">
-        <v>44.77</v>
-      </c>
-      <c r="HA2">
-        <v>204.12</v>
-      </c>
-      <c r="HB2">
-        <v>237.86</v>
-      </c>
-      <c r="HC2">
-        <v>231.47</v>
-      </c>
-      <c r="HD2">
-        <v>126.67</v>
-      </c>
-      <c r="HE2">
-        <v>655.25</v>
-      </c>
-      <c r="HF2">
-        <v>129.82</v>
-      </c>
-      <c r="HG2">
-        <v>344.06</v>
-      </c>
-      <c r="HH2">
-        <v>76.2</v>
-      </c>
-      <c r="HI2">
-        <v>334.55</v>
-      </c>
-      <c r="HJ2">
-        <v>83.88</v>
-      </c>
-      <c r="HK2">
-        <v>25.94</v>
-      </c>
-      <c r="HL2">
-        <v>155.71</v>
-      </c>
-      <c r="HM2">
-        <v>110.29</v>
-      </c>
-      <c r="HN2">
-        <v>81.61</v>
-      </c>
-      <c r="HO2">
-        <v>236.68</v>
-      </c>
-      <c r="HP2">
-        <v>81.8</v>
-      </c>
-      <c r="HQ2">
-        <v>144.82</v>
-      </c>
-      <c r="HR2">
-        <v>608.0700000000001</v>
-      </c>
-      <c r="HS2">
-        <v>35.75</v>
-      </c>
-      <c r="HT2">
-        <v>69.12</v>
-      </c>
-      <c r="HU2">
-        <v>242.4</v>
-      </c>
-      <c r="HV2">
-        <v>589.16</v>
-      </c>
-      <c r="HW2">
-        <v>227.33</v>
-      </c>
-      <c r="HX2">
-        <v>53.13</v>
-      </c>
-      <c r="HY2">
-        <v>958</v>
-      </c>
-      <c r="HZ2">
-        <v>42.1</v>
-      </c>
-      <c r="IA2">
-        <v>13.4</v>
-      </c>
-      <c r="IB2">
-        <v>329.24</v>
-      </c>
-      <c r="IC2">
-        <v>57.97</v>
-      </c>
-      <c r="ID2">
-        <v>79.06</v>
-      </c>
-      <c r="IE2">
-        <v>120.13</v>
-      </c>
-      <c r="IF2">
-        <v>73.98</v>
-      </c>
-      <c r="IG2">
-        <v>154.01</v>
-      </c>
-      <c r="IH2">
-        <v>193.08</v>
-      </c>
-      <c r="II2">
-        <v>91.16</v>
-      </c>
-      <c r="IJ2">
-        <v>297.23</v>
-      </c>
-      <c r="IK2">
-        <v>261.99</v>
-      </c>
-      <c r="IL2">
-        <v>23.62</v>
-      </c>
-      <c r="IM2">
-        <v>41.9</v>
-      </c>
-      <c r="IN2">
-        <v>118.06</v>
-      </c>
-      <c r="IO2">
-        <v>453.59</v>
-      </c>
-      <c r="IP2">
-        <v>62.45</v>
-      </c>
-      <c r="IQ2">
-        <v>184.59</v>
-      </c>
-      <c r="IR2">
-        <v>232.91</v>
-      </c>
-      <c r="IS2">
-        <v>217.33</v>
-      </c>
-      <c r="IT2">
-        <v>36.74</v>
-      </c>
-      <c r="IU2">
-        <v>28.91</v>
-      </c>
-      <c r="IV2">
-        <v>354.13</v>
-      </c>
-      <c r="IW2">
-        <v>170.49</v>
-      </c>
-      <c r="IX2">
-        <v>499.02</v>
-      </c>
-      <c r="IY2">
-        <v>43.88</v>
-      </c>
-      <c r="IZ2">
-        <v>194.5</v>
-      </c>
-      <c r="JA2">
-        <v>164.49</v>
-      </c>
-      <c r="JB2">
-        <v>718.29</v>
-      </c>
-      <c r="JC2">
-        <v>105.86</v>
-      </c>
-      <c r="JD2">
-        <v>31.98</v>
-      </c>
-      <c r="JE2">
-        <v>133.23</v>
-      </c>
-      <c r="JF2">
-        <v>302.82</v>
-      </c>
-      <c r="JG2">
-        <v>233.93</v>
-      </c>
-      <c r="JH2">
-        <v>85.11</v>
-      </c>
-      <c r="JI2">
-        <v>214.91</v>
-      </c>
-      <c r="JJ2">
-        <v>60.03</v>
-      </c>
-      <c r="JK2">
-        <v>57.17</v>
-      </c>
-      <c r="JL2">
-        <v>64.13</v>
-      </c>
-      <c r="JM2">
-        <v>43.63</v>
-      </c>
-      <c r="JN2">
-        <v>120.46</v>
-      </c>
-      <c r="JO2">
-        <v>210.42</v>
-      </c>
-      <c r="JP2">
-        <v>28.56</v>
-      </c>
-      <c r="JQ2">
-        <v>94.79000000000001</v>
-      </c>
-      <c r="JR2">
-        <v>88.28</v>
-      </c>
-      <c r="JS2">
-        <v>147.99</v>
-      </c>
-      <c r="JT2">
-        <v>101.17</v>
-      </c>
-      <c r="JU2">
-        <v>26.05</v>
-      </c>
-      <c r="JV2">
-        <v>155.39</v>
-      </c>
-      <c r="JW2">
-        <v>67.38</v>
-      </c>
-      <c r="JX2">
-        <v>29.48</v>
-      </c>
-      <c r="JY2">
-        <v>215.89</v>
-      </c>
-      <c r="JZ2">
-        <v>168.46</v>
-      </c>
-      <c r="KA2">
-        <v>82.42</v>
-      </c>
-      <c r="KB2">
-        <v>65.41</v>
-      </c>
-      <c r="KC2">
-        <v>329.14</v>
-      </c>
-      <c r="KD2">
-        <v>179.72</v>
-      </c>
-      <c r="KE2">
-        <v>40.65</v>
-      </c>
-      <c r="KF2">
-        <v>263.58</v>
-      </c>
-      <c r="KG2">
-        <v>60.89</v>
-      </c>
-      <c r="KH2">
-        <v>430.59</v>
-      </c>
-      <c r="KI2">
-        <v>79.25</v>
-      </c>
-      <c r="KJ2">
-        <v>99.08</v>
-      </c>
-      <c r="KK2">
-        <v>279.42</v>
-      </c>
-      <c r="KL2">
-        <v>173.48</v>
-      </c>
-      <c r="KM2">
-        <v>360.58</v>
-      </c>
-      <c r="KN2">
-        <v>152.99</v>
-      </c>
-      <c r="KO2">
-        <v>20.23</v>
-      </c>
-      <c r="KP2">
-        <v>35.49</v>
-      </c>
-      <c r="KQ2">
-        <v>64.92</v>
-      </c>
-      <c r="KR2">
-        <v>146.63</v>
-      </c>
-      <c r="KS2">
-        <v>38.99</v>
-      </c>
-      <c r="KT2">
-        <v>35.75</v>
-      </c>
-      <c r="KU2">
-        <v>290.66</v>
-      </c>
-      <c r="KV2">
-        <v>327.06</v>
-      </c>
-      <c r="KW2">
-        <v>174</v>
-      </c>
-      <c r="KX2">
-        <v>124.94</v>
-      </c>
-      <c r="KY2">
-        <v>87.81</v>
-      </c>
-      <c r="KZ2">
-        <v>174.17</v>
-      </c>
-      <c r="LA2">
-        <v>117.61</v>
-      </c>
-      <c r="LB2">
-        <v>111.63</v>
-      </c>
-      <c r="LC2">
-        <v>42.18</v>
-      </c>
-      <c r="LD2">
-        <v>32.63</v>
-      </c>
-      <c r="LE2">
-        <v>99.52</v>
-      </c>
-      <c r="LF2">
-        <v>210.1</v>
-      </c>
-      <c r="LG2">
-        <v>28.34</v>
-      </c>
-      <c r="LH2">
-        <v>187.9</v>
-      </c>
-      <c r="LI2">
-        <v>20.63</v>
-      </c>
-      <c r="LJ2">
-        <v>53.64</v>
-      </c>
-      <c r="LK2">
-        <v>94.26000000000001</v>
-      </c>
-      <c r="LL2">
-        <v>25.83</v>
-      </c>
-      <c r="LM2">
-        <v>38.71</v>
-      </c>
-      <c r="LN2">
-        <v>47.01</v>
-      </c>
-      <c r="LO2">
-        <v>115.34</v>
-      </c>
-      <c r="LP2">
-        <v>63.86</v>
-      </c>
-      <c r="LQ2">
-        <v>60.59</v>
-      </c>
-      <c r="LR2">
-        <v>123.08</v>
-      </c>
-      <c r="LS2">
-        <v>52.82</v>
-      </c>
-      <c r="LT2">
-        <v>87.22</v>
-      </c>
-      <c r="LU2">
-        <v>317.17</v>
-      </c>
-      <c r="LV2">
-        <v>34.81</v>
-      </c>
-      <c r="LW2">
-        <v>19.68</v>
-      </c>
-      <c r="LX2">
-        <v>181.55</v>
-      </c>
-      <c r="LY2">
-        <v>92.73999999999999</v>
-      </c>
-      <c r="LZ2">
-        <v>28.69</v>
-      </c>
-      <c r="MA2">
-        <v>16.83</v>
-      </c>
-      <c r="MB2">
-        <v>73.40000000000001</v>
-      </c>
-      <c r="MC2">
-        <v>84.09</v>
-      </c>
-      <c r="MD2">
-        <v>390.98</v>
-      </c>
-      <c r="ME2">
-        <v>122.49</v>
-      </c>
-      <c r="MF2">
-        <v>30.93</v>
-      </c>
-      <c r="MG2">
-        <v>64.91</v>
-      </c>
-      <c r="MH2">
-        <v>24.55</v>
-      </c>
-      <c r="MI2">
-        <v>421.59</v>
-      </c>
-      <c r="MJ2">
-        <v>46.86</v>
-      </c>
-      <c r="MK2">
-        <v>551.34</v>
-      </c>
-      <c r="ML2">
-        <v>15.59</v>
-      </c>
-      <c r="MM2">
-        <v>75.15000000000001</v>
-      </c>
-      <c r="MN2">
-        <v>602.11</v>
-      </c>
-      <c r="MO2">
-        <v>70.63</v>
-      </c>
-      <c r="MP2">
-        <v>82.23</v>
-      </c>
-      <c r="MQ2">
-        <v>40.68</v>
-      </c>
-      <c r="MR2">
-        <v>23.8</v>
-      </c>
-      <c r="MS2">
-        <v>15.6</v>
-      </c>
-      <c r="MT2">
-        <v>28.61</v>
-      </c>
-      <c r="MU2">
-        <v>264.41</v>
-      </c>
-      <c r="MV2">
-        <v>29.06</v>
-      </c>
-      <c r="MW2">
-        <v>325.71</v>
-      </c>
-      <c r="MX2">
-        <v>194.26</v>
-      </c>
-      <c r="MY2">
-        <v>115.94</v>
-      </c>
-      <c r="MZ2">
-        <v>531.99</v>
-      </c>
-      <c r="NA2">
-        <v>15.8</v>
-      </c>
-      <c r="NB2">
-        <v>198.51</v>
-      </c>
-      <c r="NC2">
-        <v>22.22</v>
-      </c>
-      <c r="ND2">
-        <v>214</v>
-      </c>
-      <c r="NE2">
-        <v>214.47</v>
-      </c>
-      <c r="NF2">
-        <v>82.16</v>
-      </c>
-      <c r="NG2">
-        <v>44.58</v>
-      </c>
-      <c r="NH2">
-        <v>13.05</v>
-      </c>
-      <c r="NI2">
-        <v>12.23</v>
-      </c>
-      <c r="NJ2">
-        <v>95.29000000000001</v>
-      </c>
-      <c r="NK2">
-        <v>129.19</v>
-      </c>
-      <c r="NL2">
-        <v>346.35</v>
-      </c>
-      <c r="NM2">
-        <v>57.72</v>
-      </c>
-      <c r="NN2">
-        <v>46.78</v>
-      </c>
-      <c r="NO2">
-        <v>107.23</v>
-      </c>
-      <c r="NP2">
-        <v>51.56</v>
-      </c>
-      <c r="NQ2">
-        <v>48.88</v>
-      </c>
-      <c r="NR2">
-        <v>59.23</v>
-      </c>
-      <c r="NS2">
-        <v>40.88</v>
-      </c>
-      <c r="NT2">
-        <v>70.91</v>
-      </c>
-      <c r="NU2">
-        <v>165.17</v>
-      </c>
-      <c r="NV2">
-        <v>29.82</v>
-      </c>
-      <c r="NW2">
-        <v>38.04</v>
-      </c>
-      <c r="NX2">
-        <v>35.81</v>
-      </c>
-      <c r="NY2">
-        <v>449.6</v>
-      </c>
-      <c r="NZ2">
-        <v>39.41</v>
-      </c>
-      <c r="OA2">
-        <v>83.02</v>
-      </c>
-      <c r="OB2">
-        <v>224.74</v>
-      </c>
-      <c r="OC2">
-        <v>88.91</v>
-      </c>
-      <c r="OD2">
-        <v>144.47</v>
-      </c>
-      <c r="OE2">
-        <v>67.51000000000001</v>
-      </c>
-      <c r="OF2">
-        <v>71.43000000000001</v>
-      </c>
-      <c r="OG2">
-        <v>21.54</v>
-      </c>
-      <c r="OH2">
-        <v>41.37</v>
-      </c>
-      <c r="OI2">
-        <v>47.55</v>
-      </c>
-      <c r="OJ2">
-        <v>174.01</v>
-      </c>
-      <c r="OK2">
-        <v>38.77</v>
-      </c>
-      <c r="OL2">
-        <v>30.83</v>
-      </c>
-      <c r="OM2">
-        <v>25.26</v>
-      </c>
-      <c r="ON2">
-        <v>24.8</v>
-      </c>
-      <c r="OO2">
-        <v>26.23</v>
-      </c>
-      <c r="OP2">
-        <v>54.65</v>
-      </c>
-      <c r="OQ2">
-        <v>207.13</v>
-      </c>
-      <c r="OR2">
-        <v>136.91</v>
-      </c>
-      <c r="OS2">
-        <v>43.67</v>
-      </c>
-      <c r="OT2">
-        <v>44.95</v>
-      </c>
-      <c r="OU2">
-        <v>74.55</v>
-      </c>
-      <c r="OV2">
-        <v>87.72</v>
-      </c>
-      <c r="OW2">
-        <v>28.04</v>
-      </c>
-      <c r="OX2">
-        <v>55.58</v>
-      </c>
-      <c r="OY2">
-        <v>354.6</v>
-      </c>
-      <c r="OZ2">
-        <v>213.98</v>
-      </c>
-      <c r="PA2">
-        <v>127.64</v>
-      </c>
-      <c r="PB2">
-        <v>100.73</v>
-      </c>
-      <c r="PC2">
-        <v>150.24</v>
-      </c>
-      <c r="PD2">
-        <v>510.75</v>
-      </c>
-      <c r="PE2">
-        <v>65.09</v>
-      </c>
-      <c r="PF2">
-        <v>172.82</v>
-      </c>
-      <c r="PG2">
-        <v>71.09</v>
-      </c>
-      <c r="PH2">
-        <v>128.91</v>
-      </c>
-      <c r="PI2">
-        <v>112.51</v>
-      </c>
-      <c r="PJ2">
-        <v>62.2</v>
-      </c>
-      <c r="PK2">
-        <v>824.76</v>
-      </c>
-      <c r="PL2">
-        <v>25.23</v>
-      </c>
-      <c r="PM2">
-        <v>99.17</v>
-      </c>
-      <c r="PN2">
-        <v>10.87</v>
-      </c>
-      <c r="PO2">
-        <v>145.06</v>
-      </c>
-      <c r="PP2">
-        <v>21.59</v>
-      </c>
-      <c r="PQ2">
-        <v>291.09</v>
-      </c>
-      <c r="PR2">
-        <v>23.57</v>
-      </c>
-      <c r="PS2">
-        <v>18.21</v>
-      </c>
-      <c r="PT2">
-        <v>36.46</v>
-      </c>
-      <c r="PU2">
-        <v>235.08</v>
-      </c>
-      <c r="PV2">
-        <v>42.08</v>
-      </c>
-      <c r="PW2">
-        <v>48.23</v>
-      </c>
-      <c r="PX2">
-        <v>102.09</v>
-      </c>
-      <c r="PY2">
-        <v>170.63</v>
-      </c>
-      <c r="PZ2">
-        <v>41.43</v>
-      </c>
-      <c r="QA2">
-        <v>75.2</v>
-      </c>
-      <c r="QB2">
-        <v>12.83</v>
-      </c>
-      <c r="QC2">
-        <v>127.37</v>
-      </c>
-      <c r="QD2">
-        <v>159.52</v>
-      </c>
-      <c r="QE2">
-        <v>35.55</v>
-      </c>
-      <c r="QF2">
-        <v>19.82</v>
-      </c>
-      <c r="QG2">
-        <v>127.06</v>
-      </c>
-      <c r="QH2">
-        <v>41.44</v>
-      </c>
-      <c r="QI2">
+      <c r="UB2">
+        <v>165.22</v>
+      </c>
+      <c r="UC2">
+        <v>39.23</v>
+      </c>
+      <c r="UD2">
+        <v>16.12</v>
+      </c>
+      <c r="UE2">
+        <v>197.22</v>
+      </c>
+      <c r="UF2">
+        <v>33.87</v>
+      </c>
+      <c r="UG2">
+        <v>325.31</v>
+      </c>
+      <c r="UH2">
+        <v>30.5</v>
+      </c>
+      <c r="UI2">
+        <v>82.34999999999999</v>
+      </c>
+      <c r="UJ2">
+        <v>125.17</v>
+      </c>
+      <c r="UK2">
+        <v>69.81</v>
+      </c>
+      <c r="UL2">
+        <v>11.13</v>
+      </c>
+      <c r="UM2">
+        <v>23.15</v>
+      </c>
+      <c r="UN2">
         <v>22.37</v>
       </c>
-      <c r="QJ2">
-        <v>61.15</v>
-      </c>
-      <c r="QK2">
-        <v>27.07</v>
-      </c>
-      <c r="QL2">
-        <v>83.34999999999999</v>
-      </c>
-      <c r="QM2">
-        <v>96.97</v>
-      </c>
-      <c r="QN2">
-        <v>24.32</v>
-      </c>
-      <c r="QO2">
-        <v>15.93</v>
-      </c>
-      <c r="QP2">
-        <v>532.9299999999999</v>
-      </c>
-      <c r="QQ2">
-        <v>117.96</v>
-      </c>
-      <c r="QR2">
-        <v>89.17</v>
-      </c>
-      <c r="QS2">
-        <v>40.38</v>
-      </c>
-      <c r="QT2">
-        <v>114.44</v>
-      </c>
-      <c r="QU2">
-        <v>109.94</v>
-      </c>
-      <c r="QV2">
-        <v>52.06</v>
-      </c>
-      <c r="QW2">
-        <v>41.44</v>
-      </c>
-      <c r="QX2">
-        <v>78.31</v>
-      </c>
-      <c r="QY2">
-        <v>31</v>
-      </c>
-      <c r="QZ2">
-        <v>22.46</v>
-      </c>
-      <c r="RA2">
-        <v>178.04</v>
-      </c>
-      <c r="RB2">
-        <v>44.7</v>
-      </c>
-      <c r="RC2">
-        <v>74.54000000000001</v>
-      </c>
-      <c r="RD2">
-        <v>93.28</v>
-      </c>
-      <c r="RE2">
-        <v>50.55</v>
-      </c>
-      <c r="RF2">
-        <v>56.93</v>
-      </c>
-      <c r="RG2">
-        <v>565.97</v>
-      </c>
-      <c r="RH2">
-        <v>17.11</v>
-      </c>
-      <c r="RI2">
-        <v>16.8</v>
-      </c>
-      <c r="RJ2">
+      <c r="UO2">
+        <v>939.8099999999999</v>
+      </c>
+      <c r="UP2">
+        <v>130.98</v>
+      </c>
+      <c r="UQ2">
+        <v>49.9</v>
+      </c>
+      <c r="UR2">
+        <v>15.58</v>
+      </c>
+      <c r="US2">
+        <v>210.19</v>
+      </c>
+      <c r="UT2">
+        <v>152.12</v>
+      </c>
+      <c r="UU2">
+        <v>178.25</v>
+      </c>
+      <c r="UV2">
+        <v>175.51</v>
+      </c>
+      <c r="UW2">
+        <v>17.82</v>
+      </c>
+      <c r="UX2">
+        <v>332.71</v>
+      </c>
+      <c r="UY2">
+        <v>156.75</v>
+      </c>
+      <c r="UZ2">
         <v>27.83</v>
       </c>
-      <c r="RK2">
-        <v>114.91</v>
-      </c>
-      <c r="RL2">
-        <v>90.2</v>
-      </c>
-      <c r="RM2">
-        <v>857.25</v>
-      </c>
-      <c r="RN2">
-        <v>42.12</v>
-      </c>
-      <c r="RO2">
-        <v>82.17</v>
-      </c>
-      <c r="RP2">
-        <v>197.81</v>
-      </c>
-      <c r="RQ2">
-        <v>212.6</v>
-      </c>
-      <c r="RR2">
-        <v>46.4</v>
-      </c>
-      <c r="RS2">
-        <v>28.81</v>
-      </c>
-      <c r="RT2">
-        <v>56.65</v>
-      </c>
-      <c r="RU2">
-        <v>83.13</v>
-      </c>
-      <c r="RV2">
-        <v>85.45</v>
-      </c>
-      <c r="RW2">
-        <v>29.14</v>
-      </c>
-      <c r="RX2">
-        <v>29.44</v>
-      </c>
-      <c r="RY2">
-        <v>102.91</v>
-      </c>
-      <c r="RZ2">
-        <v>70.58</v>
-      </c>
-      <c r="SA2">
-        <v>28.58</v>
-      </c>
-      <c r="SB2">
-        <v>39.65</v>
-      </c>
-      <c r="SC2">
-        <v>188.09</v>
-      </c>
-      <c r="SD2">
-        <v>56.4</v>
-      </c>
-      <c r="SE2">
-        <v>154.08</v>
-      </c>
-      <c r="SF2">
-        <v>28.89</v>
-      </c>
-      <c r="SG2">
-        <v>212.69</v>
-      </c>
-      <c r="SH2">
-        <v>42.64</v>
-      </c>
-      <c r="SI2">
-        <v>26.01</v>
-      </c>
-      <c r="SJ2">
-        <v>30.09</v>
-      </c>
-      <c r="SK2">
-        <v>59.9</v>
-      </c>
-      <c r="SL2">
-        <v>24.51</v>
-      </c>
-      <c r="SM2">
-        <v>183.61</v>
-      </c>
-      <c r="SN2">
-        <v>28.22</v>
-      </c>
-      <c r="SO2">
-        <v>23.7</v>
-      </c>
-      <c r="SP2">
-        <v>168.55</v>
-      </c>
-      <c r="SQ2">
-        <v>79.84999999999999</v>
-      </c>
-      <c r="SR2">
-        <v>83.64</v>
-      </c>
-      <c r="SS2">
-        <v>11.54</v>
-      </c>
-      <c r="ST2">
-        <v>161.22</v>
-      </c>
-      <c r="SU2">
-        <v>69.15000000000001</v>
-      </c>
-      <c r="SV2">
-        <v>56.51</v>
-      </c>
-      <c r="SW2">
-        <v>52.13</v>
-      </c>
-      <c r="SX2">
-        <v>18.69</v>
-      </c>
-      <c r="SY2">
-        <v>112.72</v>
-      </c>
-      <c r="SZ2">
-        <v>488.73</v>
-      </c>
-      <c r="TA2">
-        <v>112.26</v>
-      </c>
-      <c r="TB2">
-        <v>89.69</v>
-      </c>
-      <c r="TC2">
-        <v>100</v>
-      </c>
-      <c r="TD2">
-        <v>98.02</v>
-      </c>
-      <c r="TE2">
-        <v>32.14</v>
-      </c>
-      <c r="TF2">
-        <v>39.66</v>
-      </c>
-      <c r="TG2">
-        <v>53.6</v>
-      </c>
-      <c r="TH2">
-        <v>38.9</v>
-      </c>
-      <c r="TI2">
-        <v>37.26</v>
-      </c>
-      <c r="TJ2">
-        <v>238.07</v>
-      </c>
-      <c r="TK2">
-        <v>21.82</v>
-      </c>
-      <c r="TL2">
-        <v>83.25</v>
-      </c>
-      <c r="TM2">
-        <v>29.8</v>
-      </c>
-      <c r="TN2">
-        <v>30.82</v>
-      </c>
-      <c r="TO2">
-        <v>29.83</v>
-      </c>
-      <c r="TP2">
-        <v>456.7</v>
-      </c>
-      <c r="TQ2">
-        <v>16.06</v>
-      </c>
-      <c r="TR2">
-        <v>64.25</v>
-      </c>
-      <c r="TS2">
-        <v>174.67</v>
-      </c>
-      <c r="TT2">
-        <v>45.84</v>
-      </c>
-      <c r="TU2">
-        <v>71.34</v>
-      </c>
-      <c r="TV2">
-        <v>28.16</v>
-      </c>
-      <c r="TW2">
-        <v>156.51</v>
-      </c>
-      <c r="TX2">
-        <v>99.36</v>
-      </c>
-      <c r="TY2">
-        <v>49.34</v>
-      </c>
-      <c r="TZ2">
-        <v>166.12</v>
-      </c>
-      <c r="UA2">
+      <c r="VA2">
+        <v>590.98</v>
+      </c>
+      <c r="VB2">
+        <v>85.81999999999999</v>
+      </c>
+      <c r="VC2">
+        <v>34.76</v>
+      </c>
+      <c r="VD2">
+        <v>16.28</v>
+      </c>
+      <c r="VE2">
+        <v>39.45</v>
+      </c>
+      <c r="VF2">
+        <v>35.05</v>
+      </c>
+      <c r="VG2">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="VH2">
+        <v>30.88</v>
+      </c>
+      <c r="VI2">
+        <v>65.62</v>
+      </c>
+      <c r="VJ2">
+        <v>42.75</v>
+      </c>
+      <c r="VK2">
+        <v>150.64</v>
+      </c>
+      <c r="VL2">
+        <v>268.22</v>
+      </c>
+      <c r="VM2">
+        <v>19.69</v>
+      </c>
+      <c r="VN2">
+        <v>153.83</v>
+      </c>
+      <c r="VO2">
+        <v>98.27</v>
+      </c>
+      <c r="VP2">
+        <v>36.15</v>
+      </c>
+      <c r="VQ2">
+        <v>63.61</v>
+      </c>
+      <c r="VR2">
+        <v>102.72</v>
+      </c>
+      <c r="VS2">
+        <v>48.69</v>
+      </c>
+      <c r="VT2">
+        <v>38.22</v>
+      </c>
+      <c r="VU2">
+        <v>31.53</v>
+      </c>
+      <c r="VV2">
+        <v>141.06</v>
+      </c>
+      <c r="VW2">
+        <v>92.72</v>
+      </c>
+      <c r="VX2">
+        <v>215.46</v>
+      </c>
+      <c r="VY2">
+        <v>42.01</v>
+      </c>
+      <c r="VZ2">
+        <v>70.84999999999999</v>
+      </c>
+      <c r="WA2">
+        <v>59.6</v>
+      </c>
+      <c r="WB2">
+        <v>57.65</v>
+      </c>
+      <c r="WC2">
+        <v>38.96</v>
+      </c>
+      <c r="WD2">
+        <v>48.42</v>
+      </c>
+      <c r="WE2">
+        <v>517.72</v>
+      </c>
+      <c r="WF2">
+        <v>52.48</v>
+      </c>
+      <c r="WG2">
+        <v>14.85</v>
+      </c>
+      <c r="WH2">
+        <v>27.93</v>
+      </c>
+      <c r="WI2">
+        <v>99.45999999999999</v>
+      </c>
+      <c r="WJ2">
+        <v>50.42</v>
+      </c>
+      <c r="WK2">
+        <v>34.68</v>
+      </c>
+      <c r="WL2">
+        <v>88.77</v>
+      </c>
+      <c r="WM2">
+        <v>34.19</v>
+      </c>
+      <c r="WN2">
+        <v>121.25</v>
+      </c>
+      <c r="WO2">
+        <v>41.46</v>
+      </c>
+      <c r="WP2">
+        <v>292.79</v>
+      </c>
+      <c r="WQ2">
+        <v>18.7</v>
+      </c>
+      <c r="WR2">
+        <v>35.76</v>
+      </c>
+      <c r="WS2">
+        <v>200.64</v>
+      </c>
+      <c r="WT2">
+        <v>67.89</v>
+      </c>
+      <c r="WU2">
+        <v>23.55</v>
+      </c>
+      <c r="WV2">
+        <v>36.55</v>
+      </c>
+      <c r="WW2">
+        <v>19.24</v>
+      </c>
+      <c r="WX2">
+        <v>45.14</v>
+      </c>
+      <c r="WY2">
+        <v>87.42</v>
+      </c>
+      <c r="WZ2">
+        <v>27.57</v>
+      </c>
+      <c r="XA2">
+        <v>13.85</v>
+      </c>
+      <c r="XB2">
+        <v>52.55</v>
+      </c>
+      <c r="XC2">
+        <v>65.78</v>
+      </c>
+      <c r="XD2">
+        <v>18.86</v>
+      </c>
+      <c r="XE2">
+        <v>31.73</v>
+      </c>
+      <c r="XF2">
+        <v>47.22</v>
+      </c>
+      <c r="XG2">
+        <v>158.5</v>
+      </c>
+      <c r="XH2">
+        <v>130.58</v>
+      </c>
+      <c r="XI2">
+        <v>56.45</v>
+      </c>
+      <c r="XJ2">
+        <v>285.16</v>
+      </c>
+      <c r="XK2">
+        <v>58.64</v>
+      </c>
+      <c r="XL2">
+        <v>24.45</v>
+      </c>
+      <c r="XM2">
+        <v>133.83</v>
+      </c>
+      <c r="XN2">
+        <v>28.05</v>
+      </c>
+      <c r="XO2">
+        <v>42.66</v>
+      </c>
+      <c r="XP2">
+        <v>199.93</v>
+      </c>
+      <c r="XQ2">
+        <v>16.21</v>
+      </c>
+      <c r="XR2">
+        <v>14.56</v>
+      </c>
+      <c r="XS2">
+        <v>18.32</v>
+      </c>
+      <c r="XT2">
+        <v>32.02</v>
+      </c>
+      <c r="XU2">
+        <v>32.58</v>
+      </c>
+      <c r="XV2">
+        <v>33.7</v>
+      </c>
+      <c r="XW2">
+        <v>127.73</v>
+      </c>
+      <c r="XX2">
+        <v>55.59</v>
+      </c>
+      <c r="XY2">
+        <v>395.14</v>
+      </c>
+      <c r="XZ2">
+        <v>19.58</v>
+      </c>
+      <c r="YA2">
+        <v>29.9</v>
+      </c>
+      <c r="YB2">
+        <v>23.55</v>
+      </c>
+      <c r="YC2">
+        <v>45.92</v>
+      </c>
+      <c r="YD2">
+        <v>96.64</v>
+      </c>
+      <c r="YE2">
+        <v>9.44</v>
+      </c>
+      <c r="YF2">
+        <v>147.71</v>
+      </c>
+      <c r="YG2">
+        <v>75.47</v>
+      </c>
+      <c r="YH2">
+        <v>441.1</v>
+      </c>
+      <c r="YI2">
+        <v>77.44</v>
+      </c>
+      <c r="YJ2">
+        <v>22.37</v>
+      </c>
+      <c r="YK2">
+        <v>174.52</v>
+      </c>
+      <c r="YL2">
+        <v>49.7</v>
+      </c>
+      <c r="YM2">
+        <v>29.65</v>
+      </c>
+      <c r="YN2">
+        <v>221.64</v>
+      </c>
+      <c r="YO2">
+        <v>8.17</v>
+      </c>
+      <c r="YP2">
+        <v>7.74</v>
+      </c>
+      <c r="YQ2">
+        <v>53.4</v>
+      </c>
+      <c r="YR2">
+        <v>66.17</v>
+      </c>
+      <c r="YS2">
+        <v>25.68</v>
+      </c>
+      <c r="YT2">
+        <v>63.7</v>
+      </c>
+      <c r="YU2">
+        <v>22.09</v>
+      </c>
+      <c r="YV2">
+        <v>61.72</v>
+      </c>
+      <c r="YW2">
+        <v>22.2</v>
+      </c>
+      <c r="YX2">
+        <v>46.59</v>
+      </c>
+      <c r="YY2">
+        <v>106.15</v>
+      </c>
+      <c r="YZ2">
+        <v>76.42</v>
+      </c>
+      <c r="ZA2">
+        <v>50.13</v>
+      </c>
+      <c r="ZB2">
+        <v>63.78</v>
+      </c>
+      <c r="ZC2">
+        <v>116.5</v>
+      </c>
+      <c r="ZD2">
+        <v>60.12</v>
+      </c>
+      <c r="ZE2">
+        <v>85.08</v>
+      </c>
+      <c r="ZF2">
+        <v>17</v>
+      </c>
+      <c r="ZG2">
+        <v>84.43000000000001</v>
+      </c>
+      <c r="ZH2">
+        <v>9.74</v>
+      </c>
+      <c r="ZI2">
+        <v>116.12</v>
+      </c>
+      <c r="ZJ2">
+        <v>14.21</v>
+      </c>
+      <c r="ZK2">
+        <v>33.55</v>
+      </c>
+      <c r="ZL2">
+        <v>27.2</v>
+      </c>
+      <c r="ZM2">
         <v>39.36</v>
       </c>
-      <c r="UB2">
-        <v>16.79</v>
-      </c>
-      <c r="UC2">
-        <v>205.46</v>
-      </c>
-      <c r="UD2">
-        <v>33.81</v>
-      </c>
-      <c r="UE2">
-        <v>328.89</v>
-      </c>
-      <c r="UF2">
-        <v>30.92</v>
-      </c>
-      <c r="UG2">
-        <v>82.09</v>
-      </c>
-      <c r="UH2">
-        <v>123.58</v>
-      </c>
-      <c r="UI2">
-        <v>70.06</v>
-      </c>
-      <c r="UJ2">
-        <v>11.17</v>
-      </c>
-      <c r="UK2">
-        <v>24.01</v>
-      </c>
-      <c r="UL2">
-        <v>22.56</v>
-      </c>
-      <c r="UM2">
-        <v>938.85</v>
-      </c>
-      <c r="UN2">
-        <v>132.04</v>
-      </c>
-      <c r="UO2">
-        <v>50.37</v>
-      </c>
-      <c r="UP2">
-        <v>15.92</v>
-      </c>
-      <c r="UQ2">
-        <v>212.44</v>
-      </c>
-      <c r="UR2">
-        <v>155.46</v>
-      </c>
-      <c r="US2">
-        <v>175.42</v>
-      </c>
-      <c r="UT2">
-        <v>176.38</v>
-      </c>
-      <c r="UU2">
-        <v>18.4</v>
-      </c>
-      <c r="UV2">
-        <v>328.33</v>
-      </c>
-      <c r="UW2">
-        <v>157.13</v>
-      </c>
-      <c r="UX2">
-        <v>26.53</v>
-      </c>
-      <c r="UY2">
-        <v>640.64</v>
-      </c>
-      <c r="UZ2">
-        <v>87.97</v>
-      </c>
-      <c r="VA2">
-        <v>35.78</v>
-      </c>
-      <c r="VB2">
-        <v>16.7</v>
-      </c>
-      <c r="VC2">
-        <v>39.93</v>
-      </c>
-      <c r="VD2">
-        <v>34.77</v>
-      </c>
-      <c r="VE2">
-        <v>88.79000000000001</v>
-      </c>
-      <c r="VF2">
-        <v>30.41</v>
-      </c>
-      <c r="VG2">
-        <v>65.86</v>
-      </c>
-      <c r="VH2">
-        <v>43.17</v>
-      </c>
-      <c r="VI2">
-        <v>145.15</v>
-      </c>
-      <c r="VJ2">
-        <v>267.4</v>
-      </c>
-      <c r="VK2">
-        <v>19.73</v>
-      </c>
-      <c r="VL2">
-        <v>154.63</v>
-      </c>
-      <c r="VM2">
-        <v>96.87</v>
-      </c>
-      <c r="VN2">
-        <v>35.11</v>
-      </c>
-      <c r="VO2">
-        <v>64.20999999999999</v>
-      </c>
-      <c r="VP2">
-        <v>103.89</v>
-      </c>
-      <c r="VQ2">
-        <v>48.56</v>
-      </c>
-      <c r="VR2">
-        <v>38.28</v>
-      </c>
-      <c r="VS2">
-        <v>32.49</v>
-      </c>
-      <c r="VT2">
-        <v>141.62</v>
-      </c>
-      <c r="VU2">
-        <v>93.58</v>
-      </c>
-      <c r="VV2">
-        <v>214.16</v>
-      </c>
-      <c r="VW2">
-        <v>41.4</v>
-      </c>
-      <c r="VX2">
-        <v>74</v>
-      </c>
-      <c r="VY2">
-        <v>58.39</v>
-      </c>
-      <c r="VZ2">
-        <v>57.94</v>
-      </c>
-      <c r="WA2">
-        <v>41.01</v>
-      </c>
-      <c r="WB2">
-        <v>50.37</v>
-      </c>
-      <c r="WC2">
-        <v>519.5700000000001</v>
-      </c>
-      <c r="WD2">
-        <v>52.15</v>
-      </c>
-      <c r="WE2">
-        <v>14.77</v>
-      </c>
-      <c r="WF2">
-        <v>27.79</v>
-      </c>
-      <c r="WG2">
-        <v>100</v>
-      </c>
-      <c r="WH2">
-        <v>48.59</v>
-      </c>
-      <c r="WI2">
-        <v>34.34</v>
-      </c>
-      <c r="WJ2">
-        <v>89.09999999999999</v>
-      </c>
-      <c r="WK2">
-        <v>33.28</v>
-      </c>
-      <c r="WL2">
-        <v>122.77</v>
-      </c>
-      <c r="WM2">
-        <v>41.09</v>
-      </c>
-      <c r="WN2">
-        <v>292.84</v>
-      </c>
-      <c r="WO2">
-        <v>18.71</v>
-      </c>
-      <c r="WP2">
-        <v>36.85</v>
-      </c>
-      <c r="WQ2">
-        <v>209.83</v>
-      </c>
-      <c r="WR2">
-        <v>67.44</v>
-      </c>
-      <c r="WS2">
-        <v>23.52</v>
-      </c>
-      <c r="WT2">
-        <v>36.55</v>
-      </c>
-      <c r="WU2">
-        <v>18.84</v>
-      </c>
-      <c r="WV2">
-        <v>46.27</v>
-      </c>
-      <c r="WW2">
-        <v>87.17</v>
-      </c>
-      <c r="WX2">
-        <v>27.04</v>
-      </c>
-      <c r="WY2">
-        <v>14.26</v>
-      </c>
-      <c r="WZ2">
-        <v>52.26</v>
-      </c>
-      <c r="XA2">
-        <v>67.44</v>
-      </c>
-      <c r="XB2">
+      <c r="ZN2">
+        <v>100.66</v>
+      </c>
+      <c r="ZO2">
+        <v>112.13</v>
+      </c>
+      <c r="ZP2">
+        <v>14.66</v>
+      </c>
+      <c r="ZQ2">
+        <v>8.73</v>
+      </c>
+      <c r="ZR2">
+        <v>44.42</v>
+      </c>
+      <c r="ZS2">
+        <v>25.6</v>
+      </c>
+      <c r="ZT2">
         <v>18.31</v>
       </c>
-      <c r="XC2">
-        <v>31.88</v>
-      </c>
-      <c r="XD2">
-        <v>46.76</v>
-      </c>
-      <c r="XE2">
-        <v>153.03</v>
-      </c>
-      <c r="XF2">
-        <v>126.29</v>
-      </c>
-      <c r="XG2">
-        <v>57.28</v>
-      </c>
-      <c r="XH2">
-        <v>291.01</v>
-      </c>
-      <c r="XI2">
-        <v>60.94</v>
-      </c>
-      <c r="XJ2">
-        <v>24.63</v>
-      </c>
-      <c r="XK2">
-        <v>138.2</v>
-      </c>
-      <c r="XL2">
-        <v>28.87</v>
-      </c>
-      <c r="XM2">
-        <v>42.49</v>
-      </c>
-      <c r="XN2">
-        <v>187.6</v>
-      </c>
-      <c r="XO2">
-        <v>16.21</v>
-      </c>
-      <c r="XP2">
-        <v>14.49</v>
-      </c>
-      <c r="XQ2">
-        <v>18.57</v>
-      </c>
-      <c r="XR2">
-        <v>31.56</v>
-      </c>
-      <c r="XS2">
-        <v>32.96</v>
-      </c>
-      <c r="XT2">
-        <v>33.02</v>
-      </c>
-      <c r="XU2">
-        <v>128.5</v>
-      </c>
-      <c r="XV2">
-        <v>54.82</v>
-      </c>
-      <c r="XW2">
-        <v>395.09</v>
-      </c>
-      <c r="XX2">
-        <v>19.62</v>
-      </c>
-      <c r="XY2">
-        <v>29.67</v>
-      </c>
-      <c r="XZ2">
-        <v>23.05</v>
-      </c>
-      <c r="YA2">
-        <v>45.7</v>
-      </c>
-      <c r="YB2">
-        <v>97.3</v>
-      </c>
-      <c r="YC2">
-        <v>9.84</v>
-      </c>
-      <c r="YD2">
-        <v>147.11</v>
-      </c>
-      <c r="YE2">
-        <v>77.16</v>
-      </c>
-      <c r="YF2">
-        <v>440.87</v>
-      </c>
-      <c r="YG2">
-        <v>77.08</v>
-      </c>
-      <c r="YH2">
-        <v>22.4</v>
-      </c>
-      <c r="YI2">
-        <v>178.63</v>
-      </c>
-      <c r="YJ2">
-        <v>48.67</v>
-      </c>
-      <c r="YK2">
-        <v>30.28</v>
-      </c>
-      <c r="YL2">
-        <v>220.9</v>
-      </c>
-      <c r="YM2">
-        <v>8.24</v>
-      </c>
-      <c r="YN2">
-        <v>8.25</v>
-      </c>
-      <c r="YO2">
-        <v>52.46</v>
-      </c>
-      <c r="YP2">
-        <v>67.63</v>
-      </c>
-      <c r="YQ2">
-        <v>26.07</v>
-      </c>
-      <c r="YR2">
-        <v>63.31</v>
-      </c>
-      <c r="YS2">
-        <v>22.15</v>
-      </c>
-      <c r="YT2">
-        <v>61.58</v>
-      </c>
-      <c r="YU2">
-        <v>22.15</v>
-      </c>
-      <c r="YV2">
-        <v>46.16</v>
-      </c>
-      <c r="YW2">
-        <v>106.05</v>
-      </c>
-      <c r="YX2">
-        <v>80.02</v>
-      </c>
-      <c r="YY2">
-        <v>51.05</v>
-      </c>
-      <c r="YZ2">
-        <v>64.17</v>
-      </c>
-      <c r="ZA2">
-        <v>115.68</v>
-      </c>
-      <c r="ZB2">
-        <v>60.98</v>
-      </c>
-      <c r="ZC2">
-        <v>84.59999999999999</v>
-      </c>
-      <c r="ZD2">
-        <v>16.77</v>
-      </c>
-      <c r="ZE2">
-        <v>82.05</v>
-      </c>
-      <c r="ZF2">
-        <v>9.69</v>
-      </c>
-      <c r="ZG2">
-        <v>114.52</v>
-      </c>
-      <c r="ZH2">
-        <v>15.2</v>
-      </c>
-      <c r="ZI2">
-        <v>33.84</v>
-      </c>
-      <c r="ZJ2">
-        <v>27.34</v>
-      </c>
-      <c r="ZK2">
-        <v>38.77</v>
-      </c>
-      <c r="ZL2">
-        <v>96.13</v>
-      </c>
-      <c r="ZM2">
-        <v>112.22</v>
-      </c>
-      <c r="ZN2">
-        <v>13.12</v>
-      </c>
-      <c r="ZO2">
-        <v>9.17</v>
-      </c>
-      <c r="ZP2">
-        <v>47.01</v>
-      </c>
-      <c r="ZQ2">
-        <v>25.95</v>
-      </c>
-      <c r="ZR2">
-        <v>18.23</v>
-      </c>
-      <c r="ZS2">
-        <v>59.53</v>
-      </c>
-      <c r="ZT2">
-        <v>8.98</v>
-      </c>
       <c r="ZU2">
-        <v>327</v>
+        <v>59.87</v>
+      </c>
+      <c r="ZV2">
+        <v>8.710000000000001</v>
+      </c>
+      <c r="ZW2">
+        <v>285.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created streamlit first pages
</commit_message>
<xml_diff>
--- a/outData/FilledPriceDaily.xlsx
+++ b/outData/FilledPriceDaily.xlsx
@@ -2110,7 +2110,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-07</t>
+    <t>2025-04-08</t>
   </si>
 </sst>
 </file>
@@ -4575,2095 +4575,2095 @@
         <v>698</v>
       </c>
       <c r="B2">
-        <v>110.34</v>
+        <v>105.54</v>
       </c>
       <c r="C2">
-        <v>81.66</v>
+        <v>80.27</v>
       </c>
       <c r="D2">
-        <v>430.82</v>
+        <v>443.36</v>
       </c>
       <c r="E2">
-        <v>75.41</v>
+        <v>75.14</v>
       </c>
       <c r="F2">
-        <v>151.47</v>
+        <v>151.14</v>
       </c>
       <c r="G2">
-        <v>40.06</v>
+        <v>40.34</v>
       </c>
       <c r="H2">
-        <v>160.23</v>
+        <v>158.39</v>
       </c>
       <c r="I2">
-        <v>531.65</v>
+        <v>525.48</v>
       </c>
       <c r="J2">
+        <v>94.15000000000001</v>
+      </c>
+      <c r="K2">
+        <v>127.05</v>
+      </c>
+      <c r="L2">
+        <v>211.69</v>
+      </c>
+      <c r="M2">
+        <v>150</v>
+      </c>
+      <c r="N2">
+        <v>68.42</v>
+      </c>
+      <c r="O2">
+        <v>173.84</v>
+      </c>
+      <c r="P2">
+        <v>167.51</v>
+      </c>
+      <c r="Q2">
+        <v>218.41</v>
+      </c>
+      <c r="R2">
+        <v>88.59999999999999</v>
+      </c>
+      <c r="S2">
+        <v>29.7</v>
+      </c>
+      <c r="T2">
+        <v>29.32</v>
+      </c>
+      <c r="U2">
+        <v>42.24</v>
+      </c>
+      <c r="V2">
+        <v>88.76000000000001</v>
+      </c>
+      <c r="W2">
+        <v>55.86</v>
+      </c>
+      <c r="X2">
+        <v>47.24</v>
+      </c>
+      <c r="Y2">
+        <v>83.56</v>
+      </c>
+      <c r="Z2">
+        <v>50.95</v>
+      </c>
+      <c r="AA2">
+        <v>45.26</v>
+      </c>
+      <c r="AB2">
+        <v>55.58</v>
+      </c>
+      <c r="AC2">
+        <v>48.43</v>
+      </c>
+      <c r="AD2">
+        <v>55.56</v>
+      </c>
+      <c r="AE2">
+        <v>73</v>
+      </c>
+      <c r="AF2">
+        <v>56.74</v>
+      </c>
+      <c r="AG2">
+        <v>68</v>
+      </c>
+      <c r="AH2">
+        <v>52.27</v>
+      </c>
+      <c r="AI2">
+        <v>919.9299999999999</v>
+      </c>
+      <c r="AJ2">
+        <v>132.82</v>
+      </c>
+      <c r="AK2">
+        <v>91.66</v>
+      </c>
+      <c r="AL2">
+        <v>69.53</v>
+      </c>
+      <c r="AM2">
+        <v>140.3</v>
+      </c>
+      <c r="AN2">
+        <v>200.83</v>
+      </c>
+      <c r="AO2">
+        <v>133.28</v>
+      </c>
+      <c r="AP2">
+        <v>441.5</v>
+      </c>
+      <c r="AQ2">
+        <v>103.68</v>
+      </c>
+      <c r="AR2">
+        <v>81.79000000000001</v>
+      </c>
+      <c r="AS2">
         <v>96.97</v>
       </c>
-      <c r="K2">
-        <v>126.6</v>
-      </c>
-      <c r="L2">
-        <v>216.94</v>
-      </c>
-      <c r="M2">
-        <v>150.62</v>
-      </c>
-      <c r="N2">
-        <v>68.37</v>
-      </c>
-      <c r="O2">
-        <v>175.42</v>
-      </c>
-      <c r="P2">
-        <v>170.8</v>
-      </c>
-      <c r="Q2">
-        <v>221.75</v>
-      </c>
-      <c r="R2">
-        <v>89.19</v>
-      </c>
-      <c r="S2">
-        <v>30.22</v>
-      </c>
-      <c r="T2">
-        <v>30.04</v>
-      </c>
-      <c r="U2">
-        <v>43.68</v>
-      </c>
-      <c r="V2">
-        <v>94.38</v>
-      </c>
-      <c r="W2">
-        <v>59.27</v>
-      </c>
-      <c r="X2">
-        <v>47.5</v>
-      </c>
-      <c r="Y2">
-        <v>86.56999999999999</v>
-      </c>
-      <c r="Z2">
-        <v>51.28</v>
-      </c>
-      <c r="AA2">
-        <v>47.67</v>
-      </c>
-      <c r="AB2">
-        <v>55.85</v>
-      </c>
-      <c r="AC2">
-        <v>51.12</v>
-      </c>
-      <c r="AD2">
-        <v>55.66</v>
-      </c>
-      <c r="AE2">
-        <v>73.25</v>
-      </c>
-      <c r="AF2">
-        <v>56.69</v>
-      </c>
-      <c r="AG2">
-        <v>69.45999999999999</v>
-      </c>
-      <c r="AH2">
-        <v>52.77</v>
-      </c>
-      <c r="AI2">
-        <v>923.85</v>
-      </c>
-      <c r="AJ2">
-        <v>130.21</v>
-      </c>
-      <c r="AK2">
-        <v>96.93000000000001</v>
-      </c>
-      <c r="AL2">
-        <v>71.37</v>
-      </c>
-      <c r="AM2">
-        <v>143.19</v>
-      </c>
-      <c r="AN2">
-        <v>205.08</v>
-      </c>
-      <c r="AO2">
-        <v>134.54</v>
-      </c>
-      <c r="AP2">
-        <v>438.31</v>
-      </c>
-      <c r="AQ2">
-        <v>104.97</v>
-      </c>
-      <c r="AR2">
-        <v>83.83</v>
-      </c>
-      <c r="AS2">
-        <v>106.7</v>
-      </c>
       <c r="AT2">
-        <v>105.4</v>
+        <v>106.05</v>
       </c>
       <c r="AU2">
-        <v>31.59</v>
+        <v>31.5</v>
       </c>
       <c r="AV2">
-        <v>281.22</v>
+        <v>276.76</v>
       </c>
       <c r="AW2">
-        <v>87.02</v>
+        <v>86.84999999999999</v>
       </c>
       <c r="AX2">
-        <v>299.89</v>
+        <v>299.83</v>
       </c>
       <c r="AY2">
-        <v>72.43000000000001</v>
+        <v>72.76000000000001</v>
       </c>
       <c r="AZ2">
-        <v>42.98</v>
+        <v>41.79</v>
       </c>
       <c r="BA2">
-        <v>327.12</v>
+        <v>317.1</v>
       </c>
       <c r="BB2">
-        <v>83.15000000000001</v>
+        <v>81.88</v>
       </c>
       <c r="BC2">
-        <v>138.9</v>
+        <v>136.4</v>
       </c>
       <c r="BD2">
-        <v>322.81</v>
+        <v>313.51</v>
       </c>
       <c r="BE2">
-        <v>16.87</v>
+        <v>16.66</v>
       </c>
       <c r="BF2">
+        <v>46.4</v>
+      </c>
+      <c r="BG2">
+        <v>35.36</v>
+      </c>
+      <c r="BH2">
+        <v>40.6</v>
+      </c>
+      <c r="BI2">
+        <v>100.77</v>
+      </c>
+      <c r="BJ2">
+        <v>99.77</v>
+      </c>
+      <c r="BK2">
+        <v>248.61</v>
+      </c>
+      <c r="BL2">
+        <v>190.11</v>
+      </c>
+      <c r="BM2">
+        <v>146.85</v>
+      </c>
+      <c r="BN2">
+        <v>64.40000000000001</v>
+      </c>
+      <c r="BO2">
+        <v>36.71</v>
+      </c>
+      <c r="BP2">
+        <v>56.55</v>
+      </c>
+      <c r="BQ2">
+        <v>59.18</v>
+      </c>
+      <c r="BR2">
+        <v>136.93</v>
+      </c>
+      <c r="BS2">
+        <v>30.18</v>
+      </c>
+      <c r="BT2">
+        <v>54.28</v>
+      </c>
+      <c r="BU2">
+        <v>43.4</v>
+      </c>
+      <c r="BV2">
+        <v>37.56</v>
+      </c>
+      <c r="BW2">
+        <v>163.54</v>
+      </c>
+      <c r="BX2">
+        <v>380.51</v>
+      </c>
+      <c r="BY2">
+        <v>254.4</v>
+      </c>
+      <c r="BZ2">
+        <v>15.6</v>
+      </c>
+      <c r="CA2">
+        <v>37.62</v>
+      </c>
+      <c r="CB2">
+        <v>66.45</v>
+      </c>
+      <c r="CC2">
+        <v>101.45</v>
+      </c>
+      <c r="CD2">
+        <v>44.72</v>
+      </c>
+      <c r="CE2">
+        <v>170.72</v>
+      </c>
+      <c r="CF2">
+        <v>225.65</v>
+      </c>
+      <c r="CG2">
+        <v>50.88</v>
+      </c>
+      <c r="CH2">
+        <v>86.59</v>
+      </c>
+      <c r="CI2">
+        <v>84.20999999999999</v>
+      </c>
+      <c r="CJ2">
+        <v>133.66</v>
+      </c>
+      <c r="CK2">
+        <v>519.1900000000001</v>
+      </c>
+      <c r="CL2">
+        <v>52.27</v>
+      </c>
+      <c r="CM2">
+        <v>24.16</v>
+      </c>
+      <c r="CN2">
+        <v>273.94</v>
+      </c>
+      <c r="CO2">
+        <v>105.8</v>
+      </c>
+      <c r="CP2">
+        <v>59.63</v>
+      </c>
+      <c r="CQ2">
+        <v>274.99</v>
+      </c>
+      <c r="CR2">
+        <v>190.39</v>
+      </c>
+      <c r="CS2">
+        <v>413.33</v>
+      </c>
+      <c r="CT2">
+        <v>337.37</v>
+      </c>
+      <c r="CU2">
+        <v>102.08</v>
+      </c>
+      <c r="CV2">
+        <v>120.46</v>
+      </c>
+      <c r="CW2">
+        <v>50.76</v>
+      </c>
+      <c r="CX2">
+        <v>254.65</v>
+      </c>
+      <c r="CY2">
+        <v>102.84</v>
+      </c>
+      <c r="CZ2">
+        <v>34.42</v>
+      </c>
+      <c r="DA2">
+        <v>64.11</v>
+      </c>
+      <c r="DB2">
+        <v>112.41</v>
+      </c>
+      <c r="DC2">
+        <v>26.61</v>
+      </c>
+      <c r="DD2">
+        <v>226.21</v>
+      </c>
+      <c r="DE2">
+        <v>31.97</v>
+      </c>
+      <c r="DF2">
+        <v>92.66</v>
+      </c>
+      <c r="DG2">
+        <v>221.03</v>
+      </c>
+      <c r="DH2">
+        <v>167.18</v>
+      </c>
+      <c r="DI2">
+        <v>19.12</v>
+      </c>
+      <c r="DJ2">
+        <v>46.85</v>
+      </c>
+      <c r="DK2">
+        <v>125</v>
+      </c>
+      <c r="DL2">
+        <v>101.6</v>
+      </c>
+      <c r="DM2">
+        <v>36.5</v>
+      </c>
+      <c r="DN2">
+        <v>41.09</v>
+      </c>
+      <c r="DO2">
+        <v>37.58</v>
+      </c>
+      <c r="DP2">
+        <v>33.63</v>
+      </c>
+      <c r="DQ2">
+        <v>110.18</v>
+      </c>
+      <c r="DR2">
+        <v>10.8</v>
+      </c>
+      <c r="DS2">
+        <v>29.09</v>
+      </c>
+      <c r="DT2">
+        <v>74.02</v>
+      </c>
+      <c r="DU2">
+        <v>63.76</v>
+      </c>
+      <c r="DV2">
+        <v>56.12</v>
+      </c>
+      <c r="DW2">
+        <v>86.97</v>
+      </c>
+      <c r="DX2">
+        <v>398.85</v>
+      </c>
+      <c r="DY2">
+        <v>54.25</v>
+      </c>
+      <c r="DZ2">
+        <v>39.72</v>
+      </c>
+      <c r="EA2">
+        <v>16.23</v>
+      </c>
+      <c r="EB2">
+        <v>416.49</v>
+      </c>
+      <c r="EC2">
+        <v>72.20999999999999</v>
+      </c>
+      <c r="ED2">
+        <v>71.2</v>
+      </c>
+      <c r="EE2">
+        <v>22</v>
+      </c>
+      <c r="EF2">
+        <v>21.89</v>
+      </c>
+      <c r="EG2">
+        <v>155.48</v>
+      </c>
+      <c r="EH2">
+        <v>39.19</v>
+      </c>
+      <c r="EI2">
+        <v>27</v>
+      </c>
+      <c r="EJ2">
+        <v>86.86</v>
+      </c>
+      <c r="EK2">
+        <v>200.75</v>
+      </c>
+      <c r="EL2">
+        <v>53.27</v>
+      </c>
+      <c r="EM2">
+        <v>65.31999999999999</v>
+      </c>
+      <c r="EN2">
+        <v>116.32</v>
+      </c>
+      <c r="EO2">
+        <v>20.67</v>
+      </c>
+      <c r="EP2">
+        <v>24.55</v>
+      </c>
+      <c r="EQ2">
+        <v>166.09</v>
+      </c>
+      <c r="ER2">
+        <v>354.56</v>
+      </c>
+      <c r="ES2">
+        <v>39.55</v>
+      </c>
+      <c r="ET2">
+        <v>17.65</v>
+      </c>
+      <c r="EU2">
+        <v>124.66</v>
+      </c>
+      <c r="EV2">
+        <v>236.53</v>
+      </c>
+      <c r="EW2">
+        <v>50.65</v>
+      </c>
+      <c r="EX2">
+        <v>89.91</v>
+      </c>
+      <c r="EY2">
+        <v>60.87</v>
+      </c>
+      <c r="EZ2">
+        <v>42.18</v>
+      </c>
+      <c r="FA2">
+        <v>491.97</v>
+      </c>
+      <c r="FB2">
+        <v>35.34</v>
+      </c>
+      <c r="FC2">
+        <v>146.01</v>
+      </c>
+      <c r="FD2">
+        <v>64.51000000000001</v>
+      </c>
+      <c r="FE2">
+        <v>52.5</v>
+      </c>
+      <c r="FF2">
+        <v>89.64</v>
+      </c>
+      <c r="FG2">
+        <v>56.17</v>
+      </c>
+      <c r="FH2">
+        <v>125.1</v>
+      </c>
+      <c r="FI2">
+        <v>73.95999999999999</v>
+      </c>
+      <c r="FJ2">
+        <v>227.2</v>
+      </c>
+      <c r="FK2">
+        <v>129.46</v>
+      </c>
+      <c r="FL2">
+        <v>27.92</v>
+      </c>
+      <c r="FM2">
+        <v>216.47</v>
+      </c>
+      <c r="FN2">
+        <v>63.51</v>
+      </c>
+      <c r="FO2">
+        <v>67.04000000000001</v>
+      </c>
+      <c r="FP2">
+        <v>58.79</v>
+      </c>
+      <c r="FQ2">
+        <v>102.95</v>
+      </c>
+      <c r="FR2">
+        <v>152.69</v>
+      </c>
+      <c r="FS2">
+        <v>83.08</v>
+      </c>
+      <c r="FT2">
+        <v>179.73</v>
+      </c>
+      <c r="FU2">
+        <v>908.75</v>
+      </c>
+      <c r="FV2">
+        <v>42.17</v>
+      </c>
+      <c r="FW2">
+        <v>238.87</v>
+      </c>
+      <c r="FX2">
+        <v>81.69</v>
+      </c>
+      <c r="FY2">
+        <v>103.32</v>
+      </c>
+      <c r="FZ2">
+        <v>129.4</v>
+      </c>
+      <c r="GA2">
+        <v>130.14</v>
+      </c>
+      <c r="GB2">
+        <v>115.95</v>
+      </c>
+      <c r="GC2">
+        <v>61.79</v>
+      </c>
+      <c r="GD2">
+        <v>54.76</v>
+      </c>
+      <c r="GE2">
         <v>46.33</v>
       </c>
-      <c r="BG2">
-        <v>35.25</v>
-      </c>
-      <c r="BH2">
-        <v>41.8</v>
-      </c>
-      <c r="BI2">
-        <v>102.94</v>
-      </c>
-      <c r="BJ2">
-        <v>100</v>
-      </c>
-      <c r="BK2">
-        <v>259.1</v>
-      </c>
-      <c r="BL2">
-        <v>190.54</v>
-      </c>
-      <c r="BM2">
-        <v>145.06</v>
-      </c>
-      <c r="BN2">
-        <v>64.31999999999999</v>
-      </c>
-      <c r="BO2">
-        <v>37.51</v>
-      </c>
-      <c r="BP2">
-        <v>57.53</v>
-      </c>
-      <c r="BQ2">
-        <v>59.87</v>
-      </c>
-      <c r="BR2">
-        <v>140.15</v>
-      </c>
-      <c r="BS2">
-        <v>30.51</v>
-      </c>
-      <c r="BT2">
-        <v>54.49</v>
-      </c>
-      <c r="BU2">
-        <v>43.92</v>
-      </c>
-      <c r="BV2">
-        <v>38.49</v>
-      </c>
-      <c r="BW2">
-        <v>169.36</v>
-      </c>
-      <c r="BX2">
-        <v>381.05</v>
-      </c>
-      <c r="BY2">
-        <v>247.68</v>
-      </c>
-      <c r="BZ2">
-        <v>15.69</v>
-      </c>
-      <c r="CA2">
-        <v>38.32</v>
-      </c>
-      <c r="CB2">
-        <v>67.84999999999999</v>
-      </c>
-      <c r="CC2">
-        <v>104.66</v>
-      </c>
-      <c r="CD2">
-        <v>44.81</v>
-      </c>
-      <c r="CE2">
-        <v>172.87</v>
-      </c>
-      <c r="CF2">
-        <v>230.33</v>
-      </c>
-      <c r="CG2">
-        <v>51.21</v>
-      </c>
-      <c r="CH2">
-        <v>86.61</v>
-      </c>
-      <c r="CI2">
-        <v>85.51000000000001</v>
-      </c>
-      <c r="CJ2">
-        <v>134.65</v>
-      </c>
-      <c r="CK2">
-        <v>532.54</v>
-      </c>
-      <c r="CL2">
-        <v>52.93</v>
-      </c>
-      <c r="CM2">
-        <v>24.14</v>
-      </c>
-      <c r="CN2">
-        <v>280.06</v>
-      </c>
-      <c r="CO2">
-        <v>106.15</v>
-      </c>
-      <c r="CP2">
-        <v>60.64</v>
-      </c>
-      <c r="CQ2">
-        <v>274.32</v>
-      </c>
-      <c r="CR2">
-        <v>201.47</v>
-      </c>
-      <c r="CS2">
-        <v>425.86</v>
-      </c>
-      <c r="CT2">
-        <v>345.34</v>
-      </c>
-      <c r="CU2">
-        <v>103.07</v>
-      </c>
-      <c r="CV2">
-        <v>117.32</v>
-      </c>
-      <c r="CW2">
-        <v>58.1</v>
-      </c>
-      <c r="CX2">
-        <v>262.39</v>
-      </c>
-      <c r="CY2">
-        <v>105.66</v>
-      </c>
-      <c r="CZ2">
-        <v>34.55</v>
-      </c>
-      <c r="DA2">
-        <v>65.06</v>
-      </c>
-      <c r="DB2">
-        <v>112.67</v>
-      </c>
-      <c r="DC2">
-        <v>26.75</v>
-      </c>
-      <c r="DD2">
-        <v>220.37</v>
-      </c>
-      <c r="DE2">
-        <v>35</v>
-      </c>
-      <c r="DF2">
-        <v>94.75</v>
-      </c>
-      <c r="DG2">
-        <v>225.78</v>
-      </c>
-      <c r="DH2">
-        <v>168.72</v>
-      </c>
-      <c r="DI2">
-        <v>19.88</v>
-      </c>
-      <c r="DJ2">
-        <v>46.94</v>
-      </c>
-      <c r="DK2">
-        <v>125.68</v>
-      </c>
-      <c r="DL2">
-        <v>102.55</v>
-      </c>
-      <c r="DM2">
-        <v>37.08</v>
-      </c>
-      <c r="DN2">
-        <v>41.95</v>
-      </c>
-      <c r="DO2">
-        <v>38.16</v>
-      </c>
-      <c r="DP2">
-        <v>33.66</v>
-      </c>
-      <c r="DQ2">
-        <v>113.03</v>
-      </c>
-      <c r="DR2">
-        <v>11.06</v>
-      </c>
-      <c r="DS2">
-        <v>29.8</v>
-      </c>
-      <c r="DT2">
-        <v>74.43000000000001</v>
-      </c>
-      <c r="DU2">
-        <v>63.99</v>
-      </c>
-      <c r="DV2">
-        <v>56.96</v>
-      </c>
-      <c r="DW2">
-        <v>89.17</v>
-      </c>
-      <c r="DX2">
-        <v>405.58</v>
-      </c>
-      <c r="DY2">
-        <v>55.56</v>
-      </c>
-      <c r="DZ2">
-        <v>40.74</v>
-      </c>
-      <c r="EA2">
-        <v>16.47</v>
-      </c>
-      <c r="EB2">
-        <v>418.01</v>
-      </c>
-      <c r="EC2">
-        <v>73.92</v>
-      </c>
-      <c r="ED2">
-        <v>72.16</v>
-      </c>
-      <c r="EE2">
-        <v>22.31</v>
-      </c>
-      <c r="EF2">
-        <v>22.1</v>
-      </c>
-      <c r="EG2">
-        <v>156.98</v>
-      </c>
-      <c r="EH2">
-        <v>40.04</v>
-      </c>
-      <c r="EI2">
-        <v>27.15</v>
-      </c>
-      <c r="EJ2">
-        <v>87.22</v>
-      </c>
-      <c r="EK2">
-        <v>200.21</v>
-      </c>
-      <c r="EL2">
-        <v>55.61</v>
-      </c>
-      <c r="EM2">
-        <v>64.28</v>
-      </c>
-      <c r="EN2">
-        <v>119.62</v>
-      </c>
-      <c r="EO2">
-        <v>20.58</v>
-      </c>
-      <c r="EP2">
-        <v>26.04</v>
-      </c>
-      <c r="EQ2">
-        <v>171.34</v>
-      </c>
-      <c r="ER2">
-        <v>357.86</v>
-      </c>
-      <c r="ES2">
-        <v>39.56</v>
-      </c>
-      <c r="ET2">
-        <v>18.32</v>
-      </c>
-      <c r="EU2">
-        <v>129.72</v>
-      </c>
-      <c r="EV2">
-        <v>233.83</v>
-      </c>
-      <c r="EW2">
-        <v>50.95</v>
-      </c>
-      <c r="EX2">
-        <v>90.47</v>
-      </c>
-      <c r="EY2">
-        <v>61.62</v>
-      </c>
-      <c r="EZ2">
-        <v>42.9</v>
-      </c>
-      <c r="FA2">
-        <v>481.57</v>
-      </c>
-      <c r="FB2">
+      <c r="GF2">
+        <v>136.11</v>
+      </c>
+      <c r="GG2">
+        <v>274.73</v>
+      </c>
+      <c r="GH2">
+        <v>26.69</v>
+      </c>
+      <c r="GI2">
+        <v>88.56999999999999</v>
+      </c>
+      <c r="GJ2">
+        <v>63.78</v>
+      </c>
+      <c r="GK2">
+        <v>45.48</v>
+      </c>
+      <c r="GL2">
+        <v>267.12</v>
+      </c>
+      <c r="GM2">
+        <v>426.02</v>
+      </c>
+      <c r="GN2">
+        <v>208.55</v>
+      </c>
+      <c r="GO2">
+        <v>113.29</v>
+      </c>
+      <c r="GP2">
+        <v>94.06</v>
+      </c>
+      <c r="GQ2">
+        <v>89.06999999999999</v>
+      </c>
+      <c r="GR2">
+        <v>42.23</v>
+      </c>
+      <c r="GS2">
+        <v>117.13</v>
+      </c>
+      <c r="GT2">
+        <v>66.37</v>
+      </c>
+      <c r="GU2">
+        <v>31.36</v>
+      </c>
+      <c r="GV2">
+        <v>20.21</v>
+      </c>
+      <c r="GW2">
+        <v>70.19</v>
+      </c>
+      <c r="GX2">
+        <v>53.07</v>
+      </c>
+      <c r="GY2">
+        <v>139.21</v>
+      </c>
+      <c r="GZ2">
+        <v>41.42</v>
+      </c>
+      <c r="HA2">
+        <v>163.77</v>
+      </c>
+      <c r="HB2">
+        <v>208.27</v>
+      </c>
+      <c r="HC2">
+        <v>217.22</v>
+      </c>
+      <c r="HD2">
+        <v>97.26000000000001</v>
+      </c>
+      <c r="HE2">
+        <v>652.83</v>
+      </c>
+      <c r="HF2">
+        <v>123.75</v>
+      </c>
+      <c r="HG2">
+        <v>317.5</v>
+      </c>
+      <c r="HH2">
+        <v>67.11</v>
+      </c>
+      <c r="HI2">
+        <v>308.27</v>
+      </c>
+      <c r="HJ2">
+        <v>69.56</v>
+      </c>
+      <c r="HK2">
+        <v>19.44</v>
+      </c>
+      <c r="HL2">
+        <v>149.23</v>
+      </c>
+      <c r="HM2">
+        <v>95.12</v>
+      </c>
+      <c r="HN2">
+        <v>70.48</v>
+      </c>
+      <c r="HO2">
+        <v>221.81</v>
+      </c>
+      <c r="HP2">
+        <v>64.83</v>
+      </c>
+      <c r="HQ2">
+        <v>140.87</v>
+      </c>
+      <c r="HR2">
+        <v>571.76</v>
+      </c>
+      <c r="HS2">
+        <v>32.84</v>
+      </c>
+      <c r="HT2">
+        <v>63.77</v>
+      </c>
+      <c r="HU2">
+        <v>218.48</v>
+      </c>
+      <c r="HV2">
+        <v>510.52</v>
+      </c>
+      <c r="HW2">
+        <v>206.03</v>
+      </c>
+      <c r="HX2">
+        <v>48.02</v>
+      </c>
+      <c r="HY2">
+        <v>815.72</v>
+      </c>
+      <c r="HZ2">
+        <v>35.88</v>
+      </c>
+      <c r="IA2">
+        <v>12.81</v>
+      </c>
+      <c r="IB2">
+        <v>309.39</v>
+      </c>
+      <c r="IC2">
+        <v>37.49</v>
+      </c>
+      <c r="ID2">
+        <v>70.23999999999999</v>
+      </c>
+      <c r="IE2">
+        <v>106.53</v>
+      </c>
+      <c r="IF2">
+        <v>68.88</v>
+      </c>
+      <c r="IG2">
+        <v>124.5</v>
+      </c>
+      <c r="IH2">
+        <v>168.53</v>
+      </c>
+      <c r="II2">
+        <v>72.7</v>
+      </c>
+      <c r="IJ2">
+        <v>251.5</v>
+      </c>
+      <c r="IK2">
+        <v>218.97</v>
+      </c>
+      <c r="IL2">
+        <v>22.32</v>
+      </c>
+      <c r="IM2">
+        <v>39.65</v>
+      </c>
+      <c r="IN2">
+        <v>91.92</v>
+      </c>
+      <c r="IO2">
+        <v>396.7</v>
+      </c>
+      <c r="IP2">
+        <v>56.4</v>
+      </c>
+      <c r="IQ2">
+        <v>161.94</v>
+      </c>
+      <c r="IR2">
+        <v>220.65</v>
+      </c>
+      <c r="IS2">
+        <v>206.27</v>
+      </c>
+      <c r="IT2">
+        <v>30.82</v>
+      </c>
+      <c r="IU2">
+        <v>21.88</v>
+      </c>
+      <c r="IV2">
+        <v>335.24</v>
+      </c>
+      <c r="IW2">
+        <v>159.1</v>
+      </c>
+      <c r="IX2">
+        <v>553.08</v>
+      </c>
+      <c r="IY2">
         <v>38.09</v>
       </c>
-      <c r="FC2">
-        <v>154</v>
-      </c>
-      <c r="FD2">
-        <v>64.36</v>
-      </c>
-      <c r="FE2">
-        <v>53.62</v>
-      </c>
-      <c r="FF2">
-        <v>90.56</v>
-      </c>
-      <c r="FG2">
-        <v>61.23</v>
-      </c>
-      <c r="FH2">
-        <v>126.28</v>
-      </c>
-      <c r="FI2">
-        <v>73.73</v>
-      </c>
-      <c r="FJ2">
-        <v>230.93</v>
-      </c>
-      <c r="FK2">
-        <v>132.07</v>
-      </c>
-      <c r="FL2">
-        <v>28.08</v>
-      </c>
-      <c r="FM2">
-        <v>220.56</v>
-      </c>
-      <c r="FN2">
-        <v>64.33</v>
-      </c>
-      <c r="FO2">
-        <v>67.06</v>
-      </c>
-      <c r="FP2">
-        <v>59.81</v>
-      </c>
-      <c r="FQ2">
-        <v>103.21</v>
-      </c>
-      <c r="FR2">
-        <v>150.66</v>
-      </c>
-      <c r="FS2">
-        <v>86.22</v>
-      </c>
-      <c r="FT2">
-        <v>181.41</v>
-      </c>
-      <c r="FU2">
-        <v>908.13</v>
-      </c>
-      <c r="FV2">
-        <v>42.58</v>
-      </c>
-      <c r="FW2">
-        <v>236.44</v>
-      </c>
-      <c r="FX2">
-        <v>81.64</v>
-      </c>
-      <c r="FY2">
-        <v>105.47</v>
-      </c>
-      <c r="FZ2">
-        <v>133.09</v>
-      </c>
-      <c r="GA2">
-        <v>132.12</v>
-      </c>
-      <c r="GB2">
-        <v>116.86</v>
-      </c>
-      <c r="GC2">
-        <v>63.34</v>
-      </c>
-      <c r="GD2">
-        <v>54.72</v>
-      </c>
-      <c r="GE2">
-        <v>47.31</v>
-      </c>
-      <c r="GF2">
-        <v>136.67</v>
-      </c>
-      <c r="GG2">
-        <v>274.56</v>
-      </c>
-      <c r="GH2">
-        <v>27.09</v>
-      </c>
-      <c r="GI2">
-        <v>87.23</v>
-      </c>
-      <c r="GJ2">
-        <v>63.91</v>
-      </c>
-      <c r="GK2">
-        <v>46</v>
-      </c>
-      <c r="GL2">
-        <v>275.67</v>
-      </c>
-      <c r="GM2">
-        <v>427.95</v>
-      </c>
-      <c r="GN2">
-        <v>212.76</v>
-      </c>
-      <c r="GO2">
-        <v>114.33</v>
-      </c>
-      <c r="GP2">
-        <v>95.78</v>
-      </c>
-      <c r="GQ2">
-        <v>88.76000000000001</v>
-      </c>
-      <c r="GR2">
-        <v>42.24</v>
-      </c>
-      <c r="GS2">
-        <v>116.9</v>
-      </c>
-      <c r="GT2">
-        <v>66.45999999999999</v>
-      </c>
-      <c r="GU2">
-        <v>32.01</v>
-      </c>
-      <c r="GV2">
-        <v>20.47</v>
-      </c>
-      <c r="GW2">
-        <v>70.94</v>
-      </c>
-      <c r="GX2">
-        <v>55.19</v>
-      </c>
-      <c r="GY2">
-        <v>145.09</v>
-      </c>
-      <c r="GZ2">
-        <v>41.58</v>
-      </c>
-      <c r="HA2">
-        <v>164.87</v>
-      </c>
-      <c r="HB2">
-        <v>209.97</v>
-      </c>
-      <c r="HC2">
-        <v>220.24</v>
-      </c>
-      <c r="HD2">
-        <v>101.9</v>
-      </c>
-      <c r="HE2">
-        <v>661.97</v>
-      </c>
-      <c r="HF2">
-        <v>124.63</v>
-      </c>
-      <c r="HG2">
-        <v>316.89</v>
-      </c>
-      <c r="HH2">
-        <v>66.91</v>
-      </c>
-      <c r="HI2">
-        <v>312.32</v>
-      </c>
-      <c r="HJ2">
-        <v>71.65000000000001</v>
-      </c>
-      <c r="HK2">
-        <v>20.6</v>
-      </c>
-      <c r="HL2">
-        <v>151.23</v>
-      </c>
-      <c r="HM2">
-        <v>95.78</v>
-      </c>
-      <c r="HN2">
-        <v>70.75</v>
-      </c>
-      <c r="HO2">
-        <v>222.25</v>
-      </c>
-      <c r="HP2">
-        <v>70.38</v>
-      </c>
-      <c r="HQ2">
-        <v>142.36</v>
-      </c>
-      <c r="HR2">
-        <v>575.0700000000001</v>
-      </c>
-      <c r="HS2">
-        <v>33.47</v>
-      </c>
-      <c r="HT2">
-        <v>63.85</v>
-      </c>
-      <c r="HU2">
-        <v>237.93</v>
-      </c>
-      <c r="HV2">
-        <v>524.25</v>
-      </c>
-      <c r="HW2">
-        <v>208.27</v>
-      </c>
-      <c r="HX2">
-        <v>49.35</v>
-      </c>
-      <c r="HY2">
-        <v>817.5</v>
-      </c>
-      <c r="HZ2">
-        <v>37.44</v>
-      </c>
-      <c r="IA2">
-        <v>13.11</v>
-      </c>
-      <c r="IB2">
-        <v>310.77</v>
-      </c>
-      <c r="IC2">
-        <v>40.51</v>
-      </c>
-      <c r="ID2">
-        <v>73.3</v>
-      </c>
-      <c r="IE2">
-        <v>108.05</v>
-      </c>
-      <c r="IF2">
-        <v>68.66</v>
-      </c>
-      <c r="IG2">
-        <v>127.16</v>
-      </c>
-      <c r="IH2">
-        <v>168.32</v>
-      </c>
-      <c r="II2">
-        <v>73.65000000000001</v>
-      </c>
-      <c r="IJ2">
-        <v>252.45</v>
-      </c>
-      <c r="IK2">
-        <v>227.62</v>
-      </c>
-      <c r="IL2">
-        <v>22.31</v>
-      </c>
-      <c r="IM2">
-        <v>40.42</v>
-      </c>
-      <c r="IN2">
-        <v>95.56</v>
-      </c>
-      <c r="IO2">
-        <v>398</v>
-      </c>
-      <c r="IP2">
-        <v>56.7</v>
-      </c>
-      <c r="IQ2">
-        <v>162.93</v>
-      </c>
-      <c r="IR2">
-        <v>223.74</v>
-      </c>
-      <c r="IS2">
-        <v>207.92</v>
-      </c>
-      <c r="IT2">
-        <v>31.57</v>
-      </c>
-      <c r="IU2">
-        <v>23.38</v>
-      </c>
-      <c r="IV2">
-        <v>341.51</v>
-      </c>
-      <c r="IW2">
-        <v>162.6</v>
-      </c>
-      <c r="IX2">
-        <v>524.7</v>
-      </c>
-      <c r="IY2">
+      <c r="IZ2">
+        <v>156.03</v>
+      </c>
+      <c r="JA2">
+        <v>149.97</v>
+      </c>
+      <c r="JB2">
+        <v>599.51</v>
+      </c>
+      <c r="JC2">
+        <v>101.28</v>
+      </c>
+      <c r="JD2">
+        <v>27.4</v>
+      </c>
+      <c r="JE2">
+        <v>123.22</v>
+      </c>
+      <c r="JF2">
+        <v>271.94</v>
+      </c>
+      <c r="JG2">
+        <v>216.87</v>
+      </c>
+      <c r="JH2">
+        <v>77.89</v>
+      </c>
+      <c r="JI2">
+        <v>149.72</v>
+      </c>
+      <c r="JJ2">
+        <v>48.72</v>
+      </c>
+      <c r="JK2">
+        <v>49.15</v>
+      </c>
+      <c r="JL2">
+        <v>54.63</v>
+      </c>
+      <c r="JM2">
+        <v>40.26</v>
+      </c>
+      <c r="JN2">
+        <v>110.1</v>
+      </c>
+      <c r="JO2">
+        <v>182.86</v>
+      </c>
+      <c r="JP2">
+        <v>25.05</v>
+      </c>
+      <c r="JQ2">
+        <v>78.95</v>
+      </c>
+      <c r="JR2">
+        <v>78.45</v>
+      </c>
+      <c r="JS2">
+        <v>137.01</v>
+      </c>
+      <c r="JT2">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="JU2">
+        <v>21.84</v>
+      </c>
+      <c r="JV2">
+        <v>141.27</v>
+      </c>
+      <c r="JW2">
+        <v>51.18</v>
+      </c>
+      <c r="JX2">
+        <v>24.21</v>
+      </c>
+      <c r="JY2">
+        <v>208.13</v>
+      </c>
+      <c r="JZ2">
+        <v>150.5</v>
+      </c>
+      <c r="KA2">
+        <v>73.5</v>
+      </c>
+      <c r="KB2">
+        <v>64.55</v>
+      </c>
+      <c r="KC2">
+        <v>311.53</v>
+      </c>
+      <c r="KD2">
+        <v>159.58</v>
+      </c>
+      <c r="KE2">
+        <v>28.93</v>
+      </c>
+      <c r="KF2">
+        <v>255.03</v>
+      </c>
+      <c r="KG2">
+        <v>53.19</v>
+      </c>
+      <c r="KH2">
+        <v>430.9</v>
+      </c>
+      <c r="KI2">
+        <v>73.58</v>
+      </c>
+      <c r="KJ2">
+        <v>79.69</v>
+      </c>
+      <c r="KK2">
+        <v>262.08</v>
+      </c>
+      <c r="KL2">
+        <v>159.8</v>
+      </c>
+      <c r="KM2">
+        <v>294.77</v>
+      </c>
+      <c r="KN2">
+        <v>148.21</v>
+      </c>
+      <c r="KO2">
+        <v>18.89</v>
+      </c>
+      <c r="KP2">
+        <v>31</v>
+      </c>
+      <c r="KQ2">
+        <v>58.03</v>
+      </c>
+      <c r="KR2">
+        <v>126.61</v>
+      </c>
+      <c r="KS2">
+        <v>33.42</v>
+      </c>
+      <c r="KT2">
+        <v>31.69</v>
+      </c>
+      <c r="KU2">
+        <v>244.39</v>
+      </c>
+      <c r="KV2">
+        <v>290.96</v>
+      </c>
+      <c r="KW2">
+        <v>149.76</v>
+      </c>
+      <c r="KX2">
+        <v>110.23</v>
+      </c>
+      <c r="KY2">
+        <v>75.33</v>
+      </c>
+      <c r="KZ2">
+        <v>133.95</v>
+      </c>
+      <c r="LA2">
+        <v>110.43</v>
+      </c>
+      <c r="LB2">
+        <v>98</v>
+      </c>
+      <c r="LC2">
+        <v>36.4</v>
+      </c>
+      <c r="LD2">
+        <v>24.28</v>
+      </c>
+      <c r="LE2">
+        <v>76.94</v>
+      </c>
+      <c r="LF2">
+        <v>183.47</v>
+      </c>
+      <c r="LG2">
+        <v>24.79</v>
+      </c>
+      <c r="LH2">
+        <v>183.26</v>
+      </c>
+      <c r="LI2">
+        <v>18.05</v>
+      </c>
+      <c r="LJ2">
+        <v>47.6</v>
+      </c>
+      <c r="LK2">
+        <v>88.81999999999999</v>
+      </c>
+      <c r="LL2">
+        <v>21.9</v>
+      </c>
+      <c r="LM2">
+        <v>36.99</v>
+      </c>
+      <c r="LN2">
+        <v>43.52</v>
+      </c>
+      <c r="LO2">
+        <v>106.69</v>
+      </c>
+      <c r="LP2">
+        <v>60.07</v>
+      </c>
+      <c r="LQ2">
+        <v>57.65</v>
+      </c>
+      <c r="LR2">
+        <v>102.86</v>
+      </c>
+      <c r="LS2">
+        <v>48.95</v>
+      </c>
+      <c r="LT2">
+        <v>77.31</v>
+      </c>
+      <c r="LU2">
+        <v>280.26</v>
+      </c>
+      <c r="LV2">
+        <v>30.4</v>
+      </c>
+      <c r="LW2">
+        <v>19</v>
+      </c>
+      <c r="LX2">
+        <v>145.28</v>
+      </c>
+      <c r="LY2">
+        <v>80.59</v>
+      </c>
+      <c r="LZ2">
+        <v>25.65</v>
+      </c>
+      <c r="MA2">
+        <v>15.54</v>
+      </c>
+      <c r="MB2">
+        <v>57.06</v>
+      </c>
+      <c r="MC2">
+        <v>74.8</v>
+      </c>
+      <c r="MD2">
+        <v>360.23</v>
+      </c>
+      <c r="ME2">
+        <v>99.29000000000001</v>
+      </c>
+      <c r="MF2">
+        <v>26.2</v>
+      </c>
+      <c r="MG2">
+        <v>58.31</v>
+      </c>
+      <c r="MH2">
+        <v>21.78</v>
+      </c>
+      <c r="MI2">
+        <v>394.72</v>
+      </c>
+      <c r="MJ2">
         <v>39.18</v>
       </c>
-      <c r="IZ2">
-        <v>154.14</v>
-      </c>
-      <c r="JA2">
-        <v>150.71</v>
-      </c>
-      <c r="JB2">
-        <v>604.62</v>
-      </c>
-      <c r="JC2">
-        <v>101.57</v>
-      </c>
-      <c r="JD2">
-        <v>27.71</v>
-      </c>
-      <c r="JE2">
-        <v>125.26</v>
-      </c>
-      <c r="JF2">
-        <v>279.69</v>
-      </c>
-      <c r="JG2">
-        <v>214.44</v>
-      </c>
-      <c r="JH2">
-        <v>79.39</v>
-      </c>
-      <c r="JI2">
-        <v>160.04</v>
-      </c>
-      <c r="JJ2">
-        <v>49.38</v>
-      </c>
-      <c r="JK2">
-        <v>50.3</v>
-      </c>
-      <c r="JL2">
-        <v>54.9</v>
-      </c>
-      <c r="JM2">
-        <v>41.19</v>
-      </c>
-      <c r="JN2">
-        <v>109.83</v>
-      </c>
-      <c r="JO2">
-        <v>187.46</v>
-      </c>
-      <c r="JP2">
-        <v>25.12</v>
-      </c>
-      <c r="JQ2">
-        <v>81.18000000000001</v>
-      </c>
-      <c r="JR2">
-        <v>81.2</v>
-      </c>
-      <c r="JS2">
-        <v>140.49</v>
-      </c>
-      <c r="JT2">
-        <v>88.14</v>
-      </c>
-      <c r="JU2">
-        <v>22.63</v>
-      </c>
-      <c r="JV2">
-        <v>142.36</v>
-      </c>
-      <c r="JW2">
-        <v>53.4</v>
-      </c>
-      <c r="JX2">
-        <v>24.97</v>
-      </c>
-      <c r="JY2">
-        <v>207.27</v>
-      </c>
-      <c r="JZ2">
-        <v>154.13</v>
-      </c>
-      <c r="KA2">
-        <v>74.09</v>
-      </c>
-      <c r="KB2">
-        <v>64.64</v>
-      </c>
-      <c r="KC2">
-        <v>310.86</v>
-      </c>
-      <c r="KD2">
-        <v>166.28</v>
-      </c>
-      <c r="KE2">
-        <v>29.85</v>
-      </c>
-      <c r="KF2">
-        <v>252.37</v>
-      </c>
-      <c r="KG2">
-        <v>54.41</v>
-      </c>
-      <c r="KH2">
-        <v>423.14</v>
-      </c>
-      <c r="KI2">
-        <v>75.08</v>
-      </c>
-      <c r="KJ2">
-        <v>80</v>
-      </c>
-      <c r="KK2">
-        <v>263.39</v>
-      </c>
-      <c r="KL2">
-        <v>164.31</v>
-      </c>
-      <c r="KM2">
-        <v>306.48</v>
-      </c>
-      <c r="KN2">
-        <v>150.88</v>
-      </c>
-      <c r="KO2">
-        <v>19.47</v>
-      </c>
-      <c r="KP2">
-        <v>31.05</v>
-      </c>
-      <c r="KQ2">
-        <v>58.26</v>
-      </c>
-      <c r="KR2">
-        <v>132.38</v>
-      </c>
-      <c r="KS2">
-        <v>34.07</v>
-      </c>
-      <c r="KT2">
-        <v>31.91</v>
-      </c>
-      <c r="KU2">
-        <v>245.45</v>
-      </c>
-      <c r="KV2">
-        <v>303.08</v>
-      </c>
-      <c r="KW2">
-        <v>152.81</v>
-      </c>
-      <c r="KX2">
-        <v>111.04</v>
-      </c>
-      <c r="KY2">
-        <v>76.3</v>
-      </c>
-      <c r="KZ2">
-        <v>137.79</v>
-      </c>
-      <c r="LA2">
-        <v>110.14</v>
-      </c>
-      <c r="LB2">
-        <v>99.66</v>
-      </c>
-      <c r="LC2">
-        <v>36.8</v>
-      </c>
-      <c r="LD2">
-        <v>24.99</v>
-      </c>
-      <c r="LE2">
-        <v>77.81</v>
-      </c>
-      <c r="LF2">
-        <v>180.53</v>
-      </c>
-      <c r="LG2">
-        <v>25.11</v>
-      </c>
-      <c r="LH2">
-        <v>184.75</v>
-      </c>
-      <c r="LI2">
-        <v>18.23</v>
-      </c>
-      <c r="LJ2">
-        <v>47.58</v>
-      </c>
-      <c r="LK2">
-        <v>89.62</v>
-      </c>
-      <c r="LL2">
-        <v>22.07</v>
-      </c>
-      <c r="LM2">
-        <v>36.4</v>
-      </c>
-      <c r="LN2">
-        <v>43.86</v>
-      </c>
-      <c r="LO2">
-        <v>107.37</v>
-      </c>
-      <c r="LP2">
-        <v>60.9</v>
-      </c>
-      <c r="LQ2">
-        <v>58.23</v>
-      </c>
-      <c r="LR2">
-        <v>103.69</v>
-      </c>
-      <c r="LS2">
-        <v>49.78</v>
-      </c>
-      <c r="LT2">
-        <v>76.56</v>
-      </c>
-      <c r="LU2">
-        <v>289.69</v>
-      </c>
-      <c r="LV2">
-        <v>30.51</v>
-      </c>
-      <c r="LW2">
-        <v>19.19</v>
-      </c>
-      <c r="LX2">
-        <v>152.51</v>
-      </c>
-      <c r="LY2">
-        <v>82.06</v>
-      </c>
-      <c r="LZ2">
-        <v>26.17</v>
-      </c>
-      <c r="MA2">
-        <v>15.79</v>
-      </c>
-      <c r="MB2">
-        <v>57.48</v>
-      </c>
-      <c r="MC2">
-        <v>76.41</v>
-      </c>
-      <c r="MD2">
-        <v>364.35</v>
-      </c>
-      <c r="ME2">
-        <v>103.59</v>
-      </c>
-      <c r="MF2">
-        <v>26.08</v>
-      </c>
-      <c r="MG2">
-        <v>57.84</v>
-      </c>
-      <c r="MH2">
-        <v>22.38</v>
-      </c>
-      <c r="MI2">
-        <v>403.12</v>
-      </c>
-      <c r="MJ2">
-        <v>39.61</v>
-      </c>
       <c r="MK2">
-        <v>465.51</v>
+        <v>462.22</v>
       </c>
       <c r="ML2">
-        <v>13.24</v>
+        <v>12.66</v>
       </c>
       <c r="MM2">
-        <v>56.6</v>
+        <v>53.23</v>
       </c>
       <c r="MN2">
-        <v>556.24</v>
+        <v>544.0700000000001</v>
       </c>
       <c r="MO2">
-        <v>66.98</v>
+        <v>65.59</v>
       </c>
       <c r="MP2">
-        <v>77.13</v>
+        <v>77.7</v>
       </c>
       <c r="MQ2">
-        <v>35.75</v>
+        <v>35.26</v>
       </c>
       <c r="MR2">
         <v>21.34</v>
       </c>
       <c r="MS2">
-        <v>13.29</v>
+        <v>13.22</v>
       </c>
       <c r="MT2">
-        <v>27.05</v>
+        <v>26.5</v>
       </c>
       <c r="MU2">
-        <v>254.71</v>
+        <v>281.95</v>
       </c>
       <c r="MV2">
-        <v>26.4</v>
+        <v>26.29</v>
       </c>
       <c r="MW2">
-        <v>284.72</v>
+        <v>281.39</v>
       </c>
       <c r="MX2">
-        <v>167.95</v>
+        <v>165.45</v>
       </c>
       <c r="MY2">
-        <v>113.75</v>
+        <v>112.69</v>
       </c>
       <c r="MZ2">
-        <v>485.52</v>
+        <v>479.92</v>
       </c>
       <c r="NA2">
-        <v>13.51</v>
+        <v>13.23</v>
       </c>
       <c r="NB2">
-        <v>181.04</v>
+        <v>175.97</v>
       </c>
       <c r="NC2">
-        <v>19.32</v>
+        <v>18.91</v>
       </c>
       <c r="ND2">
-        <v>181.46</v>
+        <v>172.42</v>
       </c>
       <c r="NE2">
-        <v>186.55</v>
+        <v>175.67</v>
       </c>
       <c r="NF2">
-        <v>69.34</v>
+        <v>68.42</v>
       </c>
       <c r="NG2">
-        <v>39.84</v>
+        <v>39.49</v>
       </c>
       <c r="NH2">
-        <v>10.69</v>
+        <v>10.23</v>
       </c>
       <c r="NI2">
-        <v>10.53</v>
+        <v>10.15</v>
       </c>
       <c r="NJ2">
-        <v>78.26000000000001</v>
+        <v>75.77</v>
       </c>
       <c r="NK2">
-        <v>96.59</v>
+        <v>92.87</v>
       </c>
       <c r="NL2">
-        <v>312.13</v>
+        <v>312.21</v>
       </c>
       <c r="NM2">
-        <v>43.28</v>
+        <v>42.13</v>
       </c>
       <c r="NN2">
-        <v>41.8</v>
+        <v>40.46</v>
       </c>
       <c r="NO2">
-        <v>104.18</v>
+        <v>100.97</v>
       </c>
       <c r="NP2">
-        <v>48</v>
+        <v>48.57</v>
       </c>
       <c r="NQ2">
-        <v>42.65</v>
+        <v>42.17</v>
       </c>
       <c r="NR2">
-        <v>45.27</v>
+        <v>41.93</v>
       </c>
       <c r="NS2">
-        <v>36.14</v>
+        <v>36.16</v>
       </c>
       <c r="NT2">
-        <v>53.3</v>
+        <v>50.66</v>
       </c>
       <c r="NU2">
-        <v>149.1</v>
+        <v>144.41</v>
       </c>
       <c r="NV2">
-        <v>29</v>
+        <v>28.33</v>
       </c>
       <c r="NW2">
-        <v>33.54</v>
+        <v>33.69</v>
       </c>
       <c r="NX2">
-        <v>31.71</v>
+        <v>30.08</v>
       </c>
       <c r="NY2">
-        <v>436.57</v>
+        <v>430.72</v>
       </c>
       <c r="NZ2">
-        <v>35.12</v>
+        <v>35.2</v>
       </c>
       <c r="OA2">
-        <v>76.88</v>
+        <v>75.72</v>
       </c>
       <c r="OB2">
-        <v>213</v>
+        <v>204.54</v>
       </c>
       <c r="OC2">
-        <v>82.08</v>
+        <v>80.45999999999999</v>
       </c>
       <c r="OD2">
-        <v>124.94</v>
+        <v>124.86</v>
       </c>
       <c r="OE2">
-        <v>62.01</v>
+        <v>60.03</v>
       </c>
       <c r="OF2">
-        <v>67.54000000000001</v>
+        <v>65.48</v>
       </c>
       <c r="OG2">
-        <v>18.68</v>
+        <v>18.34</v>
       </c>
       <c r="OH2">
-        <v>36.2</v>
+        <v>36.12</v>
       </c>
       <c r="OI2">
-        <v>44.4</v>
+        <v>44.7</v>
       </c>
       <c r="OJ2">
-        <v>150.67</v>
+        <v>147.79</v>
       </c>
       <c r="OK2">
-        <v>34.72</v>
+        <v>34.75</v>
       </c>
       <c r="OL2">
-        <v>28.62</v>
+        <v>27.53</v>
       </c>
       <c r="OM2">
-        <v>23.5</v>
+        <v>23.28</v>
       </c>
       <c r="ON2">
-        <v>24.15</v>
+        <v>23.22</v>
       </c>
       <c r="OO2">
-        <v>23.28</v>
+        <v>22.92</v>
       </c>
       <c r="OP2">
-        <v>47.22</v>
+        <v>46.68</v>
       </c>
       <c r="OQ2">
-        <v>183.31</v>
+        <v>187.54</v>
       </c>
       <c r="OR2">
-        <v>113.76</v>
+        <v>112.67</v>
       </c>
       <c r="OS2">
-        <v>38.97</v>
+        <v>38.64</v>
       </c>
       <c r="OT2">
         <v>36.24</v>
       </c>
       <c r="OU2">
-        <v>67.73999999999999</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="OV2">
-        <v>73.65000000000001</v>
+        <v>72.15000000000001</v>
       </c>
       <c r="OW2">
         <v>0.02</v>
       </c>
       <c r="OX2">
-        <v>45.28</v>
+        <v>43.07</v>
       </c>
       <c r="OY2">
-        <v>299.93</v>
+        <v>291.54</v>
       </c>
       <c r="OZ2">
-        <v>182.92</v>
+        <v>180.4</v>
       </c>
       <c r="PA2">
-        <v>124.86</v>
+        <v>123.95</v>
       </c>
       <c r="PB2">
-        <v>94.34</v>
+        <v>94.23</v>
       </c>
       <c r="PC2">
-        <v>134.45</v>
+        <v>131.55</v>
       </c>
       <c r="PD2">
-        <v>472.7</v>
+        <v>463.18</v>
       </c>
       <c r="PE2">
-        <v>65.23</v>
+        <v>64.06</v>
       </c>
       <c r="PF2">
-        <v>154.65</v>
+        <v>151.62</v>
       </c>
       <c r="PG2">
-        <v>60.96</v>
+        <v>58.73</v>
       </c>
       <c r="PH2">
-        <v>109.04</v>
+        <v>102.88</v>
       </c>
       <c r="PI2">
-        <v>95.89</v>
+        <v>95.17</v>
       </c>
       <c r="PJ2">
-        <v>53.16</v>
+        <v>52.99</v>
       </c>
       <c r="PK2">
-        <v>723.73</v>
+        <v>726.24</v>
       </c>
       <c r="PL2">
-        <v>23.26</v>
+        <v>22.46</v>
       </c>
       <c r="PM2">
-        <v>85.19</v>
+        <v>83.39</v>
       </c>
       <c r="PN2">
-        <v>9.460000000000001</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="PO2">
-        <v>129.78</v>
+        <v>126.32</v>
       </c>
       <c r="PP2">
-        <v>18.27</v>
+        <v>17.48</v>
       </c>
       <c r="PQ2">
-        <v>257.85</v>
+        <v>255.31</v>
       </c>
       <c r="PR2">
-        <v>21.84</v>
+        <v>21.93</v>
       </c>
       <c r="PS2">
-        <v>15.25</v>
+        <v>15.22</v>
       </c>
       <c r="PT2">
-        <v>37</v>
+        <v>36.67</v>
       </c>
       <c r="PU2">
-        <v>228.53</v>
+        <v>226.49</v>
       </c>
       <c r="PV2">
-        <v>39.94</v>
+        <v>40.05</v>
       </c>
       <c r="PW2">
-        <v>42.11</v>
+        <v>41.51</v>
       </c>
       <c r="PX2">
-        <v>96.92</v>
+        <v>98.22</v>
       </c>
       <c r="PY2">
-        <v>147.2</v>
+        <v>146.03</v>
       </c>
       <c r="PZ2">
-        <v>36.35</v>
+        <v>36.53</v>
       </c>
       <c r="QA2">
-        <v>59.09</v>
+        <v>57.34</v>
       </c>
       <c r="QB2">
-        <v>12.67</v>
+        <v>13.16</v>
       </c>
       <c r="QC2">
-        <v>120.78</v>
+        <v>118.52</v>
       </c>
       <c r="QD2">
-        <v>143.65</v>
+        <v>139.81</v>
       </c>
       <c r="QE2">
-        <v>33.56</v>
+        <v>33.76</v>
       </c>
       <c r="QF2">
-        <v>19.26</v>
+        <v>18.24</v>
       </c>
       <c r="QG2">
-        <v>120.81</v>
+        <v>115.1</v>
       </c>
       <c r="QH2">
-        <v>35.58</v>
+        <v>35.03</v>
       </c>
       <c r="QI2">
-        <v>19.69</v>
+        <v>18.7</v>
       </c>
       <c r="QJ2">
-        <v>57.87</v>
+        <v>56.51</v>
       </c>
       <c r="QK2">
-        <v>26.58</v>
+        <v>25.66</v>
       </c>
       <c r="QL2">
-        <v>13.14</v>
+        <v>13.23</v>
       </c>
       <c r="QM2">
-        <v>75.27</v>
+        <v>74.62</v>
       </c>
       <c r="QN2">
-        <v>81.61</v>
+        <v>79.17</v>
       </c>
       <c r="QO2">
-        <v>24.78</v>
+        <v>23.93</v>
       </c>
       <c r="QP2">
-        <v>13.91</v>
+        <v>13.81</v>
       </c>
       <c r="QQ2">
-        <v>531.0599999999999</v>
+        <v>519.95</v>
       </c>
       <c r="QR2">
-        <v>100.92</v>
+        <v>100.31</v>
       </c>
       <c r="QS2">
-        <v>82.37</v>
+        <v>83.11</v>
       </c>
       <c r="QT2">
-        <v>33.43</v>
+        <v>31.57</v>
       </c>
       <c r="QU2">
-        <v>94.52</v>
+        <v>89.76000000000001</v>
       </c>
       <c r="QV2">
-        <v>100.08</v>
+        <v>96.79000000000001</v>
       </c>
       <c r="QW2">
-        <v>46.36</v>
+        <v>46</v>
       </c>
       <c r="QX2">
-        <v>45.69</v>
+        <v>44.09</v>
       </c>
       <c r="QY2">
-        <v>62.2</v>
+        <v>60.25</v>
       </c>
       <c r="QZ2">
-        <v>28.21</v>
+        <v>28.56</v>
       </c>
       <c r="RA2">
-        <v>19.75</v>
+        <v>19.18</v>
       </c>
       <c r="RB2">
-        <v>141.92</v>
+        <v>137.27</v>
       </c>
       <c r="RC2">
-        <v>41.95</v>
+        <v>41.98</v>
       </c>
       <c r="RD2">
-        <v>71.91</v>
+        <v>71.95</v>
       </c>
       <c r="RE2">
-        <v>77.06999999999999</v>
+        <v>76.14</v>
       </c>
       <c r="RF2">
-        <v>46.49</v>
+        <v>45.92</v>
       </c>
       <c r="RG2">
         <v>50.85</v>
       </c>
       <c r="RH2">
-        <v>506.56</v>
+        <v>506.97</v>
       </c>
       <c r="RI2">
-        <v>16.38</v>
+        <v>15.79</v>
       </c>
       <c r="RJ2">
-        <v>15.53</v>
+        <v>14.46</v>
       </c>
       <c r="RK2">
-        <v>22.83</v>
+        <v>22.82</v>
       </c>
       <c r="RL2">
-        <v>101.27</v>
+        <v>101.3</v>
       </c>
       <c r="RM2">
-        <v>68.17</v>
+        <v>65.56999999999999</v>
       </c>
       <c r="RN2">
-        <v>747.74</v>
+        <v>740.0700000000001</v>
       </c>
       <c r="RO2">
-        <v>41.14</v>
+        <v>39.93</v>
       </c>
       <c r="RP2">
-        <v>70.06</v>
+        <v>69.36</v>
       </c>
       <c r="RQ2">
-        <v>177.26</v>
+        <v>171.2</v>
       </c>
       <c r="RR2">
-        <v>180.62</v>
+        <v>174.64</v>
       </c>
       <c r="RS2">
-        <v>38.76</v>
+        <v>38.27</v>
       </c>
       <c r="RT2">
-        <v>26.74</v>
+        <v>26.65</v>
       </c>
       <c r="RU2">
-        <v>47.77</v>
+        <v>47.9</v>
       </c>
       <c r="RV2">
-        <v>70.25</v>
+        <v>68.48</v>
       </c>
       <c r="RW2">
-        <v>79.34</v>
+        <v>79.01000000000001</v>
       </c>
       <c r="RX2">
-        <v>24.5</v>
+        <v>23.86</v>
       </c>
       <c r="RY2">
+        <v>28.01</v>
+      </c>
+      <c r="RZ2">
+        <v>94.83</v>
+      </c>
+      <c r="SA2">
+        <v>49.2</v>
+      </c>
+      <c r="SB2">
+        <v>23.74</v>
+      </c>
+      <c r="SC2">
+        <v>36.76</v>
+      </c>
+      <c r="SD2">
+        <v>158.47</v>
+      </c>
+      <c r="SE2">
+        <v>55.69</v>
+      </c>
+      <c r="SF2">
+        <v>143.04</v>
+      </c>
+      <c r="SG2">
+        <v>26.99</v>
+      </c>
+      <c r="SH2">
+        <v>204.66</v>
+      </c>
+      <c r="SI2">
+        <v>37.15</v>
+      </c>
+      <c r="SJ2">
+        <v>23.2</v>
+      </c>
+      <c r="SK2">
+        <v>26.93</v>
+      </c>
+      <c r="SL2">
+        <v>56.52</v>
+      </c>
+      <c r="SM2">
+        <v>21.32</v>
+      </c>
+      <c r="SN2">
+        <v>170.96</v>
+      </c>
+      <c r="SO2">
+        <v>26.06</v>
+      </c>
+      <c r="SP2">
+        <v>20.87</v>
+      </c>
+      <c r="SQ2">
+        <v>158.93</v>
+      </c>
+      <c r="SR2">
+        <v>87.7</v>
+      </c>
+      <c r="SS2">
+        <v>78.92</v>
+      </c>
+      <c r="ST2">
+        <v>8.34</v>
+      </c>
+      <c r="SU2">
+        <v>141.59</v>
+      </c>
+      <c r="SV2">
+        <v>60.22</v>
+      </c>
+      <c r="SW2">
+        <v>53.39</v>
+      </c>
+      <c r="SX2">
+        <v>54.75</v>
+      </c>
+      <c r="SY2">
+        <v>16.07</v>
+      </c>
+      <c r="SZ2">
+        <v>108.36</v>
+      </c>
+      <c r="TA2">
+        <v>452.51</v>
+      </c>
+      <c r="TB2">
+        <v>103.19</v>
+      </c>
+      <c r="TC2">
+        <v>75.06999999999999</v>
+      </c>
+      <c r="TD2">
+        <v>93.17</v>
+      </c>
+      <c r="TE2">
+        <v>87.54000000000001</v>
+      </c>
+      <c r="TF2">
+        <v>23.27</v>
+      </c>
+      <c r="TG2">
+        <v>33.94</v>
+      </c>
+      <c r="TH2">
+        <v>52.48</v>
+      </c>
+      <c r="TI2">
+        <v>32.45</v>
+      </c>
+      <c r="TJ2">
+        <v>32.5</v>
+      </c>
+      <c r="TK2">
+        <v>240.46</v>
+      </c>
+      <c r="TL2">
+        <v>17.99</v>
+      </c>
+      <c r="TM2">
+        <v>73.75</v>
+      </c>
+      <c r="TN2">
+        <v>27.11</v>
+      </c>
+      <c r="TO2">
+        <v>26.47</v>
+      </c>
+      <c r="TP2">
+        <v>25.14</v>
+      </c>
+      <c r="TQ2">
+        <v>437.46</v>
+      </c>
+      <c r="TR2">
+        <v>14.65</v>
+      </c>
+      <c r="TS2">
+        <v>55.91</v>
+      </c>
+      <c r="TT2">
+        <v>160.48</v>
+      </c>
+      <c r="TU2">
+        <v>40.78</v>
+      </c>
+      <c r="TV2">
+        <v>66.75</v>
+      </c>
+      <c r="TW2">
+        <v>24.6</v>
+      </c>
+      <c r="TX2">
+        <v>106.6</v>
+      </c>
+      <c r="TY2">
+        <v>82.66</v>
+      </c>
+      <c r="TZ2">
+        <v>45.66</v>
+      </c>
+      <c r="UA2">
+        <v>148.34</v>
+      </c>
+      <c r="UB2">
+        <v>37.11</v>
+      </c>
+      <c r="UC2">
+        <v>13.44</v>
+      </c>
+      <c r="UD2">
+        <v>161.86</v>
+      </c>
+      <c r="UE2">
+        <v>30.53</v>
+      </c>
+      <c r="UF2">
+        <v>292.74</v>
+      </c>
+      <c r="UG2">
         <v>28.21</v>
       </c>
-      <c r="RZ2">
-        <v>98.20999999999999</v>
-      </c>
-      <c r="SA2">
-        <v>53.38</v>
-      </c>
-      <c r="SB2">
-        <v>24.1</v>
-      </c>
-      <c r="SC2">
-        <v>36.42</v>
-      </c>
-      <c r="SD2">
-        <v>161.51</v>
-      </c>
-      <c r="SE2">
-        <v>55.17</v>
-      </c>
-      <c r="SF2">
-        <v>145.45</v>
-      </c>
-      <c r="SG2">
-        <v>27.06</v>
-      </c>
-      <c r="SH2">
-        <v>213.39</v>
-      </c>
-      <c r="SI2">
-        <v>38.72</v>
-      </c>
-      <c r="SJ2">
-        <v>23.04</v>
-      </c>
-      <c r="SK2">
-        <v>27.41</v>
-      </c>
-      <c r="SL2">
-        <v>57.19</v>
-      </c>
-      <c r="SM2">
-        <v>21.24</v>
-      </c>
-      <c r="SN2">
-        <v>172.59</v>
-      </c>
-      <c r="SO2">
-        <v>26.8</v>
-      </c>
-      <c r="SP2">
-        <v>22.08</v>
-      </c>
-      <c r="SQ2">
-        <v>161.6</v>
-      </c>
-      <c r="SR2">
-        <v>92.02</v>
-      </c>
-      <c r="SS2">
-        <v>79.78</v>
-      </c>
-      <c r="ST2">
-        <v>9.1</v>
-      </c>
-      <c r="SU2">
-        <v>144.14</v>
-      </c>
-      <c r="SV2">
-        <v>61.9</v>
-      </c>
-      <c r="SW2">
-        <v>53.77</v>
-      </c>
-      <c r="SX2">
-        <v>54.66</v>
-      </c>
-      <c r="SY2">
-        <v>16.42</v>
-      </c>
-      <c r="SZ2">
-        <v>109.17</v>
-      </c>
-      <c r="TA2">
-        <v>459.82</v>
-      </c>
-      <c r="TB2">
-        <v>105.52</v>
-      </c>
-      <c r="TC2">
-        <v>80</v>
-      </c>
-      <c r="TD2">
-        <v>90.02</v>
-      </c>
-      <c r="TE2">
-        <v>88.12</v>
-      </c>
-      <c r="TF2">
-        <v>24.51</v>
-      </c>
-      <c r="TG2">
-        <v>34.31</v>
-      </c>
-      <c r="TH2">
-        <v>56.54</v>
-      </c>
-      <c r="TI2">
-        <v>33.19</v>
-      </c>
-      <c r="TJ2">
-        <v>33.57</v>
-      </c>
-      <c r="TK2">
-        <v>250.83</v>
-      </c>
-      <c r="TL2">
-        <v>18.7</v>
-      </c>
-      <c r="TM2">
-        <v>76.45</v>
-      </c>
-      <c r="TN2">
-        <v>27.25</v>
-      </c>
-      <c r="TO2">
-        <v>26.78</v>
-      </c>
-      <c r="TP2">
-        <v>26.58</v>
-      </c>
-      <c r="TQ2">
-        <v>440.45</v>
-      </c>
-      <c r="TR2">
-        <v>14.75</v>
-      </c>
-      <c r="TS2">
-        <v>56.33</v>
-      </c>
-      <c r="TT2">
-        <v>161.73</v>
-      </c>
-      <c r="TU2">
-        <v>40.76</v>
-      </c>
-      <c r="TV2">
-        <v>67.17</v>
-      </c>
-      <c r="TW2">
-        <v>25.04</v>
-      </c>
-      <c r="TX2">
-        <v>112.84</v>
-      </c>
-      <c r="TY2">
-        <v>85.67</v>
-      </c>
-      <c r="TZ2">
-        <v>45.1</v>
-      </c>
-      <c r="UA2">
-        <v>151.41</v>
-      </c>
-      <c r="UB2">
-        <v>37.16</v>
-      </c>
-      <c r="UC2">
-        <v>13.93</v>
-      </c>
-      <c r="UD2">
-        <v>164.39</v>
-      </c>
-      <c r="UE2">
-        <v>31.44</v>
-      </c>
-      <c r="UF2">
-        <v>287.97</v>
-      </c>
-      <c r="UG2">
-        <v>28.53</v>
-      </c>
       <c r="UH2">
-        <v>73.27</v>
+        <v>71.95999999999999</v>
       </c>
       <c r="UI2">
-        <v>109.03</v>
+        <v>104.96</v>
       </c>
       <c r="UJ2">
-        <v>62.52</v>
+        <v>61.82</v>
       </c>
       <c r="UK2">
-        <v>9.92</v>
+        <v>10.06</v>
       </c>
       <c r="UL2">
-        <v>21.27</v>
+        <v>21.06</v>
       </c>
       <c r="UM2">
-        <v>21.4</v>
+        <v>21.07</v>
       </c>
       <c r="UN2">
-        <v>889.4299999999999</v>
+        <v>884.02</v>
       </c>
       <c r="UO2">
-        <v>119.23</v>
+        <v>114.62</v>
       </c>
       <c r="UP2">
-        <v>46.79</v>
+        <v>45.08</v>
       </c>
       <c r="UQ2">
-        <v>14.08</v>
+        <v>14.16</v>
       </c>
       <c r="UR2">
-        <v>180.86</v>
+        <v>173.63</v>
       </c>
       <c r="US2">
-        <v>132.85</v>
+        <v>128.96</v>
       </c>
       <c r="UT2">
-        <v>157.65</v>
+        <v>156.58</v>
       </c>
       <c r="UU2">
-        <v>150.98</v>
+        <v>146.87</v>
       </c>
       <c r="UV2">
-        <v>15.92</v>
+        <v>15.71</v>
       </c>
       <c r="UW2">
-        <v>301.01</v>
+        <v>302.06</v>
       </c>
       <c r="UX2">
-        <v>144.93</v>
+        <v>141.38</v>
       </c>
       <c r="UY2">
-        <v>23.57</v>
+        <v>22.76</v>
       </c>
       <c r="UZ2">
-        <v>488.62</v>
+        <v>455.19</v>
       </c>
       <c r="VA2">
-        <v>75.09</v>
+        <v>73.84</v>
       </c>
       <c r="VB2">
-        <v>31.54</v>
+        <v>28.87</v>
       </c>
       <c r="VC2">
-        <v>14.91</v>
+        <v>14.78</v>
       </c>
       <c r="VD2">
-        <v>37.49</v>
+        <v>37.45</v>
       </c>
       <c r="VE2">
         <v>35.05</v>
       </c>
       <c r="VF2">
-        <v>72.31999999999999</v>
+        <v>71.03</v>
       </c>
       <c r="VG2">
-        <v>25.9</v>
+        <v>26.97</v>
       </c>
       <c r="VH2">
-        <v>59.03</v>
+        <v>56.27</v>
       </c>
       <c r="VI2">
-        <v>36.12</v>
+        <v>35.23</v>
       </c>
       <c r="VJ2">
-        <v>134.12</v>
+        <v>126.65</v>
       </c>
       <c r="VK2">
-        <v>245.2</v>
+        <v>245.05</v>
       </c>
       <c r="VL2">
-        <v>17.99</v>
+        <v>17</v>
       </c>
       <c r="VM2">
-        <v>142.92</v>
+        <v>142.99</v>
       </c>
       <c r="VN2">
-        <v>78.51000000000001</v>
+        <v>76.48999999999999</v>
       </c>
       <c r="VO2">
-        <v>28.61</v>
+        <v>26.8</v>
       </c>
       <c r="VP2">
-        <v>52.12</v>
+        <v>48.03</v>
       </c>
       <c r="VQ2">
-        <v>96.14</v>
+        <v>92.02</v>
       </c>
       <c r="VR2">
-        <v>45.87</v>
+        <v>45.37</v>
       </c>
       <c r="VS2">
-        <v>33.37</v>
+        <v>33.24</v>
       </c>
       <c r="VT2">
-        <v>29.76</v>
+        <v>29.41</v>
       </c>
       <c r="VU2">
-        <v>128.35</v>
+        <v>126.1</v>
       </c>
       <c r="VV2">
-        <v>83.2</v>
+        <v>81.16</v>
       </c>
       <c r="VW2">
-        <v>221</v>
+        <v>221.71</v>
       </c>
       <c r="VX2">
-        <v>38.61</v>
+        <v>38.55</v>
       </c>
       <c r="VY2">
-        <v>60.31</v>
+        <v>59.75</v>
       </c>
       <c r="VZ2">
-        <v>54.85</v>
+        <v>54.33</v>
       </c>
       <c r="WA2">
-        <v>55.28</v>
+        <v>55.2</v>
       </c>
       <c r="WB2">
-        <v>32.19</v>
+        <v>31.11</v>
       </c>
       <c r="WC2">
-        <v>45.05</v>
+        <v>43.65</v>
       </c>
       <c r="WD2">
-        <v>437.87</v>
+        <v>419.31</v>
       </c>
       <c r="WE2">
-        <v>47.53</v>
+        <v>46.88</v>
       </c>
       <c r="WF2">
-        <v>14.2</v>
+        <v>13.92</v>
       </c>
       <c r="WG2">
-        <v>25.37</v>
+        <v>25.21</v>
       </c>
       <c r="WH2">
-        <v>91.89</v>
+        <v>89.93000000000001</v>
       </c>
       <c r="WI2">
-        <v>41.54</v>
+        <v>40.42</v>
       </c>
       <c r="WJ2">
-        <v>29.83</v>
+        <v>29.48</v>
       </c>
       <c r="WK2">
-        <v>89.40000000000001</v>
+        <v>89.5</v>
       </c>
       <c r="WL2">
-        <v>31.2</v>
+        <v>32.03</v>
       </c>
       <c r="WM2">
-        <v>111.06</v>
+        <v>110.79</v>
       </c>
       <c r="WN2">
-        <v>32.71</v>
+        <v>31.18</v>
       </c>
       <c r="WO2">
-        <v>264.08</v>
+        <v>254.34</v>
       </c>
       <c r="WP2">
-        <v>17.21</v>
+        <v>16.8</v>
       </c>
       <c r="WQ2">
-        <v>29.23</v>
+        <v>27.65</v>
       </c>
       <c r="WR2">
-        <v>163.29</v>
+        <v>153.5</v>
       </c>
       <c r="WS2">
-        <v>54.95</v>
+        <v>54.27</v>
       </c>
       <c r="WT2">
-        <v>21.8</v>
+        <v>21.29</v>
       </c>
       <c r="WU2">
         <v>36.55</v>
       </c>
       <c r="WV2">
-        <v>16.6</v>
+        <v>16.24</v>
       </c>
       <c r="WW2">
-        <v>39.04</v>
+        <v>36.25</v>
       </c>
       <c r="WX2">
-        <v>77.53</v>
+        <v>76.17</v>
       </c>
       <c r="WY2">
-        <v>26.26</v>
+        <v>25.26</v>
       </c>
       <c r="WZ2">
-        <v>13.18</v>
+        <v>12.8</v>
       </c>
       <c r="XA2">
-        <v>44.86</v>
+        <v>43.98</v>
       </c>
       <c r="XB2">
-        <v>61.19</v>
+        <v>59.52</v>
       </c>
       <c r="XC2">
-        <v>16.84</v>
+        <v>17</v>
       </c>
       <c r="XD2">
-        <v>29.34</v>
+        <v>28.45</v>
       </c>
       <c r="XE2">
-        <v>40.61</v>
+        <v>39.93</v>
       </c>
       <c r="XF2">
-        <v>124.53</v>
+        <v>119.25</v>
       </c>
       <c r="XG2">
-        <v>102.69</v>
+        <v>102.19</v>
       </c>
       <c r="XH2">
-        <v>48.73</v>
+        <v>46.53</v>
       </c>
       <c r="XI2">
-        <v>278.09</v>
+        <v>277.03</v>
       </c>
       <c r="XJ2">
-        <v>58.63</v>
+        <v>56.7</v>
       </c>
       <c r="XK2">
-        <v>21.8</v>
+        <v>21.5</v>
       </c>
       <c r="XL2">
-        <v>132.9</v>
+        <v>133.36</v>
       </c>
       <c r="XM2">
-        <v>24.56</v>
+        <v>23.65</v>
       </c>
       <c r="XN2">
-        <v>42.2</v>
+        <v>41.81</v>
       </c>
       <c r="XO2">
-        <v>188.98</v>
+        <v>186.58</v>
       </c>
       <c r="XP2">
-        <v>15.48</v>
+        <v>15.19</v>
       </c>
       <c r="XQ2">
-        <v>13.28</v>
+        <v>13</v>
       </c>
       <c r="XR2">
-        <v>16.78</v>
+        <v>16.42</v>
       </c>
       <c r="XS2">
-        <v>30.63</v>
+        <v>30.48</v>
       </c>
       <c r="XT2">
-        <v>31.18</v>
+        <v>30.93</v>
       </c>
       <c r="XU2">
-        <v>31.03</v>
+        <v>30.85</v>
       </c>
       <c r="XV2">
-        <v>98.41</v>
+        <v>97.28</v>
       </c>
       <c r="XW2">
-        <v>52.78</v>
+        <v>52.91</v>
       </c>
       <c r="XX2">
-        <v>350.48</v>
+        <v>354.26</v>
       </c>
       <c r="XY2">
-        <v>15.45</v>
+        <v>14.55</v>
       </c>
       <c r="XZ2">
-        <v>27.34</v>
+        <v>26.74</v>
       </c>
       <c r="YA2">
-        <v>22.52</v>
+        <v>22.43</v>
       </c>
       <c r="YB2">
-        <v>37.53</v>
+        <v>35.05</v>
       </c>
       <c r="YC2">
-        <v>84.67</v>
+        <v>84.41</v>
       </c>
       <c r="YD2">
-        <v>8.92</v>
+        <v>8.57</v>
       </c>
       <c r="YE2">
-        <v>124.73</v>
+        <v>123.21</v>
       </c>
       <c r="YF2">
-        <v>71.38</v>
+        <v>70.68000000000001</v>
       </c>
       <c r="YG2">
-        <v>458.22</v>
+        <v>465.31</v>
       </c>
       <c r="YH2">
-        <v>62.16</v>
+        <v>61</v>
       </c>
       <c r="YI2">
-        <v>20.55</v>
+        <v>20.21</v>
       </c>
       <c r="YJ2">
-        <v>153.33</v>
+        <v>151.41</v>
       </c>
       <c r="YK2">
-        <v>44.53</v>
+        <v>43.81</v>
       </c>
       <c r="YL2">
-        <v>29.92</v>
+        <v>29.61</v>
       </c>
       <c r="YM2">
-        <v>214.43</v>
+        <v>208.57</v>
       </c>
       <c r="YN2">
-        <v>6.9</v>
+        <v>6.77</v>
       </c>
       <c r="YO2">
-        <v>6.32</v>
+        <v>5.84</v>
       </c>
       <c r="YP2">
-        <v>48.55</v>
+        <v>47.45</v>
       </c>
       <c r="YQ2">
-        <v>56.83</v>
+        <v>55.55</v>
       </c>
       <c r="YR2">
-        <v>25.99</v>
+        <v>24.99</v>
       </c>
       <c r="YS2">
-        <v>56.08</v>
+        <v>52.22</v>
       </c>
       <c r="YT2">
-        <v>20.21</v>
+        <v>19.53</v>
       </c>
       <c r="YU2">
-        <v>55.57</v>
+        <v>55.52</v>
       </c>
       <c r="YV2">
-        <v>19.86</v>
+        <v>20</v>
       </c>
       <c r="YW2">
-        <v>40.66</v>
+        <v>39.2</v>
       </c>
       <c r="YX2">
-        <v>94.52</v>
+        <v>90.5</v>
       </c>
       <c r="YY2">
-        <v>67.38</v>
+        <v>66.47</v>
       </c>
       <c r="YZ2">
-        <v>46.2</v>
+        <v>46.75</v>
       </c>
       <c r="ZA2">
-        <v>57.67</v>
+        <v>56.21</v>
       </c>
       <c r="ZB2">
-        <v>97.54000000000001</v>
+        <v>94.51000000000001</v>
       </c>
       <c r="ZC2">
-        <v>53.06</v>
+        <v>46.05</v>
       </c>
       <c r="ZD2">
-        <v>77.56</v>
+        <v>74.33</v>
       </c>
       <c r="ZE2">
-        <v>15.52</v>
+        <v>15.95</v>
       </c>
       <c r="ZF2">
-        <v>75.31999999999999</v>
+        <v>75.48</v>
       </c>
       <c r="ZG2">
-        <v>8.33</v>
+        <v>8.16</v>
       </c>
       <c r="ZH2">
-        <v>119.13</v>
+        <v>120.03</v>
       </c>
       <c r="ZI2">
-        <v>13.72</v>
+        <v>13.24</v>
       </c>
       <c r="ZJ2">
-        <v>33.6</v>
+        <v>33.57</v>
       </c>
       <c r="ZK2">
-        <v>25.62</v>
+        <v>25.49</v>
       </c>
       <c r="ZL2">
-        <v>36.01</v>
+        <v>35.79</v>
       </c>
       <c r="ZM2">
-        <v>87.23999999999999</v>
+        <v>85.90000000000001</v>
       </c>
       <c r="ZN2">
-        <v>102.87</v>
+        <v>101.96</v>
       </c>
       <c r="ZO2">
-        <v>14.12</v>
+        <v>13.87</v>
       </c>
       <c r="ZP2">
-        <v>7.55</v>
+        <v>7.22</v>
       </c>
       <c r="ZQ2">
-        <v>39.3</v>
+        <v>39.23</v>
       </c>
       <c r="ZR2">
-        <v>23.6</v>
+        <v>23.06</v>
       </c>
       <c r="ZS2">
-        <v>16.97</v>
+        <v>16.36</v>
       </c>
       <c r="ZT2">
-        <v>51.44</v>
+        <v>51.28</v>
       </c>
       <c r="ZU2">
-        <v>8.35</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="ZV2">
-        <v>263.86</v>
+        <v>264.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed the Overview page with all the financial statements displayed
</commit_message>
<xml_diff>
--- a/outData/FilledPriceDaily.xlsx
+++ b/outData/FilledPriceDaily.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="695">
   <si>
     <t>GPC</t>
   </si>
@@ -403,9 +403,6 @@
     <t>WLY</t>
   </si>
   <si>
-    <t>WLYB</t>
-  </si>
-  <si>
     <t>ALRS</t>
   </si>
   <si>
@@ -1777,18 +1774,12 @@
     <t>DVN</t>
   </si>
   <si>
-    <t>IIPR</t>
-  </si>
-  <si>
     <t>PHM</t>
   </si>
   <si>
     <t>NYT</t>
   </si>
   <si>
-    <t>MBIN</t>
-  </si>
-  <si>
     <t>VICI</t>
   </si>
   <si>
@@ -2074,12 +2065,6 @@
     <t>KDP</t>
   </si>
   <si>
-    <t>MCBS</t>
-  </si>
-  <si>
-    <t>BSVN</t>
-  </si>
-  <si>
     <t>NRG</t>
   </si>
   <si>
@@ -2113,7 +2098,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-09</t>
+    <t>2025-04-11</t>
   </si>
 </sst>
 </file>
@@ -2471,15 +2456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ZW2"/>
+  <dimension ref="A1:ZR2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:699">
+    <row r="1" spans="1:694">
       <c r="A1" s="1" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4560,2119 +4545,2089 @@
       <c r="ZR1" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="ZS1" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="ZT1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:694">
+      <c r="A2" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="ZU1" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="ZV1" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="ZW1" s="1" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="2" spans="1:699">
-      <c r="A2" s="1" t="s">
-        <v>699</v>
-      </c>
       <c r="B2">
-        <v>113.98</v>
+        <v>115.25</v>
       </c>
       <c r="C2">
-        <v>90.16</v>
+        <v>88.73999999999999</v>
       </c>
       <c r="D2">
-        <v>462.24</v>
+        <v>474.9</v>
       </c>
       <c r="E2">
-        <v>75.09999999999999</v>
+        <v>78.23</v>
       </c>
       <c r="F2">
-        <v>165.86</v>
+        <v>162.11</v>
       </c>
       <c r="G2">
-        <v>40.4</v>
+        <v>41.26</v>
       </c>
       <c r="H2">
-        <v>162.32</v>
+        <v>166.91</v>
       </c>
       <c r="I2">
-        <v>596.1</v>
+        <v>565.37</v>
       </c>
       <c r="J2">
-        <v>104.43</v>
+        <v>100.49</v>
       </c>
       <c r="K2">
-        <v>134.63</v>
+        <v>131.09</v>
       </c>
       <c r="L2">
-        <v>223.2</v>
+        <v>220.35</v>
       </c>
       <c r="M2">
-        <v>150.97</v>
+        <v>151.73</v>
       </c>
       <c r="N2">
-        <v>69.95</v>
+        <v>71.43000000000001</v>
       </c>
       <c r="O2">
-        <v>181.26</v>
+        <v>183.76</v>
       </c>
       <c r="P2">
-        <v>187.29</v>
+        <v>185.56</v>
       </c>
       <c r="Q2">
-        <v>234.87</v>
+        <v>232.32</v>
       </c>
       <c r="R2">
-        <v>90.23</v>
+        <v>94</v>
       </c>
       <c r="S2">
-        <v>30.32</v>
+        <v>30.96</v>
       </c>
       <c r="T2">
-        <v>29.71</v>
+        <v>30.31</v>
       </c>
       <c r="U2">
-        <v>45.3</v>
+        <v>46.11</v>
       </c>
       <c r="V2">
-        <v>97.69</v>
+        <v>92.78</v>
       </c>
       <c r="W2">
-        <v>64.22</v>
+        <v>59.01</v>
       </c>
       <c r="X2">
-        <v>47.81</v>
+        <v>50.34</v>
       </c>
       <c r="Y2">
-        <v>90.38</v>
+        <v>90.26000000000001</v>
       </c>
       <c r="Z2">
-        <v>50.95</v>
+        <v>53.42</v>
       </c>
       <c r="AA2">
-        <v>49.69</v>
+        <v>48.07</v>
       </c>
       <c r="AB2">
-        <v>58.73</v>
+        <v>56.88</v>
       </c>
       <c r="AC2">
-        <v>53.78</v>
+        <v>53.73</v>
       </c>
       <c r="AD2">
-        <v>56.36</v>
+        <v>56.65</v>
       </c>
       <c r="AE2">
-        <v>74.59999999999999</v>
+        <v>76.45999999999999</v>
       </c>
       <c r="AF2">
-        <v>57.99</v>
+        <v>58.36</v>
       </c>
       <c r="AG2">
-        <v>71.06999999999999</v>
+        <v>70.43000000000001</v>
       </c>
       <c r="AH2">
-        <v>53.09</v>
+        <v>52.73</v>
       </c>
       <c r="AI2">
-        <v>965.37</v>
+        <v>994</v>
       </c>
       <c r="AJ2">
+        <v>144.19</v>
+      </c>
+      <c r="AK2">
+        <v>100.73</v>
+      </c>
+      <c r="AL2">
+        <v>71.12</v>
+      </c>
+      <c r="AM2">
+        <v>144.43</v>
+      </c>
+      <c r="AN2">
+        <v>201.78</v>
+      </c>
+      <c r="AO2">
+        <v>139.76</v>
+      </c>
+      <c r="AP2">
+        <v>465.14</v>
+      </c>
+      <c r="AQ2">
+        <v>111.24</v>
+      </c>
+      <c r="AR2">
+        <v>92.8</v>
+      </c>
+      <c r="AS2">
+        <v>104.37</v>
+      </c>
+      <c r="AT2">
+        <v>109.84</v>
+      </c>
+      <c r="AU2">
+        <v>31.84</v>
+      </c>
+      <c r="AV2">
+        <v>299.54</v>
+      </c>
+      <c r="AW2">
+        <v>89.33</v>
+      </c>
+      <c r="AX2">
+        <v>309.9</v>
+      </c>
+      <c r="AY2">
+        <v>76.52</v>
+      </c>
+      <c r="AZ2">
+        <v>45.84</v>
+      </c>
+      <c r="BA2">
+        <v>347.6</v>
+      </c>
+      <c r="BB2">
+        <v>82.90000000000001</v>
+      </c>
+      <c r="BC2">
+        <v>141.44</v>
+      </c>
+      <c r="BD2">
+        <v>336.77</v>
+      </c>
+      <c r="BE2">
+        <v>17.9</v>
+      </c>
+      <c r="BF2">
+        <v>45.64</v>
+      </c>
+      <c r="BG2">
+        <v>37.06</v>
+      </c>
+      <c r="BH2">
+        <v>43.37</v>
+      </c>
+      <c r="BI2">
+        <v>103.14</v>
+      </c>
+      <c r="BJ2">
+        <v>106.83</v>
+      </c>
+      <c r="BK2">
+        <v>269.01</v>
+      </c>
+      <c r="BL2">
+        <v>206.04</v>
+      </c>
+      <c r="BM2">
+        <v>151.48</v>
+      </c>
+      <c r="BN2">
+        <v>67.73999999999999</v>
+      </c>
+      <c r="BO2">
+        <v>37.27</v>
+      </c>
+      <c r="BP2">
+        <v>55.94</v>
+      </c>
+      <c r="BQ2">
+        <v>63.41</v>
+      </c>
+      <c r="BR2">
+        <v>135.63</v>
+      </c>
+      <c r="BS2">
+        <v>31.52</v>
+      </c>
+      <c r="BT2">
+        <v>53.42</v>
+      </c>
+      <c r="BU2">
+        <v>42.72</v>
+      </c>
+      <c r="BV2">
+        <v>39.7</v>
+      </c>
+      <c r="BW2">
+        <v>172.77</v>
+      </c>
+      <c r="BX2">
+        <v>419.23</v>
+      </c>
+      <c r="BY2">
+        <v>276.65</v>
+      </c>
+      <c r="BZ2">
+        <v>16.5</v>
+      </c>
+      <c r="CA2">
+        <v>39.37</v>
+      </c>
+      <c r="CB2">
+        <v>72.38</v>
+      </c>
+      <c r="CC2">
+        <v>104.35</v>
+      </c>
+      <c r="CD2">
+        <v>43.72</v>
+      </c>
+      <c r="CE2">
+        <v>183.5</v>
+      </c>
+      <c r="CF2">
+        <v>235.32</v>
+      </c>
+      <c r="CG2">
+        <v>51.47</v>
+      </c>
+      <c r="CH2">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="CI2">
+        <v>89.38</v>
+      </c>
+      <c r="CJ2">
+        <v>144.11</v>
+      </c>
+      <c r="CK2">
+        <v>560.16</v>
+      </c>
+      <c r="CL2">
+        <v>55.22</v>
+      </c>
+      <c r="CM2">
+        <v>24.13</v>
+      </c>
+      <c r="CN2">
+        <v>293.45</v>
+      </c>
+      <c r="CO2">
+        <v>107.73</v>
+      </c>
+      <c r="CP2">
+        <v>64.5</v>
+      </c>
+      <c r="CQ2">
+        <v>283.37</v>
+      </c>
+      <c r="CR2">
+        <v>210.7</v>
+      </c>
+      <c r="CS2">
+        <v>441.83</v>
+      </c>
+      <c r="CT2">
+        <v>350.28</v>
+      </c>
+      <c r="CU2">
+        <v>102.76</v>
+      </c>
+      <c r="CV2">
+        <v>128.26</v>
+      </c>
+      <c r="CW2">
+        <v>56.67</v>
+      </c>
+      <c r="CX2">
+        <v>263.48</v>
+      </c>
+      <c r="CY2">
+        <v>110.15</v>
+      </c>
+      <c r="CZ2">
+        <v>33.77</v>
+      </c>
+      <c r="DA2">
+        <v>65.81</v>
+      </c>
+      <c r="DB2">
+        <v>118.86</v>
+      </c>
+      <c r="DC2">
+        <v>26.53</v>
+      </c>
+      <c r="DD2">
+        <v>238.01</v>
+      </c>
+      <c r="DE2">
+        <v>34.24</v>
+      </c>
+      <c r="DF2">
+        <v>99.76000000000001</v>
+      </c>
+      <c r="DG2">
+        <v>235.48</v>
+      </c>
+      <c r="DH2">
+        <v>181.13</v>
+      </c>
+      <c r="DI2">
+        <v>20.52</v>
+      </c>
+      <c r="DJ2">
+        <v>47.82</v>
+      </c>
+      <c r="DK2">
+        <v>131.77</v>
+      </c>
+      <c r="DL2">
+        <v>104.35</v>
+      </c>
+      <c r="DM2">
+        <v>37.86</v>
+      </c>
+      <c r="DN2">
+        <v>41.82</v>
+      </c>
+      <c r="DO2">
+        <v>37.63</v>
+      </c>
+      <c r="DP2">
+        <v>33.84</v>
+      </c>
+      <c r="DQ2">
+        <v>114.37</v>
+      </c>
+      <c r="DR2">
+        <v>10.62</v>
+      </c>
+      <c r="DS2">
+        <v>29.63</v>
+      </c>
+      <c r="DT2">
+        <v>79.70999999999999</v>
+      </c>
+      <c r="DU2">
+        <v>64.83</v>
+      </c>
+      <c r="DV2">
+        <v>57.87</v>
+      </c>
+      <c r="DW2">
+        <v>91.26000000000001</v>
+      </c>
+      <c r="DX2">
+        <v>425.44</v>
+      </c>
+      <c r="DY2">
+        <v>56.32</v>
+      </c>
+      <c r="DZ2">
+        <v>42.49</v>
+      </c>
+      <c r="EA2">
+        <v>16.11</v>
+      </c>
+      <c r="EB2">
+        <v>457.25</v>
+      </c>
+      <c r="EC2">
+        <v>75.98</v>
+      </c>
+      <c r="ED2">
+        <v>80.64</v>
+      </c>
+      <c r="EE2">
+        <v>22.25</v>
+      </c>
+      <c r="EF2">
+        <v>22.1</v>
+      </c>
+      <c r="EG2">
+        <v>179.58</v>
+      </c>
+      <c r="EH2">
+        <v>39.29</v>
+      </c>
+      <c r="EI2">
+        <v>25.8</v>
+      </c>
+      <c r="EJ2">
+        <v>89.86</v>
+      </c>
+      <c r="EK2">
+        <v>222.03</v>
+      </c>
+      <c r="EL2">
+        <v>54.39</v>
+      </c>
+      <c r="EM2">
+        <v>68.45</v>
+      </c>
+      <c r="EN2">
+        <v>126.78</v>
+      </c>
+      <c r="EO2">
+        <v>20.2</v>
+      </c>
+      <c r="EP2">
+        <v>24.64</v>
+      </c>
+      <c r="EQ2">
+        <v>179.16</v>
+      </c>
+      <c r="ER2">
+        <v>388.45</v>
+      </c>
+      <c r="ES2">
+        <v>40.48</v>
+      </c>
+      <c r="ET2">
+        <v>18.48</v>
+      </c>
+      <c r="EU2">
+        <v>139.25</v>
+      </c>
+      <c r="EV2">
+        <v>245.13</v>
+      </c>
+      <c r="EW2">
+        <v>55.22</v>
+      </c>
+      <c r="EX2">
+        <v>91.91</v>
+      </c>
+      <c r="EY2">
+        <v>62.14</v>
+      </c>
+      <c r="EZ2">
+        <v>43.31</v>
+      </c>
+      <c r="FA2">
+        <v>533.99</v>
+      </c>
+      <c r="FB2">
+        <v>38.71</v>
+      </c>
+      <c r="FC2">
+        <v>147.6</v>
+      </c>
+      <c r="FD2">
+        <v>66.52</v>
+      </c>
+      <c r="FE2">
+        <v>56.1</v>
+      </c>
+      <c r="FF2">
+        <v>97.12</v>
+      </c>
+      <c r="FG2">
+        <v>60.43</v>
+      </c>
+      <c r="FH2">
+        <v>131.11</v>
+      </c>
+      <c r="FI2">
+        <v>75.04000000000001</v>
+      </c>
+      <c r="FJ2">
+        <v>243.92</v>
+      </c>
+      <c r="FK2">
+        <v>132.88</v>
+      </c>
+      <c r="FL2">
+        <v>27.78</v>
+      </c>
+      <c r="FM2">
+        <v>229.38</v>
+      </c>
+      <c r="FN2">
+        <v>68</v>
+      </c>
+      <c r="FO2">
+        <v>69.56</v>
+      </c>
+      <c r="FP2">
+        <v>60.59</v>
+      </c>
+      <c r="FQ2">
+        <v>106.96</v>
+      </c>
+      <c r="FR2">
+        <v>156.1</v>
+      </c>
+      <c r="FS2">
+        <v>89.73999999999999</v>
+      </c>
+      <c r="FT2">
+        <v>189.56</v>
+      </c>
+      <c r="FU2">
+        <v>963.41</v>
+      </c>
+      <c r="FV2">
+        <v>43.73</v>
+      </c>
+      <c r="FW2">
+        <v>249.97</v>
+      </c>
+      <c r="FX2">
+        <v>82.29000000000001</v>
+      </c>
+      <c r="FY2">
+        <v>114.78</v>
+      </c>
+      <c r="FZ2">
+        <v>134.5</v>
+      </c>
+      <c r="GA2">
+        <v>139.11</v>
+      </c>
+      <c r="GB2">
+        <v>118.94</v>
+      </c>
+      <c r="GC2">
+        <v>64.34</v>
+      </c>
+      <c r="GD2">
+        <v>56.26</v>
+      </c>
+      <c r="GE2">
+        <v>49.41</v>
+      </c>
+      <c r="GF2">
+        <v>145.09</v>
+      </c>
+      <c r="GG2">
+        <v>284.33</v>
+      </c>
+      <c r="GH2">
+        <v>28.01</v>
+      </c>
+      <c r="GI2">
+        <v>92.90000000000001</v>
+      </c>
+      <c r="GJ2">
+        <v>68.31</v>
+      </c>
+      <c r="GK2">
+        <v>48.94</v>
+      </c>
+      <c r="GL2">
+        <v>285.88</v>
+      </c>
+      <c r="GM2">
+        <v>468.77</v>
+      </c>
+      <c r="GN2">
+        <v>221.09</v>
+      </c>
+      <c r="GO2">
+        <v>119.5</v>
+      </c>
+      <c r="GP2">
+        <v>99.29000000000001</v>
+      </c>
+      <c r="GQ2">
+        <v>87.86</v>
+      </c>
+      <c r="GR2">
+        <v>44.12</v>
+      </c>
+      <c r="GS2">
+        <v>125.72</v>
+      </c>
+      <c r="GT2">
+        <v>68.22</v>
+      </c>
+      <c r="GU2">
+        <v>33.42</v>
+      </c>
+      <c r="GV2">
+        <v>19.85</v>
+      </c>
+      <c r="GW2">
+        <v>71.81999999999999</v>
+      </c>
+      <c r="GX2">
+        <v>50.71</v>
+      </c>
+      <c r="GY2">
+        <v>148.25</v>
+      </c>
+      <c r="GZ2">
+        <v>42.19</v>
+      </c>
+      <c r="HA2">
+        <v>173.81</v>
+      </c>
+      <c r="HB2">
+        <v>218.59</v>
+      </c>
+      <c r="HC2">
+        <v>231.6</v>
+      </c>
+      <c r="HD2">
+        <v>105.88</v>
+      </c>
+      <c r="HE2">
+        <v>689.36</v>
+      </c>
+      <c r="HF2">
+        <v>127.96</v>
+      </c>
+      <c r="HG2">
+        <v>353.43</v>
+      </c>
+      <c r="HH2">
+        <v>71.09</v>
+      </c>
+      <c r="HI2">
+        <v>333.4</v>
+      </c>
+      <c r="HJ2">
+        <v>72.61</v>
+      </c>
+      <c r="HK2">
+        <v>21.31</v>
+      </c>
+      <c r="HL2">
+        <v>153.89</v>
+      </c>
+      <c r="HM2">
+        <v>98.83</v>
+      </c>
+      <c r="HN2">
+        <v>75.26000000000001</v>
+      </c>
+      <c r="HO2">
+        <v>220.2</v>
+      </c>
+      <c r="HP2">
+        <v>68.97</v>
+      </c>
+      <c r="HQ2">
+        <v>146.09</v>
+      </c>
+      <c r="HR2">
+        <v>593.39</v>
+      </c>
+      <c r="HS2">
+        <v>33.72</v>
+      </c>
+      <c r="HT2">
+        <v>63.93</v>
+      </c>
+      <c r="HU2">
+        <v>222.03</v>
+      </c>
+      <c r="HV2">
+        <v>554.42</v>
+      </c>
+      <c r="HW2">
+        <v>225.79</v>
+      </c>
+      <c r="HX2">
+        <v>51.67</v>
+      </c>
+      <c r="HY2">
+        <v>878.78</v>
+      </c>
+      <c r="HZ2">
+        <v>37.7</v>
+      </c>
+      <c r="IA2">
+        <v>12.75</v>
+      </c>
+      <c r="IB2">
+        <v>336.17</v>
+      </c>
+      <c r="IC2">
+        <v>38.38</v>
+      </c>
+      <c r="ID2">
+        <v>73.56999999999999</v>
+      </c>
+      <c r="IE2">
+        <v>107.93</v>
+      </c>
+      <c r="IF2">
+        <v>68.58</v>
+      </c>
+      <c r="IG2">
+        <v>132.35</v>
+      </c>
+      <c r="IH2">
+        <v>178.14</v>
+      </c>
+      <c r="II2">
+        <v>78.34999999999999</v>
+      </c>
+      <c r="IJ2">
+        <v>277.53</v>
+      </c>
+      <c r="IK2">
+        <v>229.38</v>
+      </c>
+      <c r="IL2">
+        <v>21.65</v>
+      </c>
+      <c r="IM2">
+        <v>39.38</v>
+      </c>
+      <c r="IN2">
+        <v>97.08</v>
+      </c>
+      <c r="IO2">
+        <v>428.43</v>
+      </c>
+      <c r="IP2">
+        <v>56.46</v>
+      </c>
+      <c r="IQ2">
+        <v>168.51</v>
+      </c>
+      <c r="IR2">
+        <v>233.34</v>
+      </c>
+      <c r="IS2">
+        <v>221.81</v>
+      </c>
+      <c r="IT2">
+        <v>32.21</v>
+      </c>
+      <c r="IU2">
+        <v>23.44</v>
+      </c>
+      <c r="IV2">
+        <v>353.86</v>
+      </c>
+      <c r="IW2">
+        <v>165.65</v>
+      </c>
+      <c r="IX2">
+        <v>599.47</v>
+      </c>
+      <c r="IY2">
+        <v>39.46</v>
+      </c>
+      <c r="IZ2">
+        <v>181.94</v>
+      </c>
+      <c r="JA2">
+        <v>154.3</v>
+      </c>
+      <c r="JB2">
+        <v>670.22</v>
+      </c>
+      <c r="JC2">
+        <v>104.63</v>
+      </c>
+      <c r="JD2">
+        <v>27.16</v>
+      </c>
+      <c r="JE2">
+        <v>127.51</v>
+      </c>
+      <c r="JF2">
+        <v>292.51</v>
+      </c>
+      <c r="JG2">
+        <v>227.11</v>
+      </c>
+      <c r="JH2">
+        <v>82.81999999999999</v>
+      </c>
+      <c r="JI2">
+        <v>155.4</v>
+      </c>
+      <c r="JJ2">
+        <v>51.1</v>
+      </c>
+      <c r="JK2">
+        <v>51.82</v>
+      </c>
+      <c r="JL2">
+        <v>54.34</v>
+      </c>
+      <c r="JM2">
+        <v>41.83</v>
+      </c>
+      <c r="JN2">
+        <v>114.79</v>
+      </c>
+      <c r="JO2">
+        <v>199.1</v>
+      </c>
+      <c r="JP2">
+        <v>25.2</v>
+      </c>
+      <c r="JQ2">
+        <v>79.18000000000001</v>
+      </c>
+      <c r="JR2">
+        <v>85.13</v>
+      </c>
+      <c r="JS2">
+        <v>146.75</v>
+      </c>
+      <c r="JT2">
+        <v>90.47</v>
+      </c>
+      <c r="JU2">
+        <v>21.59</v>
+      </c>
+      <c r="JV2">
+        <v>146.7</v>
+      </c>
+      <c r="JW2">
+        <v>53.96</v>
+      </c>
+      <c r="JX2">
+        <v>25.59</v>
+      </c>
+      <c r="JY2">
+        <v>210.02</v>
+      </c>
+      <c r="JZ2">
+        <v>160.73</v>
+      </c>
+      <c r="KA2">
+        <v>77.67</v>
+      </c>
+      <c r="KB2">
+        <v>64.53</v>
+      </c>
+      <c r="KC2">
+        <v>334.02</v>
+      </c>
+      <c r="KD2">
+        <v>169.68</v>
+      </c>
+      <c r="KE2">
+        <v>31.13</v>
+      </c>
+      <c r="KF2">
+        <v>261.54</v>
+      </c>
+      <c r="KG2">
+        <v>57.33</v>
+      </c>
+      <c r="KH2">
+        <v>439.81</v>
+      </c>
+      <c r="KI2">
+        <v>78.14</v>
+      </c>
+      <c r="KJ2">
+        <v>85.43000000000001</v>
+      </c>
+      <c r="KK2">
+        <v>279.55</v>
+      </c>
+      <c r="KL2">
+        <v>163.99</v>
+      </c>
+      <c r="KM2">
+        <v>311.02</v>
+      </c>
+      <c r="KN2">
+        <v>157.04</v>
+      </c>
+      <c r="KO2">
+        <v>19.46</v>
+      </c>
+      <c r="KP2">
+        <v>31.02</v>
+      </c>
+      <c r="KQ2">
+        <v>59.46</v>
+      </c>
+      <c r="KR2">
+        <v>133.87</v>
+      </c>
+      <c r="KS2">
+        <v>33.84</v>
+      </c>
+      <c r="KT2">
+        <v>31.3</v>
+      </c>
+      <c r="KU2">
+        <v>251.96</v>
+      </c>
+      <c r="KV2">
+        <v>311.27</v>
+      </c>
+      <c r="KW2">
+        <v>151.99</v>
+      </c>
+      <c r="KX2">
+        <v>120.41</v>
+      </c>
+      <c r="KY2">
+        <v>79.41</v>
+      </c>
+      <c r="KZ2">
+        <v>142.78</v>
+      </c>
+      <c r="LA2">
+        <v>109.57</v>
+      </c>
+      <c r="LB2">
+        <v>102.51</v>
+      </c>
+      <c r="LC2">
+        <v>37.86</v>
+      </c>
+      <c r="LD2">
+        <v>23.85</v>
+      </c>
+      <c r="LE2">
+        <v>76.92</v>
+      </c>
+      <c r="LF2">
+        <v>192.55</v>
+      </c>
+      <c r="LG2">
+        <v>24.54</v>
+      </c>
+      <c r="LH2">
+        <v>194.7</v>
+      </c>
+      <c r="LI2">
+        <v>17.82</v>
+      </c>
+      <c r="LJ2">
+        <v>47.36</v>
+      </c>
+      <c r="LK2">
+        <v>91.91</v>
+      </c>
+      <c r="LL2">
+        <v>21.43</v>
+      </c>
+      <c r="LM2">
+        <v>37.58</v>
+      </c>
+      <c r="LN2">
+        <v>46.5</v>
+      </c>
+      <c r="LO2">
+        <v>108.78</v>
+      </c>
+      <c r="LP2">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="LQ2">
+        <v>60.54</v>
+      </c>
+      <c r="LR2">
+        <v>109.06</v>
+      </c>
+      <c r="LS2">
+        <v>51.73</v>
+      </c>
+      <c r="LT2">
+        <v>80.79000000000001</v>
+      </c>
+      <c r="LU2">
+        <v>285.98</v>
+      </c>
+      <c r="LV2">
+        <v>30.64</v>
+      </c>
+      <c r="LW2">
+        <v>18.44</v>
+      </c>
+      <c r="LX2">
+        <v>155.06</v>
+      </c>
+      <c r="LY2">
+        <v>81.45</v>
+      </c>
+      <c r="LZ2">
+        <v>25.18</v>
+      </c>
+      <c r="MA2">
+        <v>15.79</v>
+      </c>
+      <c r="MB2">
+        <v>56.01</v>
+      </c>
+      <c r="MC2">
+        <v>79.47</v>
+      </c>
+      <c r="MD2">
+        <v>376.3</v>
+      </c>
+      <c r="ME2">
+        <v>102.71</v>
+      </c>
+      <c r="MF2">
+        <v>26.12</v>
+      </c>
+      <c r="MG2">
+        <v>59.98</v>
+      </c>
+      <c r="MH2">
+        <v>22.51</v>
+      </c>
+      <c r="MI2">
+        <v>422.37</v>
+      </c>
+      <c r="MJ2">
+        <v>41.26</v>
+      </c>
+      <c r="MK2">
+        <v>494.44</v>
+      </c>
+      <c r="ML2">
+        <v>12.77</v>
+      </c>
+      <c r="MM2">
+        <v>56.89</v>
+      </c>
+      <c r="MN2">
+        <v>587.04</v>
+      </c>
+      <c r="MO2">
+        <v>70.51000000000001</v>
+      </c>
+      <c r="MP2">
+        <v>82.14</v>
+      </c>
+      <c r="MQ2">
+        <v>34.13</v>
+      </c>
+      <c r="MR2">
+        <v>20.97</v>
+      </c>
+      <c r="MS2">
+        <v>12.92</v>
+      </c>
+      <c r="MT2">
+        <v>26.65</v>
+      </c>
+      <c r="MU2">
+        <v>295.04</v>
+      </c>
+      <c r="MV2">
+        <v>25.39</v>
+      </c>
+      <c r="MW2">
+        <v>284.34</v>
+      </c>
+      <c r="MX2">
+        <v>167.09</v>
+      </c>
+      <c r="MY2">
+        <v>117.38</v>
+      </c>
+      <c r="MZ2">
+        <v>509.75</v>
+      </c>
+      <c r="NA2">
+        <v>13.73</v>
+      </c>
+      <c r="NB2">
+        <v>188.94</v>
+      </c>
+      <c r="NC2">
+        <v>19.23</v>
+      </c>
+      <c r="ND2">
+        <v>198.15</v>
+      </c>
+      <c r="NE2">
+        <v>175.05</v>
+      </c>
+      <c r="NF2">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="NG2">
+        <v>38.53</v>
+      </c>
+      <c r="NH2">
+        <v>10.3</v>
+      </c>
+      <c r="NI2">
+        <v>10.52</v>
+      </c>
+      <c r="NJ2">
+        <v>86.23</v>
+      </c>
+      <c r="NK2">
+        <v>97.38</v>
+      </c>
+      <c r="NL2">
+        <v>348.77</v>
+      </c>
+      <c r="NM2">
+        <v>45.09</v>
+      </c>
+      <c r="NN2">
+        <v>41.16</v>
+      </c>
+      <c r="NO2">
+        <v>106.42</v>
+      </c>
+      <c r="NP2">
+        <v>48.41</v>
+      </c>
+      <c r="NQ2">
+        <v>42</v>
+      </c>
+      <c r="NR2">
+        <v>44.24</v>
+      </c>
+      <c r="NS2">
+        <v>36.09</v>
+      </c>
+      <c r="NT2">
+        <v>51.73</v>
+      </c>
+      <c r="NU2">
+        <v>149.44</v>
+      </c>
+      <c r="NV2">
+        <v>29.03</v>
+      </c>
+      <c r="NW2">
+        <v>32.89</v>
+      </c>
+      <c r="NX2">
+        <v>31.44</v>
+      </c>
+      <c r="NY2">
+        <v>462.17</v>
+      </c>
+      <c r="NZ2">
+        <v>34.91</v>
+      </c>
+      <c r="OA2">
+        <v>80.31999999999999</v>
+      </c>
+      <c r="OB2">
+        <v>213.99</v>
+      </c>
+      <c r="OC2">
+        <v>83.18000000000001</v>
+      </c>
+      <c r="OD2">
+        <v>135.33</v>
+      </c>
+      <c r="OE2">
+        <v>62.89</v>
+      </c>
+      <c r="OF2">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="OG2">
+        <v>18.97</v>
+      </c>
+      <c r="OH2">
+        <v>36.79</v>
+      </c>
+      <c r="OI2">
+        <v>45.04</v>
+      </c>
+      <c r="OJ2">
+        <v>151.99</v>
+      </c>
+      <c r="OK2">
+        <v>34.45</v>
+      </c>
+      <c r="OL2">
+        <v>28.08</v>
+      </c>
+      <c r="OM2">
+        <v>22.21</v>
+      </c>
+      <c r="ON2">
+        <v>22.73</v>
+      </c>
+      <c r="OO2">
+        <v>24.59</v>
+      </c>
+      <c r="OP2">
+        <v>48.19</v>
+      </c>
+      <c r="OQ2">
+        <v>215.74</v>
+      </c>
+      <c r="OR2">
+        <v>125.55</v>
+      </c>
+      <c r="OS2">
+        <v>38.62</v>
+      </c>
+      <c r="OT2">
+        <v>37.69</v>
+      </c>
+      <c r="OU2">
+        <v>71.53</v>
+      </c>
+      <c r="OV2">
+        <v>78.15000000000001</v>
+      </c>
+      <c r="OW2">
+        <v>0.02</v>
+      </c>
+      <c r="OX2">
+        <v>45.64</v>
+      </c>
+      <c r="OY2">
+        <v>317.67</v>
+      </c>
+      <c r="OZ2">
+        <v>193.71</v>
+      </c>
+      <c r="PA2">
+        <v>126.88</v>
+      </c>
+      <c r="PB2">
+        <v>97.53</v>
+      </c>
+      <c r="PC2">
+        <v>140.03</v>
+      </c>
+      <c r="PD2">
+        <v>508.93</v>
+      </c>
+      <c r="PE2">
+        <v>67.05</v>
+      </c>
+      <c r="PF2">
+        <v>155.91</v>
+      </c>
+      <c r="PG2">
+        <v>61.94</v>
+      </c>
+      <c r="PH2">
+        <v>102.41</v>
+      </c>
+      <c r="PI2">
+        <v>98.61</v>
+      </c>
+      <c r="PJ2">
+        <v>51.69</v>
+      </c>
+      <c r="PK2">
+        <v>732.41</v>
+      </c>
+      <c r="PL2">
+        <v>22.62</v>
+      </c>
+      <c r="PM2">
+        <v>87.47</v>
+      </c>
+      <c r="PN2">
+        <v>9.18</v>
+      </c>
+      <c r="PO2">
+        <v>139.02</v>
+      </c>
+      <c r="PP2">
+        <v>18.18</v>
+      </c>
+      <c r="PQ2">
+        <v>273.35</v>
+      </c>
+      <c r="PR2">
+        <v>21.59</v>
+      </c>
+      <c r="PS2">
+        <v>15.19</v>
+      </c>
+      <c r="PT2">
+        <v>37.17</v>
+      </c>
+      <c r="PU2">
+        <v>242.3</v>
+      </c>
+      <c r="PV2">
+        <v>39.39</v>
+      </c>
+      <c r="PW2">
+        <v>45.66</v>
+      </c>
+      <c r="PX2">
+        <v>99.13</v>
+      </c>
+      <c r="PY2">
+        <v>148.8</v>
+      </c>
+      <c r="PZ2">
+        <v>36.44</v>
+      </c>
+      <c r="QA2">
+        <v>61.48</v>
+      </c>
+      <c r="QB2">
+        <v>12.73</v>
+      </c>
+      <c r="QC2">
+        <v>125.15</v>
+      </c>
+      <c r="QD2">
+        <v>149.83</v>
+      </c>
+      <c r="QE2">
+        <v>33.13</v>
+      </c>
+      <c r="QF2">
+        <v>17.74</v>
+      </c>
+      <c r="QG2">
+        <v>119.78</v>
+      </c>
+      <c r="QH2">
+        <v>35.95</v>
+      </c>
+      <c r="QI2">
+        <v>18.78</v>
+      </c>
+      <c r="QJ2">
+        <v>58.1</v>
+      </c>
+      <c r="QK2">
+        <v>25.94</v>
+      </c>
+      <c r="QL2">
+        <v>13.3</v>
+      </c>
+      <c r="QM2">
+        <v>78.66</v>
+      </c>
+      <c r="QN2">
+        <v>85.98</v>
+      </c>
+      <c r="QO2">
+        <v>24</v>
+      </c>
+      <c r="QP2">
+        <v>14.21</v>
+      </c>
+      <c r="QQ2">
+        <v>563.63</v>
+      </c>
+      <c r="QR2">
+        <v>108.12</v>
+      </c>
+      <c r="QS2">
+        <v>86.63</v>
+      </c>
+      <c r="QT2">
+        <v>32.5</v>
+      </c>
+      <c r="QU2">
+        <v>96.23</v>
+      </c>
+      <c r="QV2">
+        <v>105.64</v>
+      </c>
+      <c r="QW2">
+        <v>45.9</v>
+      </c>
+      <c r="QX2">
+        <v>47.5</v>
+      </c>
+      <c r="QY2">
+        <v>67.48</v>
+      </c>
+      <c r="QZ2">
+        <v>28.52</v>
+      </c>
+      <c r="RA2">
+        <v>18.66</v>
+      </c>
+      <c r="RB2">
+        <v>147.11</v>
+      </c>
+      <c r="RC2">
+        <v>41.61</v>
+      </c>
+      <c r="RD2">
+        <v>75</v>
+      </c>
+      <c r="RE2">
+        <v>82.64</v>
+      </c>
+      <c r="RF2">
+        <v>47.68</v>
+      </c>
+      <c r="RG2">
+        <v>50.56</v>
+      </c>
+      <c r="RH2">
+        <v>541.7</v>
+      </c>
+      <c r="RI2">
+        <v>15.64</v>
+      </c>
+      <c r="RJ2">
+        <v>14.87</v>
+      </c>
+      <c r="RK2">
+        <v>24.53</v>
+      </c>
+      <c r="RL2">
+        <v>104.37</v>
+      </c>
+      <c r="RM2">
+        <v>71.67</v>
+      </c>
+      <c r="RN2">
+        <v>776.83</v>
+      </c>
+      <c r="RO2">
+        <v>39.52</v>
+      </c>
+      <c r="RP2">
+        <v>73.38</v>
+      </c>
+      <c r="RQ2">
+        <v>185.93</v>
+      </c>
+      <c r="RR2">
+        <v>188.73</v>
+      </c>
+      <c r="RS2">
+        <v>39.6</v>
+      </c>
+      <c r="RT2">
+        <v>28.07</v>
+      </c>
+      <c r="RU2">
+        <v>46.2</v>
+      </c>
+      <c r="RV2">
+        <v>68.73999999999999</v>
+      </c>
+      <c r="RW2">
+        <v>81.72</v>
+      </c>
+      <c r="RX2">
+        <v>24.33</v>
+      </c>
+      <c r="RY2">
+        <v>30.19</v>
+      </c>
+      <c r="RZ2">
+        <v>96.67</v>
+      </c>
+      <c r="SA2">
+        <v>56.54</v>
+      </c>
+      <c r="SB2">
+        <v>23.6</v>
+      </c>
+      <c r="SC2">
+        <v>39.33</v>
+      </c>
+      <c r="SD2">
+        <v>171.13</v>
+      </c>
+      <c r="SE2">
+        <v>56.7</v>
+      </c>
+      <c r="SF2">
+        <v>166.25</v>
+      </c>
+      <c r="SG2">
+        <v>28.26</v>
+      </c>
+      <c r="SH2">
+        <v>213.22</v>
+      </c>
+      <c r="SI2">
+        <v>36.06</v>
+      </c>
+      <c r="SJ2">
+        <v>25.15</v>
+      </c>
+      <c r="SK2">
+        <v>28.04</v>
+      </c>
+      <c r="SL2">
+        <v>60.08</v>
+      </c>
+      <c r="SM2">
+        <v>22.94</v>
+      </c>
+      <c r="SN2">
+        <v>185.63</v>
+      </c>
+      <c r="SO2">
+        <v>27.11</v>
+      </c>
+      <c r="SP2">
+        <v>21.36</v>
+      </c>
+      <c r="SQ2">
+        <v>166.54</v>
+      </c>
+      <c r="SR2">
+        <v>89.04000000000001</v>
+      </c>
+      <c r="SS2">
+        <v>85.34999999999999</v>
+      </c>
+      <c r="ST2">
+        <v>8.49</v>
+      </c>
+      <c r="SU2">
+        <v>151.2</v>
+      </c>
+      <c r="SV2">
+        <v>62.58</v>
+      </c>
+      <c r="SW2">
+        <v>55.46</v>
+      </c>
+      <c r="SX2">
+        <v>59.08</v>
+      </c>
+      <c r="SY2">
+        <v>14.97</v>
+      </c>
+      <c r="SZ2">
+        <v>113.27</v>
+      </c>
+      <c r="TA2">
+        <v>491.69</v>
+      </c>
+      <c r="TB2">
+        <v>103.63</v>
+      </c>
+      <c r="TC2">
+        <v>77.43000000000001</v>
+      </c>
+      <c r="TD2">
+        <v>103.25</v>
+      </c>
+      <c r="TE2">
+        <v>91.14</v>
+      </c>
+      <c r="TF2">
+        <v>23.95</v>
+      </c>
+      <c r="TG2">
+        <v>33.94</v>
+      </c>
+      <c r="TH2">
+        <v>54.74</v>
+      </c>
+      <c r="TI2">
+        <v>34.69</v>
+      </c>
+      <c r="TJ2">
+        <v>34.53</v>
+      </c>
+      <c r="TK2">
+        <v>265.13</v>
+      </c>
+      <c r="TL2">
+        <v>19.03</v>
+      </c>
+      <c r="TM2">
+        <v>81.38</v>
+      </c>
+      <c r="TN2">
+        <v>26.85</v>
+      </c>
+      <c r="TO2">
+        <v>26.16</v>
+      </c>
+      <c r="TP2">
+        <v>27.18</v>
+      </c>
+      <c r="TQ2">
+        <v>482.34</v>
+      </c>
+      <c r="TR2">
+        <v>14.01</v>
+      </c>
+      <c r="TS2">
+        <v>58.13</v>
+      </c>
+      <c r="TT2">
+        <v>167.9</v>
+      </c>
+      <c r="TU2">
+        <v>40.81</v>
+      </c>
+      <c r="TV2">
+        <v>67.34</v>
+      </c>
+      <c r="TW2">
+        <v>25.16</v>
+      </c>
+      <c r="TX2">
+        <v>112.72</v>
+      </c>
+      <c r="TY2">
+        <v>86.39</v>
+      </c>
+      <c r="TZ2">
+        <v>47.49</v>
+      </c>
+      <c r="UA2">
+        <v>152.23</v>
+      </c>
+      <c r="UB2">
+        <v>38.49</v>
+      </c>
+      <c r="UC2">
+        <v>14.32</v>
+      </c>
+      <c r="UD2">
+        <v>174.15</v>
+      </c>
+      <c r="UE2">
+        <v>32.12</v>
+      </c>
+      <c r="UF2">
+        <v>316.65</v>
+      </c>
+      <c r="UG2">
+        <v>27.95</v>
+      </c>
+      <c r="UH2">
+        <v>76.06999999999999</v>
+      </c>
+      <c r="UI2">
+        <v>108.54</v>
+      </c>
+      <c r="UJ2">
+        <v>64.64</v>
+      </c>
+      <c r="UK2">
+        <v>10.17</v>
+      </c>
+      <c r="UL2">
+        <v>22.3</v>
+      </c>
+      <c r="UM2">
+        <v>22.38</v>
+      </c>
+      <c r="UN2">
+        <v>910.05</v>
+      </c>
+      <c r="UO2">
+        <v>120.62</v>
+      </c>
+      <c r="UP2">
+        <v>47.3</v>
+      </c>
+      <c r="UQ2">
+        <v>14.11</v>
+      </c>
+      <c r="UR2">
+        <v>189.78</v>
+      </c>
+      <c r="US2">
+        <v>144.94</v>
+      </c>
+      <c r="UT2">
+        <v>157.95</v>
+      </c>
+      <c r="UU2">
+        <v>151.27</v>
+      </c>
+      <c r="UV2">
+        <v>15.2</v>
+      </c>
+      <c r="UW2">
+        <v>321.74</v>
+      </c>
+      <c r="UX2">
+        <v>145</v>
+      </c>
+      <c r="UY2">
+        <v>25.81</v>
+      </c>
+      <c r="UZ2">
+        <v>533.13</v>
+      </c>
+      <c r="VA2">
+        <v>73.34</v>
+      </c>
+      <c r="VB2">
+        <v>31.12</v>
+      </c>
+      <c r="VC2">
+        <v>15.01</v>
+      </c>
+      <c r="VD2">
+        <v>37.61</v>
+      </c>
+      <c r="VE2">
+        <v>35.05</v>
+      </c>
+      <c r="VF2">
+        <v>72.16</v>
+      </c>
+      <c r="VG2">
+        <v>27.04</v>
+      </c>
+      <c r="VH2">
+        <v>61.74</v>
+      </c>
+      <c r="VI2">
+        <v>35.68</v>
+      </c>
+      <c r="VJ2">
+        <v>137.21</v>
+      </c>
+      <c r="VK2">
+        <v>269.57</v>
+      </c>
+      <c r="VL2">
+        <v>17.48</v>
+      </c>
+      <c r="VM2">
         <v>143.57</v>
       </c>
-      <c r="AK2">
-        <v>103.11</v>
-      </c>
-      <c r="AL2">
-        <v>73.61</v>
-      </c>
-      <c r="AM2">
-        <v>145.59</v>
-      </c>
-      <c r="AN2">
-        <v>209.35</v>
-      </c>
-      <c r="AO2">
-        <v>135.15</v>
-      </c>
-      <c r="AP2">
-        <v>473.99</v>
-      </c>
-      <c r="AQ2">
-        <v>115.5</v>
-      </c>
-      <c r="AR2">
-        <v>89.59999999999999</v>
-      </c>
-      <c r="AS2">
-        <v>105.64</v>
-      </c>
-      <c r="AT2">
-        <v>105.77</v>
-      </c>
-      <c r="AU2">
-        <v>33.44</v>
-      </c>
-      <c r="AV2">
-        <v>294.69</v>
-      </c>
-      <c r="AW2">
-        <v>89.06</v>
-      </c>
-      <c r="AX2">
-        <v>303.96</v>
-      </c>
-      <c r="AY2">
-        <v>76.19</v>
-      </c>
-      <c r="AZ2">
-        <v>44.38</v>
-      </c>
-      <c r="BA2">
-        <v>342.53</v>
-      </c>
-      <c r="BB2">
-        <v>85.28</v>
-      </c>
-      <c r="BC2">
-        <v>139.82</v>
-      </c>
-      <c r="BD2">
-        <v>336.25</v>
-      </c>
-      <c r="BE2">
-        <v>18.58</v>
-      </c>
-      <c r="BF2">
-        <v>48.11</v>
-      </c>
-      <c r="BG2">
-        <v>37.03</v>
-      </c>
-      <c r="BH2">
-        <v>42.89</v>
-      </c>
-      <c r="BI2">
-        <v>105.8</v>
-      </c>
-      <c r="BJ2">
-        <v>105.3</v>
-      </c>
-      <c r="BK2">
-        <v>270.2</v>
-      </c>
-      <c r="BL2">
-        <v>203.99</v>
-      </c>
-      <c r="BM2">
-        <v>148.89</v>
-      </c>
-      <c r="BN2">
-        <v>68</v>
-      </c>
-      <c r="BO2">
-        <v>37.78</v>
-      </c>
-      <c r="BP2">
-        <v>60.5</v>
-      </c>
-      <c r="BQ2">
-        <v>64.01000000000001</v>
-      </c>
-      <c r="BR2">
-        <v>146.03</v>
-      </c>
-      <c r="BS2">
-        <v>31.27</v>
-      </c>
-      <c r="BT2">
-        <v>56.31</v>
-      </c>
-      <c r="BU2">
-        <v>45.21</v>
-      </c>
-      <c r="BV2">
-        <v>39.22</v>
-      </c>
-      <c r="BW2">
-        <v>170.71</v>
-      </c>
-      <c r="BX2">
-        <v>402</v>
-      </c>
-      <c r="BY2">
-        <v>271.52</v>
-      </c>
-      <c r="BZ2">
-        <v>16.28</v>
-      </c>
-      <c r="CA2">
-        <v>37.76</v>
-      </c>
-      <c r="CB2">
-        <v>73.03</v>
-      </c>
-      <c r="CC2">
-        <v>107.22</v>
-      </c>
-      <c r="CD2">
-        <v>46.49</v>
-      </c>
-      <c r="CE2">
-        <v>184.69</v>
-      </c>
-      <c r="CF2">
-        <v>237.55</v>
-      </c>
-      <c r="CG2">
-        <v>54.31</v>
-      </c>
-      <c r="CH2">
-        <v>94.34</v>
-      </c>
-      <c r="CI2">
-        <v>90.92</v>
-      </c>
-      <c r="CJ2">
-        <v>143.75</v>
-      </c>
-      <c r="CK2">
-        <v>553.76</v>
-      </c>
-      <c r="CL2">
-        <v>53.98</v>
-      </c>
-      <c r="CM2">
-        <v>25.37</v>
-      </c>
-      <c r="CN2">
-        <v>301.01</v>
-      </c>
-      <c r="CO2">
-        <v>114.51</v>
-      </c>
-      <c r="CP2">
-        <v>62.56</v>
-      </c>
-      <c r="CQ2">
-        <v>284.62</v>
-      </c>
-      <c r="CR2">
-        <v>203.53</v>
-      </c>
-      <c r="CS2">
-        <v>445.97</v>
-      </c>
-      <c r="CT2">
-        <v>362.97</v>
-      </c>
-      <c r="CU2">
-        <v>108.29</v>
-      </c>
-      <c r="CV2">
-        <v>128.43</v>
-      </c>
-      <c r="CW2">
-        <v>60.47</v>
-      </c>
-      <c r="CX2">
-        <v>271.95</v>
-      </c>
-      <c r="CY2">
-        <v>109.93</v>
-      </c>
-      <c r="CZ2">
-        <v>36.38</v>
-      </c>
-      <c r="DA2">
-        <v>67.58</v>
-      </c>
-      <c r="DB2">
-        <v>116.64</v>
-      </c>
-      <c r="DC2">
-        <v>27.64</v>
-      </c>
-      <c r="DD2">
-        <v>238.88</v>
-      </c>
-      <c r="DE2">
-        <v>36.68</v>
-      </c>
-      <c r="DF2">
-        <v>98.31999999999999</v>
-      </c>
-      <c r="DG2">
-        <v>235.31</v>
-      </c>
-      <c r="DH2">
-        <v>184.6</v>
-      </c>
-      <c r="DI2">
-        <v>20.72</v>
-      </c>
-      <c r="DJ2">
-        <v>47.48</v>
-      </c>
-      <c r="DK2">
-        <v>130.45</v>
-      </c>
-      <c r="DL2">
-        <v>101.91</v>
-      </c>
-      <c r="DM2">
-        <v>38.87</v>
-      </c>
-      <c r="DN2">
-        <v>41.77</v>
-      </c>
-      <c r="DO2">
-        <v>40.46</v>
-      </c>
-      <c r="DP2">
-        <v>33.03</v>
-      </c>
-      <c r="DQ2">
-        <v>115.08</v>
-      </c>
-      <c r="DR2">
-        <v>11.48</v>
-      </c>
-      <c r="DS2">
-        <v>29.69</v>
-      </c>
-      <c r="DT2">
-        <v>79</v>
-      </c>
-      <c r="DU2">
-        <v>67.40000000000001</v>
-      </c>
-      <c r="DV2">
-        <v>58.51</v>
-      </c>
-      <c r="DW2">
-        <v>91.94</v>
-      </c>
-      <c r="DX2">
-        <v>426.82</v>
-      </c>
-      <c r="DY2">
-        <v>56.31</v>
-      </c>
-      <c r="DZ2">
-        <v>42.69</v>
-      </c>
-      <c r="EA2">
-        <v>42.03</v>
-      </c>
-      <c r="EB2">
+      <c r="VN2">
+        <v>82.11</v>
+      </c>
+      <c r="VO2">
+        <v>27.75</v>
+      </c>
+      <c r="VP2">
+        <v>93.68000000000001</v>
+      </c>
+      <c r="VQ2">
+        <v>47.87</v>
+      </c>
+      <c r="VR2">
+        <v>31.05</v>
+      </c>
+      <c r="VS2">
+        <v>134.74</v>
+      </c>
+      <c r="VT2">
+        <v>86.38</v>
+      </c>
+      <c r="VU2">
+        <v>237.29</v>
+      </c>
+      <c r="VV2">
+        <v>38.45</v>
+      </c>
+      <c r="VW2">
+        <v>65.18000000000001</v>
+      </c>
+      <c r="VX2">
+        <v>56.39</v>
+      </c>
+      <c r="VY2">
+        <v>55.88</v>
+      </c>
+      <c r="VZ2">
+        <v>30.47</v>
+      </c>
+      <c r="WA2">
+        <v>45.57</v>
+      </c>
+      <c r="WB2">
+        <v>438.15</v>
+      </c>
+      <c r="WC2">
+        <v>51.16</v>
+      </c>
+      <c r="WD2">
+        <v>13.64</v>
+      </c>
+      <c r="WE2">
+        <v>26.47</v>
+      </c>
+      <c r="WF2">
+        <v>95.66</v>
+      </c>
+      <c r="WG2">
+        <v>43.15</v>
+      </c>
+      <c r="WH2">
+        <v>29.65</v>
+      </c>
+      <c r="WI2">
+        <v>93.48999999999999</v>
+      </c>
+      <c r="WJ2">
+        <v>36.43</v>
+      </c>
+      <c r="WK2">
+        <v>116.54</v>
+      </c>
+      <c r="WL2">
+        <v>32.78</v>
+      </c>
+      <c r="WM2">
+        <v>300.61</v>
+      </c>
+      <c r="WN2">
+        <v>17.47</v>
+      </c>
+      <c r="WO2">
+        <v>29.87</v>
+      </c>
+      <c r="WP2">
+        <v>168.79</v>
+      </c>
+      <c r="WQ2">
+        <v>56.45</v>
+      </c>
+      <c r="WR2">
+        <v>20.95</v>
+      </c>
+      <c r="WS2">
+        <v>36.55</v>
+      </c>
+      <c r="WT2">
+        <v>16.83</v>
+      </c>
+      <c r="WU2">
+        <v>37.16</v>
+      </c>
+      <c r="WV2">
+        <v>82.19</v>
+      </c>
+      <c r="WW2">
+        <v>26.83</v>
+      </c>
+      <c r="WX2">
+        <v>12.79</v>
+      </c>
+      <c r="WY2">
+        <v>46.41</v>
+      </c>
+      <c r="WZ2">
+        <v>64.58</v>
+      </c>
+      <c r="XA2">
+        <v>17.74</v>
+      </c>
+      <c r="XB2">
+        <v>30.74</v>
+      </c>
+      <c r="XC2">
+        <v>40.56</v>
+      </c>
+      <c r="XD2">
+        <v>129.01</v>
+      </c>
+      <c r="XE2">
+        <v>111.71</v>
+      </c>
+      <c r="XF2">
+        <v>50.51</v>
+      </c>
+      <c r="XG2">
+        <v>291.88</v>
+      </c>
+      <c r="XH2">
+        <v>57.97</v>
+      </c>
+      <c r="XI2">
+        <v>21.59</v>
+      </c>
+      <c r="XJ2">
+        <v>141.88</v>
+      </c>
+      <c r="XK2">
+        <v>23.95</v>
+      </c>
+      <c r="XL2">
+        <v>39.98</v>
+      </c>
+      <c r="XM2">
+        <v>194.47</v>
+      </c>
+      <c r="XN2">
+        <v>15.43</v>
+      </c>
+      <c r="XO2">
+        <v>12.71</v>
+      </c>
+      <c r="XP2">
         <v>16.88</v>
       </c>
-      <c r="EC2">
-        <v>439.74</v>
-      </c>
-      <c r="ED2">
-        <v>75.90000000000001</v>
-      </c>
-      <c r="EE2">
-        <v>76.47</v>
-      </c>
-      <c r="EF2">
-        <v>21.9</v>
-      </c>
-      <c r="EG2">
-        <v>22.45</v>
-      </c>
-      <c r="EH2">
-        <v>164.54</v>
-      </c>
-      <c r="EI2">
-        <v>41.03</v>
-      </c>
-      <c r="EJ2">
-        <v>28.15</v>
-      </c>
-      <c r="EK2">
-        <v>87.8</v>
-      </c>
-      <c r="EL2">
-        <v>214.35</v>
-      </c>
-      <c r="EM2">
-        <v>59.32</v>
-      </c>
-      <c r="EN2">
-        <v>66.93000000000001</v>
-      </c>
-      <c r="EO2">
-        <v>126.3</v>
-      </c>
-      <c r="EP2">
-        <v>20.3</v>
-      </c>
-      <c r="EQ2">
-        <v>25.87</v>
-      </c>
-      <c r="ER2">
-        <v>196.63</v>
-      </c>
-      <c r="ES2">
-        <v>390.49</v>
-      </c>
-      <c r="ET2">
-        <v>39.71</v>
-      </c>
-      <c r="EU2">
-        <v>18.32</v>
-      </c>
-      <c r="EV2">
-        <v>143.59</v>
-      </c>
-      <c r="EW2">
-        <v>248.1</v>
-      </c>
-      <c r="EX2">
-        <v>53.11</v>
-      </c>
-      <c r="EY2">
-        <v>93.64</v>
-      </c>
-      <c r="EZ2">
-        <v>60.46</v>
-      </c>
-      <c r="FA2">
-        <v>43.73</v>
-      </c>
-      <c r="FB2">
-        <v>512.3</v>
-      </c>
-      <c r="FC2">
-        <v>44.9</v>
-      </c>
-      <c r="FD2">
-        <v>169.5</v>
-      </c>
-      <c r="FE2">
-        <v>65.17</v>
-      </c>
-      <c r="FF2">
-        <v>56.06</v>
-      </c>
-      <c r="FG2">
-        <v>96.09999999999999</v>
-      </c>
-      <c r="FH2">
-        <v>63.65</v>
-      </c>
-      <c r="FI2">
-        <v>129.56</v>
-      </c>
-      <c r="FJ2">
-        <v>78.75</v>
-      </c>
-      <c r="FK2">
-        <v>243.72</v>
-      </c>
-      <c r="FL2">
-        <v>149.72</v>
-      </c>
-      <c r="FM2">
-        <v>29.82</v>
-      </c>
-      <c r="FN2">
-        <v>224.42</v>
-      </c>
-      <c r="FO2">
-        <v>68.94</v>
-      </c>
-      <c r="FP2">
-        <v>68.58</v>
-      </c>
-      <c r="FQ2">
-        <v>60.42</v>
-      </c>
-      <c r="FR2">
-        <v>104.36</v>
-      </c>
-      <c r="FS2">
-        <v>156.77</v>
-      </c>
-      <c r="FT2">
-        <v>93.73</v>
-      </c>
-      <c r="FU2">
-        <v>193.24</v>
-      </c>
-      <c r="FV2">
-        <v>965.1900000000001</v>
-      </c>
-      <c r="FW2">
-        <v>42.89</v>
-      </c>
-      <c r="FX2">
-        <v>253.56</v>
-      </c>
-      <c r="FY2">
-        <v>82.26000000000001</v>
-      </c>
-      <c r="FZ2">
-        <v>112.33</v>
-      </c>
-      <c r="GA2">
-        <v>133.3</v>
-      </c>
-      <c r="GB2">
-        <v>144.61</v>
-      </c>
-      <c r="GC2">
-        <v>116.31</v>
-      </c>
-      <c r="GD2">
-        <v>64.05</v>
-      </c>
-      <c r="GE2">
-        <v>55.69</v>
-      </c>
-      <c r="GF2">
-        <v>51.49</v>
-      </c>
-      <c r="GG2">
-        <v>145.77</v>
-      </c>
-      <c r="GH2">
-        <v>273.89</v>
-      </c>
-      <c r="GI2">
-        <v>28.66</v>
-      </c>
-      <c r="GJ2">
-        <v>93.59</v>
-      </c>
-      <c r="GK2">
-        <v>68.06</v>
-      </c>
-      <c r="GL2">
-        <v>48.68</v>
-      </c>
-      <c r="GM2">
-        <v>296.55</v>
-      </c>
-      <c r="GN2">
-        <v>488.68</v>
-      </c>
-      <c r="GO2">
-        <v>225.72</v>
-      </c>
-      <c r="GP2">
-        <v>132.13</v>
-      </c>
-      <c r="GQ2">
-        <v>114.72</v>
-      </c>
-      <c r="GR2">
-        <v>103.09</v>
-      </c>
-      <c r="GS2">
-        <v>43.43</v>
-      </c>
-      <c r="GT2">
-        <v>125.26</v>
-      </c>
-      <c r="GU2">
-        <v>65.83</v>
-      </c>
-      <c r="GV2">
-        <v>34.16</v>
-      </c>
-      <c r="GW2">
-        <v>20.97</v>
-      </c>
-      <c r="GX2">
-        <v>71.13</v>
-      </c>
-      <c r="GY2">
-        <v>53.74</v>
-      </c>
-      <c r="GZ2">
-        <v>158.25</v>
-      </c>
-      <c r="HA2">
-        <v>42.28</v>
-      </c>
-      <c r="HB2">
-        <v>189.54</v>
-      </c>
-      <c r="HC2">
-        <v>223.53</v>
-      </c>
-      <c r="HD2">
-        <v>232.29</v>
-      </c>
-      <c r="HE2">
-        <v>111.22</v>
-      </c>
-      <c r="HF2">
-        <v>671.76</v>
-      </c>
-      <c r="HG2">
-        <v>129.29</v>
-      </c>
-      <c r="HH2">
-        <v>351.95</v>
-      </c>
-      <c r="HI2">
-        <v>70.18000000000001</v>
-      </c>
-      <c r="HJ2">
-        <v>332.43</v>
-      </c>
-      <c r="HK2">
-        <v>77.27</v>
-      </c>
-      <c r="HL2">
-        <v>23.38</v>
-      </c>
-      <c r="HM2">
-        <v>151.8</v>
-      </c>
-      <c r="HN2">
-        <v>103.91</v>
-      </c>
-      <c r="HO2">
-        <v>76.89</v>
-      </c>
-      <c r="HP2">
-        <v>238.25</v>
-      </c>
-      <c r="HQ2">
-        <v>72.19</v>
-      </c>
-      <c r="HR2">
-        <v>139</v>
-      </c>
-      <c r="HS2">
-        <v>588.04</v>
-      </c>
-      <c r="HT2">
-        <v>35.18</v>
-      </c>
-      <c r="HU2">
-        <v>67.31</v>
-      </c>
-      <c r="HV2">
-        <v>217.49</v>
-      </c>
-      <c r="HW2">
-        <v>561.17</v>
-      </c>
-      <c r="HX2">
-        <v>231.97</v>
-      </c>
-      <c r="HY2">
-        <v>51.38</v>
-      </c>
-      <c r="HZ2">
-        <v>897.08</v>
-      </c>
-      <c r="IA2">
-        <v>38.12</v>
-      </c>
-      <c r="IB2">
-        <v>13</v>
-      </c>
-      <c r="IC2">
-        <v>329.88</v>
-      </c>
-      <c r="ID2">
-        <v>43.9</v>
-      </c>
-      <c r="IE2">
-        <v>77</v>
-      </c>
-      <c r="IF2">
-        <v>111.71</v>
-      </c>
-      <c r="IG2">
-        <v>71.52</v>
-      </c>
-      <c r="IH2">
-        <v>139.69</v>
-      </c>
-      <c r="II2">
-        <v>181.9</v>
-      </c>
-      <c r="IJ2">
-        <v>81.48</v>
-      </c>
-      <c r="IK2">
-        <v>283.59</v>
-      </c>
-      <c r="IL2">
-        <v>242.43</v>
-      </c>
-      <c r="IM2">
-        <v>23.45</v>
-      </c>
-      <c r="IN2">
-        <v>40.29</v>
-      </c>
-      <c r="IO2">
-        <v>99.66</v>
-      </c>
-      <c r="IP2">
-        <v>438.59</v>
-      </c>
-      <c r="IQ2">
-        <v>60.29</v>
-      </c>
-      <c r="IR2">
-        <v>173.8</v>
-      </c>
-      <c r="IS2">
-        <v>229.56</v>
-      </c>
-      <c r="IT2">
-        <v>203.19</v>
-      </c>
-      <c r="IU2">
-        <v>33.65</v>
-      </c>
-      <c r="IV2">
-        <v>24.28</v>
-      </c>
-      <c r="IW2">
-        <v>355.39</v>
-      </c>
-      <c r="IX2">
-        <v>169.62</v>
-      </c>
-      <c r="IY2">
-        <v>523.12</v>
-      </c>
-      <c r="IZ2">
-        <v>45.17</v>
-      </c>
-      <c r="JA2">
-        <v>168.52</v>
-      </c>
-      <c r="JB2">
-        <v>167.48</v>
-      </c>
-      <c r="JC2">
-        <v>703.3099999999999</v>
-      </c>
-      <c r="JD2">
-        <v>102.35</v>
-      </c>
-      <c r="JE2">
-        <v>28.79</v>
-      </c>
-      <c r="JF2">
-        <v>128.1</v>
-      </c>
-      <c r="JG2">
-        <v>303.75</v>
-      </c>
-      <c r="JH2">
-        <v>234.34</v>
-      </c>
-      <c r="JI2">
-        <v>83.90000000000001</v>
-      </c>
-      <c r="JJ2">
-        <v>166.62</v>
-      </c>
-      <c r="JK2">
-        <v>52.87</v>
-      </c>
-      <c r="JL2">
-        <v>52.94</v>
-      </c>
-      <c r="JM2">
-        <v>58.62</v>
-      </c>
-      <c r="JN2">
-        <v>43.24</v>
-      </c>
-      <c r="JO2">
-        <v>116.37</v>
-      </c>
-      <c r="JP2">
-        <v>199.1</v>
-      </c>
-      <c r="JQ2">
-        <v>26.69</v>
-      </c>
-      <c r="JR2">
-        <v>81.91</v>
-      </c>
-      <c r="JS2">
-        <v>83.98999999999999</v>
-      </c>
-      <c r="JT2">
-        <v>146.15</v>
-      </c>
-      <c r="JU2">
-        <v>93.93000000000001</v>
-      </c>
-      <c r="JV2">
-        <v>22.49</v>
-      </c>
-      <c r="JW2">
-        <v>149.35</v>
-      </c>
-      <c r="JX2">
-        <v>55.83</v>
-      </c>
-      <c r="JY2">
-        <v>26.64</v>
-      </c>
-      <c r="JZ2">
-        <v>205.81</v>
-      </c>
-      <c r="KA2">
-        <v>159.64</v>
-      </c>
-      <c r="KB2">
-        <v>79.34999999999999</v>
-      </c>
-      <c r="KC2">
-        <v>65.13</v>
-      </c>
-      <c r="KD2">
-        <v>343.86</v>
-      </c>
-      <c r="KE2">
-        <v>179.56</v>
-      </c>
-      <c r="KF2">
-        <v>36.88</v>
-      </c>
-      <c r="KG2">
-        <v>262.24</v>
-      </c>
-      <c r="KH2">
-        <v>58.13</v>
-      </c>
-      <c r="KI2">
-        <v>435.68</v>
-      </c>
-      <c r="KJ2">
-        <v>75.06999999999999</v>
-      </c>
-      <c r="KK2">
-        <v>88.68000000000001</v>
-      </c>
-      <c r="KL2">
-        <v>280.28</v>
-      </c>
-      <c r="KM2">
-        <v>164.06</v>
-      </c>
-      <c r="KN2">
-        <v>328.05</v>
-      </c>
-      <c r="KO2">
-        <v>170.85</v>
-      </c>
-      <c r="KP2">
-        <v>19.2</v>
-      </c>
-      <c r="KQ2">
-        <v>32.89</v>
-      </c>
-      <c r="KR2">
-        <v>61.28</v>
-      </c>
-      <c r="KS2">
-        <v>135.69</v>
-      </c>
-      <c r="KT2">
-        <v>35.82</v>
-      </c>
-      <c r="KU2">
-        <v>33.52</v>
-      </c>
-      <c r="KV2">
-        <v>262.59</v>
-      </c>
-      <c r="KW2">
-        <v>313.56</v>
-      </c>
-      <c r="KX2">
-        <v>160.23</v>
-      </c>
-      <c r="KY2">
-        <v>122.65</v>
-      </c>
-      <c r="KZ2">
-        <v>82.31999999999999</v>
-      </c>
-      <c r="LA2">
-        <v>148.64</v>
-      </c>
-      <c r="LB2">
-        <v>113.68</v>
-      </c>
-      <c r="LC2">
-        <v>105.9</v>
-      </c>
-      <c r="LD2">
-        <v>39.3</v>
-      </c>
-      <c r="LE2">
-        <v>26.36</v>
-      </c>
-      <c r="LF2">
-        <v>80.81999999999999</v>
-      </c>
-      <c r="LG2">
-        <v>193</v>
-      </c>
-      <c r="LH2">
-        <v>26.43</v>
-      </c>
-      <c r="LI2">
-        <v>192.9</v>
-      </c>
-      <c r="LJ2">
-        <v>18.9</v>
-      </c>
-      <c r="LK2">
-        <v>49.82</v>
-      </c>
-      <c r="LL2">
-        <v>90.62</v>
-      </c>
-      <c r="LM2">
-        <v>23.01</v>
-      </c>
-      <c r="LN2">
-        <v>38.59</v>
-      </c>
-      <c r="LO2">
-        <v>46.81</v>
-      </c>
-      <c r="LP2">
-        <v>108.07</v>
-      </c>
-      <c r="LQ2">
-        <v>66.18000000000001</v>
-      </c>
-      <c r="LR2">
-        <v>59.76</v>
-      </c>
-      <c r="LS2">
-        <v>110.5</v>
-      </c>
-      <c r="LT2">
-        <v>50.86</v>
-      </c>
-      <c r="LU2">
-        <v>82.81</v>
-      </c>
-      <c r="LV2">
-        <v>291.09</v>
-      </c>
-      <c r="LW2">
-        <v>31.63</v>
-      </c>
-      <c r="LX2">
-        <v>19.63</v>
-      </c>
-      <c r="LY2">
-        <v>156.3</v>
-      </c>
-      <c r="LZ2">
-        <v>87.31999999999999</v>
-      </c>
-      <c r="MA2">
-        <v>26.55</v>
-      </c>
-      <c r="MB2">
-        <v>16.63</v>
-      </c>
-      <c r="MC2">
-        <v>61.89</v>
-      </c>
-      <c r="MD2">
-        <v>80.89</v>
-      </c>
-      <c r="ME2">
-        <v>398.81</v>
-      </c>
-      <c r="MF2">
-        <v>114.05</v>
-      </c>
-      <c r="MG2">
-        <v>29.86</v>
-      </c>
-      <c r="MH2">
-        <v>65.92</v>
-      </c>
-      <c r="MI2">
-        <v>22.59</v>
-      </c>
-      <c r="MJ2">
-        <v>417.19</v>
-      </c>
-      <c r="MK2">
-        <v>43.26</v>
-      </c>
-      <c r="ML2">
-        <v>516.87</v>
-      </c>
-      <c r="MM2">
-        <v>13.66</v>
-      </c>
-      <c r="MN2">
-        <v>59.83</v>
-      </c>
-      <c r="MO2">
-        <v>596.48</v>
-      </c>
-      <c r="MP2">
-        <v>72.17</v>
-      </c>
-      <c r="MQ2">
-        <v>81.83</v>
-      </c>
-      <c r="MR2">
-        <v>36.91</v>
-      </c>
-      <c r="MS2">
-        <v>22.26</v>
-      </c>
-      <c r="MT2">
-        <v>13.86</v>
-      </c>
-      <c r="MU2">
-        <v>27.5</v>
-      </c>
-      <c r="MV2">
-        <v>285.53</v>
-      </c>
-      <c r="MW2">
-        <v>27.45</v>
-      </c>
-      <c r="MX2">
-        <v>299.94</v>
-      </c>
-      <c r="MY2">
-        <v>175.22</v>
-      </c>
-      <c r="MZ2">
-        <v>114.74</v>
-      </c>
-      <c r="NA2">
-        <v>515.4299999999999</v>
-      </c>
-      <c r="NB2">
-        <v>14.52</v>
-      </c>
-      <c r="NC2">
-        <v>189.44</v>
-      </c>
-      <c r="ND2">
-        <v>20.61</v>
-      </c>
-      <c r="NE2">
-        <v>198.85</v>
-      </c>
-      <c r="NF2">
-        <v>179.84</v>
-      </c>
-      <c r="NG2">
-        <v>75.23999999999999</v>
-      </c>
-      <c r="NH2">
-        <v>41.12</v>
-      </c>
-      <c r="NI2">
-        <v>11.14</v>
-      </c>
-      <c r="NJ2">
-        <v>11.08</v>
-      </c>
-      <c r="NK2">
-        <v>85.81</v>
-      </c>
-      <c r="NL2">
-        <v>103.13</v>
-      </c>
-      <c r="NM2">
-        <v>356.77</v>
-      </c>
-      <c r="NN2">
-        <v>48.33</v>
-      </c>
-      <c r="NO2">
-        <v>44.19</v>
-      </c>
-      <c r="NP2">
-        <v>108.32</v>
-      </c>
-      <c r="NQ2">
-        <v>49.32</v>
-      </c>
-      <c r="NR2">
-        <v>45.73</v>
-      </c>
-      <c r="NS2">
-        <v>48.06</v>
-      </c>
-      <c r="NT2">
-        <v>37.88</v>
-      </c>
-      <c r="NU2">
-        <v>53.83</v>
-      </c>
-      <c r="NV2">
-        <v>153.55</v>
-      </c>
-      <c r="NW2">
-        <v>30.42</v>
-      </c>
-      <c r="NX2">
-        <v>35.55</v>
-      </c>
-      <c r="NY2">
-        <v>32.15</v>
-      </c>
-      <c r="NZ2">
-        <v>456.35</v>
-      </c>
-      <c r="OA2">
-        <v>36.89</v>
-      </c>
-      <c r="OB2">
-        <v>79.79000000000001</v>
-      </c>
-      <c r="OC2">
-        <v>216.44</v>
-      </c>
-      <c r="OD2">
-        <v>85.31999999999999</v>
-      </c>
-      <c r="OE2">
-        <v>136.28</v>
-      </c>
-      <c r="OF2">
-        <v>61.82</v>
-      </c>
-      <c r="OG2">
-        <v>69.66</v>
-      </c>
-      <c r="OH2">
+      <c r="XQ2">
+        <v>32.4</v>
+      </c>
+      <c r="XR2">
+        <v>30.73</v>
+      </c>
+      <c r="XS2">
+        <v>31.95</v>
+      </c>
+      <c r="XT2">
+        <v>101.96</v>
+      </c>
+      <c r="XU2">
+        <v>54.93</v>
+      </c>
+      <c r="XV2">
+        <v>383.73</v>
+      </c>
+      <c r="XW2">
+        <v>15.53</v>
+      </c>
+      <c r="XX2">
+        <v>28.03</v>
+      </c>
+      <c r="XY2">
+        <v>23.94</v>
+      </c>
+      <c r="XZ2">
+        <v>36.25</v>
+      </c>
+      <c r="YA2">
+        <v>88.81999999999999</v>
+      </c>
+      <c r="YB2">
+        <v>9.33</v>
+      </c>
+      <c r="YC2">
+        <v>137.74</v>
+      </c>
+      <c r="YD2">
+        <v>74.91</v>
+      </c>
+      <c r="YE2">
+        <v>513.92</v>
+      </c>
+      <c r="YF2">
+        <v>63.21</v>
+      </c>
+      <c r="YG2">
+        <v>22.47</v>
+      </c>
+      <c r="YH2">
+        <v>158.95</v>
+      </c>
+      <c r="YI2">
+        <v>45.65</v>
+      </c>
+      <c r="YJ2">
+        <v>30.96</v>
+      </c>
+      <c r="YK2">
+        <v>219.18</v>
+      </c>
+      <c r="YL2">
+        <v>7.29</v>
+      </c>
+      <c r="YM2">
+        <v>6.45</v>
+      </c>
+      <c r="YN2">
+        <v>48.89</v>
+      </c>
+      <c r="YO2">
+        <v>59.26</v>
+      </c>
+      <c r="YP2">
+        <v>25.98</v>
+      </c>
+      <c r="YQ2">
+        <v>57.34</v>
+      </c>
+      <c r="YR2">
+        <v>20.49</v>
+      </c>
+      <c r="YS2">
+        <v>59.28</v>
+      </c>
+      <c r="YT2">
         <v>20</v>
       </c>
-      <c r="OI2">
-        <v>39.5</v>
-      </c>
-      <c r="OJ2">
-        <v>47.3</v>
-      </c>
-      <c r="OK2">
-        <v>159.4</v>
-      </c>
-      <c r="OL2">
-        <v>35.89</v>
-      </c>
-      <c r="OM2">
-        <v>28.21</v>
-      </c>
-      <c r="ON2">
-        <v>23.49</v>
-      </c>
-      <c r="OO2">
-        <v>23.6</v>
-      </c>
-      <c r="OP2">
-        <v>24.97</v>
-      </c>
-      <c r="OQ2">
-        <v>48.27</v>
-      </c>
-      <c r="OR2">
-        <v>200.08</v>
-      </c>
-      <c r="OS2">
-        <v>125.39</v>
-      </c>
-      <c r="OT2">
-        <v>40.45</v>
-      </c>
-      <c r="OU2">
-        <v>39.19</v>
-      </c>
-      <c r="OV2">
-        <v>71.98999999999999</v>
-      </c>
-      <c r="OW2">
-        <v>78.72</v>
-      </c>
-      <c r="OX2">
-        <v>28.04</v>
-      </c>
-      <c r="OY2">
-        <v>46.33</v>
-      </c>
-      <c r="OZ2">
-        <v>328.64</v>
-      </c>
-      <c r="PA2">
-        <v>195.22</v>
-      </c>
-      <c r="PB2">
-        <v>127.04</v>
-      </c>
-      <c r="PC2">
-        <v>96.34999999999999</v>
-      </c>
-      <c r="PD2">
-        <v>141.11</v>
-      </c>
-      <c r="PE2">
-        <v>499.18</v>
-      </c>
-      <c r="PF2">
-        <v>66.19</v>
-      </c>
-      <c r="PG2">
-        <v>156.81</v>
-      </c>
-      <c r="PH2">
-        <v>63.77</v>
-      </c>
-      <c r="PI2">
-        <v>107.86</v>
-      </c>
-      <c r="PJ2">
-        <v>104.13</v>
-      </c>
-      <c r="PK2">
-        <v>55.61</v>
-      </c>
-      <c r="PL2">
-        <v>753.71</v>
-      </c>
-      <c r="PM2">
-        <v>23.59</v>
-      </c>
-      <c r="PN2">
-        <v>89.88</v>
-      </c>
-      <c r="PO2">
-        <v>9.35</v>
-      </c>
-      <c r="PP2">
-        <v>141.32</v>
-      </c>
-      <c r="PQ2">
-        <v>18.68</v>
-      </c>
-      <c r="PR2">
-        <v>278.39</v>
-      </c>
-      <c r="PS2">
-        <v>23.15</v>
-      </c>
-      <c r="PT2">
-        <v>17.81</v>
-      </c>
-      <c r="PU2">
-        <v>38</v>
-      </c>
-      <c r="PV2">
-        <v>237.27</v>
-      </c>
-      <c r="PW2">
-        <v>41.22</v>
-      </c>
-      <c r="PX2">
-        <v>46.41</v>
-      </c>
-      <c r="PY2">
-        <v>101.56</v>
-      </c>
-      <c r="PZ2">
-        <v>159.48</v>
-      </c>
-      <c r="QA2">
-        <v>38.39</v>
-      </c>
-      <c r="QB2">
-        <v>63.61</v>
-      </c>
-      <c r="QC2">
-        <v>12.69</v>
-      </c>
-      <c r="QD2">
-        <v>124.65</v>
-      </c>
-      <c r="QE2">
-        <v>151.08</v>
-      </c>
-      <c r="QF2">
-        <v>34.87</v>
-      </c>
-      <c r="QG2">
-        <v>19</v>
-      </c>
-      <c r="QH2">
-        <v>121.16</v>
-      </c>
-      <c r="QI2">
-        <v>37.15</v>
-      </c>
-      <c r="QJ2">
-        <v>20.89</v>
-      </c>
-      <c r="QK2">
-        <v>60.23</v>
-      </c>
-      <c r="QL2">
-        <v>27.16</v>
-      </c>
-      <c r="QM2">
-        <v>13.73</v>
-      </c>
-      <c r="QN2">
-        <v>77.98</v>
-      </c>
-      <c r="QO2">
-        <v>89.05</v>
-      </c>
-      <c r="QP2">
-        <v>25.43</v>
-      </c>
-      <c r="QQ2">
-        <v>14.49</v>
-      </c>
-      <c r="QR2">
-        <v>549.66</v>
-      </c>
-      <c r="QS2">
-        <v>111.7</v>
-      </c>
-      <c r="QT2">
-        <v>86.79000000000001</v>
-      </c>
-      <c r="QU2">
-        <v>33.96</v>
-      </c>
-      <c r="QV2">
-        <v>98.22</v>
-      </c>
-      <c r="QW2">
-        <v>108.73</v>
-      </c>
-      <c r="QX2">
-        <v>49.24</v>
-      </c>
-      <c r="QY2">
-        <v>47.66</v>
-      </c>
-      <c r="QZ2">
-        <v>71.11</v>
-      </c>
-      <c r="RA2">
-        <v>29.84</v>
-      </c>
-      <c r="RB2">
-        <v>20.21</v>
-      </c>
-      <c r="RC2">
-        <v>155</v>
-      </c>
-      <c r="RD2">
-        <v>43.9</v>
-      </c>
-      <c r="RE2">
-        <v>73.38</v>
-      </c>
-      <c r="RF2">
-        <v>86.09999999999999</v>
-      </c>
-      <c r="RG2">
-        <v>47.81</v>
-      </c>
-      <c r="RH2">
-        <v>53.41</v>
-      </c>
-      <c r="RI2">
-        <v>549.33</v>
-      </c>
-      <c r="RJ2">
-        <v>16.94</v>
-      </c>
-      <c r="RK2">
-        <v>15.52</v>
-      </c>
-      <c r="RL2">
-        <v>24.85</v>
-      </c>
-      <c r="RM2">
-        <v>107.16</v>
-      </c>
-      <c r="RN2">
-        <v>74.2</v>
-      </c>
-      <c r="RO2">
-        <v>797.4299999999999</v>
-      </c>
-      <c r="RP2">
-        <v>41.31</v>
-      </c>
-      <c r="RQ2">
-        <v>74.36</v>
-      </c>
-      <c r="RR2">
-        <v>197.94</v>
-      </c>
-      <c r="RS2">
-        <v>191.89</v>
-      </c>
-      <c r="RT2">
-        <v>42.82</v>
-      </c>
-      <c r="RU2">
-        <v>27.41</v>
-      </c>
-      <c r="RV2">
-        <v>49.7</v>
-      </c>
-      <c r="RW2">
-        <v>73.87</v>
-      </c>
-      <c r="RX2">
-        <v>80.51000000000001</v>
-      </c>
-      <c r="RY2">
-        <v>26.01</v>
-      </c>
-      <c r="RZ2">
-        <v>29.87</v>
-      </c>
-      <c r="SA2">
-        <v>95.54000000000001</v>
-      </c>
-      <c r="SB2">
-        <v>60.27</v>
-      </c>
-      <c r="SC2">
-        <v>25.52</v>
-      </c>
-      <c r="SD2">
-        <v>41.05</v>
-      </c>
-      <c r="SE2">
-        <v>172.6</v>
-      </c>
-      <c r="SF2">
-        <v>55.97</v>
-      </c>
-      <c r="SG2">
-        <v>150.22</v>
-      </c>
-      <c r="SH2">
-        <v>29.36</v>
-      </c>
-      <c r="SI2">
-        <v>207.48</v>
-      </c>
-      <c r="SJ2">
-        <v>38</v>
-      </c>
-      <c r="SK2">
-        <v>25.29</v>
-      </c>
-      <c r="SL2">
-        <v>29.14</v>
-      </c>
-      <c r="SM2">
-        <v>62.17</v>
-      </c>
-      <c r="SN2">
-        <v>22.97</v>
-      </c>
-      <c r="SO2">
-        <v>183.4</v>
-      </c>
-      <c r="SP2">
-        <v>26.9</v>
-      </c>
-      <c r="SQ2">
-        <v>21</v>
-      </c>
-      <c r="SR2">
-        <v>168.14</v>
-      </c>
-      <c r="SS2">
-        <v>86.02</v>
-      </c>
-      <c r="ST2">
-        <v>85.28</v>
-      </c>
-      <c r="SU2">
-        <v>8.6</v>
-      </c>
-      <c r="SV2">
-        <v>155.85</v>
-      </c>
-      <c r="SW2">
-        <v>64.61</v>
-      </c>
-      <c r="SX2">
-        <v>55.68</v>
-      </c>
-      <c r="SY2">
-        <v>56.64</v>
-      </c>
-      <c r="SZ2">
-        <v>16.42</v>
-      </c>
-      <c r="TA2">
-        <v>113.73</v>
-      </c>
-      <c r="TB2">
-        <v>481.63</v>
-      </c>
-      <c r="TC2">
-        <v>105.25</v>
-      </c>
-      <c r="TD2">
-        <v>81.70999999999999</v>
-      </c>
-      <c r="TE2">
-        <v>104.08</v>
-      </c>
-      <c r="TF2">
-        <v>91.72</v>
-      </c>
-      <c r="TG2">
-        <v>25.78</v>
-      </c>
-      <c r="TH2">
-        <v>35.61</v>
-      </c>
-      <c r="TI2">
-        <v>55.26</v>
-      </c>
-      <c r="TJ2">
-        <v>34.9</v>
-      </c>
-      <c r="TK2">
-        <v>34.66</v>
-      </c>
-      <c r="TL2">
-        <v>265.63</v>
-      </c>
-      <c r="TM2">
-        <v>19.73</v>
-      </c>
-      <c r="TN2">
-        <v>82.44</v>
-      </c>
-      <c r="TO2">
-        <v>28.15</v>
-      </c>
-      <c r="TP2">
-        <v>27.31</v>
-      </c>
-      <c r="TQ2">
-        <v>27.82</v>
-      </c>
-      <c r="TR2">
-        <v>471.34</v>
-      </c>
-      <c r="TS2">
-        <v>15.2</v>
-      </c>
-      <c r="TT2">
-        <v>59.78</v>
-      </c>
-      <c r="TU2">
-        <v>170.6</v>
-      </c>
-      <c r="TV2">
-        <v>43.51</v>
-      </c>
-      <c r="TW2">
-        <v>67.73</v>
-      </c>
-      <c r="TX2">
-        <v>25.87</v>
-      </c>
-      <c r="TY2">
-        <v>125.17</v>
-      </c>
-      <c r="TZ2">
-        <v>91.51000000000001</v>
-      </c>
-      <c r="UA2">
-        <v>48.05</v>
-      </c>
-      <c r="UB2">
-        <v>165.49</v>
-      </c>
-      <c r="UC2">
-        <v>38.15</v>
-      </c>
-      <c r="UD2">
-        <v>14.83</v>
-      </c>
-      <c r="UE2">
-        <v>173.11</v>
-      </c>
-      <c r="UF2">
-        <v>32.27</v>
-      </c>
-      <c r="UG2">
-        <v>322.59</v>
-      </c>
-      <c r="UH2">
-        <v>29.18</v>
-      </c>
-      <c r="UI2">
-        <v>77.86</v>
-      </c>
-      <c r="UJ2">
-        <v>114.05</v>
-      </c>
-      <c r="UK2">
-        <v>66.86</v>
-      </c>
-      <c r="UL2">
-        <v>10.24</v>
-      </c>
-      <c r="UM2">
-        <v>23.18</v>
-      </c>
-      <c r="UN2">
-        <v>22.33</v>
-      </c>
-      <c r="UO2">
-        <v>935.14</v>
-      </c>
-      <c r="UP2">
-        <v>121.41</v>
-      </c>
-      <c r="UQ2">
-        <v>48.12</v>
-      </c>
-      <c r="UR2">
-        <v>14.82</v>
-      </c>
-      <c r="US2">
-        <v>192.71</v>
-      </c>
-      <c r="UT2">
-        <v>149.73</v>
-      </c>
-      <c r="UU2">
-        <v>168.06</v>
-      </c>
-      <c r="UV2">
-        <v>159.88</v>
-      </c>
-      <c r="UW2">
-        <v>16.46</v>
-      </c>
-      <c r="UX2">
-        <v>314.81</v>
-      </c>
-      <c r="UY2">
-        <v>145.45</v>
-      </c>
-      <c r="UZ2">
-        <v>24.68</v>
-      </c>
-      <c r="VA2">
-        <v>561.84</v>
-      </c>
-      <c r="VB2">
-        <v>78.65000000000001</v>
-      </c>
-      <c r="VC2">
-        <v>33.52</v>
-      </c>
-      <c r="VD2">
-        <v>15.41</v>
-      </c>
-      <c r="VE2">
-        <v>38.64</v>
-      </c>
-      <c r="VF2">
-        <v>35.05</v>
-      </c>
-      <c r="VG2">
-        <v>77.16</v>
-      </c>
-      <c r="VH2">
-        <v>29.94</v>
-      </c>
-      <c r="VI2">
-        <v>62</v>
-      </c>
-      <c r="VJ2">
-        <v>36.85</v>
-      </c>
-      <c r="VK2">
-        <v>147.08</v>
-      </c>
-      <c r="VL2">
-        <v>269.6</v>
-      </c>
-      <c r="VM2">
-        <v>18.04</v>
-      </c>
-      <c r="VN2">
-        <v>153.62</v>
-      </c>
-      <c r="VO2">
-        <v>86.34</v>
-      </c>
-      <c r="VP2">
-        <v>31.07</v>
-      </c>
-      <c r="VQ2">
-        <v>51.8</v>
-      </c>
-      <c r="VR2">
-        <v>97.17</v>
-      </c>
-      <c r="VS2">
-        <v>48.38</v>
-      </c>
-      <c r="VT2">
-        <v>34.77</v>
-      </c>
-      <c r="VU2">
-        <v>30.79</v>
-      </c>
-      <c r="VV2">
-        <v>135.53</v>
-      </c>
-      <c r="VW2">
-        <v>89.68000000000001</v>
-      </c>
-      <c r="VX2">
-        <v>246.22</v>
-      </c>
-      <c r="VY2">
-        <v>40.16</v>
-      </c>
-      <c r="VZ2">
-        <v>66.39</v>
-      </c>
-      <c r="WA2">
-        <v>56.42</v>
-      </c>
-      <c r="WB2">
-        <v>57.86</v>
-      </c>
-      <c r="WC2">
-        <v>32.07</v>
-      </c>
-      <c r="WD2">
-        <v>46.1</v>
-      </c>
-      <c r="WE2">
-        <v>453.55</v>
-      </c>
-      <c r="WF2">
-        <v>48.41</v>
-      </c>
-      <c r="WG2">
-        <v>14.4</v>
-      </c>
-      <c r="WH2">
-        <v>26.25</v>
-      </c>
-      <c r="WI2">
-        <v>98.44</v>
-      </c>
-      <c r="WJ2">
-        <v>45.66</v>
-      </c>
-      <c r="WK2">
-        <v>32.37</v>
-      </c>
-      <c r="WL2">
-        <v>94.98</v>
-      </c>
-      <c r="WM2">
-        <v>36.63</v>
-      </c>
-      <c r="WN2">
-        <v>118.54</v>
-      </c>
-      <c r="WO2">
-        <v>35.97</v>
-      </c>
-      <c r="WP2">
-        <v>288.11</v>
-      </c>
-      <c r="WQ2">
-        <v>18.01</v>
-      </c>
-      <c r="WR2">
-        <v>32.12</v>
-      </c>
-      <c r="WS2">
-        <v>185.87</v>
-      </c>
-      <c r="WT2">
-        <v>60.54</v>
-      </c>
-      <c r="WU2">
-        <v>22.62</v>
-      </c>
-      <c r="WV2">
-        <v>36.55</v>
-      </c>
-      <c r="WW2">
-        <v>17.49</v>
-      </c>
-      <c r="WX2">
-        <v>39.06</v>
-      </c>
-      <c r="WY2">
-        <v>84.03</v>
-      </c>
-      <c r="WZ2">
-        <v>27.16</v>
-      </c>
-      <c r="XA2">
-        <v>13.16</v>
-      </c>
-      <c r="XB2">
-        <v>49.6</v>
-      </c>
-      <c r="XC2">
-        <v>61.96</v>
-      </c>
-      <c r="XD2">
-        <v>18.38</v>
-      </c>
-      <c r="XE2">
-        <v>30.64</v>
-      </c>
-      <c r="XF2">
-        <v>43.13</v>
-      </c>
-      <c r="XG2">
-        <v>134.93</v>
-      </c>
-      <c r="XH2">
-        <v>118.02</v>
-      </c>
-      <c r="XI2">
-        <v>51.75</v>
-      </c>
-      <c r="XJ2">
-        <v>289.34</v>
-      </c>
-      <c r="XK2">
-        <v>58.06</v>
-      </c>
-      <c r="XL2">
-        <v>22.66</v>
-      </c>
-      <c r="XM2">
-        <v>139.73</v>
-      </c>
-      <c r="XN2">
-        <v>24.93</v>
-      </c>
-      <c r="XO2">
-        <v>42.38</v>
-      </c>
-      <c r="XP2">
-        <v>196.35</v>
-      </c>
-      <c r="XQ2">
-        <v>15.6</v>
-      </c>
-      <c r="XR2">
-        <v>13.25</v>
-      </c>
-      <c r="XS2">
-        <v>17.66</v>
-      </c>
-      <c r="XT2">
-        <v>32.29</v>
-      </c>
-      <c r="XU2">
-        <v>32.29</v>
-      </c>
-      <c r="XV2">
-        <v>32.27</v>
-      </c>
-      <c r="XW2">
-        <v>106.6</v>
-      </c>
-      <c r="XX2">
-        <v>55.44</v>
-      </c>
-      <c r="XY2">
-        <v>391</v>
-      </c>
-      <c r="XZ2">
-        <v>16.67</v>
-      </c>
-      <c r="YA2">
-        <v>28.05</v>
-      </c>
-      <c r="YB2">
-        <v>23.89</v>
-      </c>
-      <c r="YC2">
-        <v>39.16</v>
-      </c>
-      <c r="YD2">
-        <v>92.11</v>
-      </c>
-      <c r="YE2">
-        <v>9.02</v>
-      </c>
-      <c r="YF2">
-        <v>142.37</v>
-      </c>
-      <c r="YG2">
-        <v>72.92</v>
-      </c>
-      <c r="YH2">
-        <v>475.69</v>
-      </c>
-      <c r="YI2">
-        <v>68.54000000000001</v>
-      </c>
-      <c r="YJ2">
-        <v>21.76</v>
-      </c>
-      <c r="YK2">
-        <v>161</v>
-      </c>
-      <c r="YL2">
-        <v>47.71</v>
-      </c>
-      <c r="YM2">
-        <v>30.57</v>
-      </c>
-      <c r="YN2">
-        <v>212.14</v>
-      </c>
-      <c r="YO2">
-        <v>7.23</v>
-      </c>
-      <c r="YP2">
-        <v>6.58</v>
-      </c>
-      <c r="YQ2">
-        <v>51.51</v>
-      </c>
-      <c r="YR2">
-        <v>60.77</v>
-      </c>
-      <c r="YS2">
-        <v>25.69</v>
-      </c>
-      <c r="YT2">
-        <v>59.48</v>
-      </c>
       <c r="YU2">
-        <v>20.61</v>
+        <v>41.89</v>
       </c>
       <c r="YV2">
-        <v>58.56</v>
+        <v>93.62</v>
       </c>
       <c r="YW2">
-        <v>21.09</v>
+        <v>70.17</v>
       </c>
       <c r="YX2">
-        <v>43.8</v>
+        <v>50.33</v>
       </c>
       <c r="YY2">
-        <v>95.5</v>
+        <v>56.98</v>
       </c>
       <c r="YZ2">
-        <v>72.89</v>
+        <v>101.44</v>
       </c>
       <c r="ZA2">
-        <v>50.52</v>
+        <v>50.84</v>
       </c>
       <c r="ZB2">
-        <v>58.44</v>
+        <v>80.43000000000001</v>
       </c>
       <c r="ZC2">
-        <v>110.46</v>
+        <v>15.61</v>
       </c>
       <c r="ZD2">
-        <v>54.3</v>
+        <v>76.31</v>
       </c>
       <c r="ZE2">
-        <v>81.55</v>
+        <v>8.69</v>
       </c>
       <c r="ZF2">
-        <v>16.12</v>
+        <v>128.15</v>
       </c>
       <c r="ZG2">
-        <v>79.39</v>
+        <v>14.12</v>
       </c>
       <c r="ZH2">
-        <v>8.83</v>
+        <v>34.75</v>
       </c>
       <c r="ZI2">
-        <v>126.05</v>
+        <v>92.89</v>
       </c>
       <c r="ZJ2">
-        <v>14.41</v>
+        <v>107.52</v>
       </c>
       <c r="ZK2">
-        <v>34.69</v>
+        <v>14.23</v>
       </c>
       <c r="ZL2">
-        <v>26.69</v>
+        <v>7.55</v>
       </c>
       <c r="ZM2">
-        <v>37.16</v>
+        <v>39.88</v>
       </c>
       <c r="ZN2">
-        <v>97.39</v>
+        <v>24.45</v>
       </c>
       <c r="ZO2">
-        <v>103.85</v>
+        <v>16.83</v>
       </c>
       <c r="ZP2">
-        <v>14</v>
+        <v>55.06</v>
       </c>
       <c r="ZQ2">
-        <v>7.69</v>
+        <v>8.58</v>
       </c>
       <c r="ZR2">
-        <v>42.99</v>
-      </c>
-      <c r="ZS2">
-        <v>24.79</v>
-      </c>
-      <c r="ZT2">
-        <v>17.13</v>
-      </c>
-      <c r="ZU2">
-        <v>57.93</v>
-      </c>
-      <c r="ZV2">
-        <v>8.630000000000001</v>
-      </c>
-      <c r="ZW2">
-        <v>284.96</v>
+        <v>283.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>